<commit_message>
feat: create js timer module and wrap js reverse function
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDE908B-6EBC-1140-89BD-C70A0867874C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5A8F26-A555-DF42-9B7B-9C52426E96BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Ruby_Shuffle</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Own_Shuffle v2_aws_ec2</t>
+  </si>
+  <si>
+    <t>Inefficient_Shuffle</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9939279516720025E-2"/>
+          <c:y val="0.11022288261515602"/>
+          <c:w val="0.65941772121905062"/>
+          <c:h val="0.75782078131763986"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1292,6 +1305,159 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-FFF2-B641-A738-D0A21E628542}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Shuffle!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inefficient_Shuffle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Shuffle!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Shuffle!$I$3:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.5976296296296299E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6475814814814801E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0443629629629503E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3447925925925903E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.112558592592592</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16151374074074001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22285903703703699</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29516307407407399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E616-B54B-9751-AA92972D3C11}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1419,6 +1585,7 @@
         <c:axId val="1752059088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.30000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3677,10 +3844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EC2C70-D28D-5649-B065-1682BAD693A3}">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="162" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3690,7 +3857,7 @@
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -3709,8 +3876,11 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>50000</v>
       </c>
@@ -3732,8 +3902,11 @@
       <c r="H3">
         <v>1.20945642888888E-2</v>
       </c>
+      <c r="I3">
+        <v>3.5976296296296299E-3</v>
+      </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3+50000</f>
         <v>100000</v>
@@ -3756,8 +3929,11 @@
       <c r="H4">
         <v>2.4201441644444401E-2</v>
       </c>
+      <c r="I4">
+        <v>1.6475814814814801E-2</v>
+      </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" ref="B5:B22" si="0">B4+50000</f>
         <v>150000</v>
@@ -3780,8 +3956,11 @@
       <c r="H5">
         <v>3.6627184399999999E-2</v>
       </c>
+      <c r="I5">
+        <v>4.0443629629629503E-2</v>
+      </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>200000</v>
@@ -3804,8 +3983,11 @@
       <c r="H6">
         <v>4.9392725311111003E-2</v>
       </c>
+      <c r="I6">
+        <v>7.3447925925925903E-2</v>
+      </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>250000</v>
@@ -3828,8 +4010,11 @@
       <c r="H7">
         <v>6.1969233688888799E-2</v>
       </c>
+      <c r="I7">
+        <v>0.112558592592592</v>
+      </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>300000</v>
@@ -3852,8 +4037,11 @@
       <c r="H8">
         <v>7.5429640999999895E-2</v>
       </c>
+      <c r="I8">
+        <v>0.16151374074074001</v>
+      </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>350000</v>
@@ -3876,8 +4064,11 @@
       <c r="H9">
         <v>8.9336647666666602E-2</v>
       </c>
+      <c r="I9">
+        <v>0.22285903703703699</v>
+      </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>400000</v>
@@ -3900,8 +4091,11 @@
       <c r="H10">
         <v>0.102615948822222</v>
       </c>
+      <c r="I10">
+        <v>0.29516307407407399</v>
+      </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>450000</v>
@@ -3925,7 +4119,7 @@
         <v>0.113187225777777</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>500000</v>
@@ -3949,7 +4143,7 @@
         <v>0.12756304697777701</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>550000</v>
@@ -3973,7 +4167,7 @@
         <v>0.14113324488888801</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>600000</v>
@@ -3997,7 +4191,7 @@
         <v>0.157276132155555</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>650000</v>
@@ -4021,7 +4215,7 @@
         <v>0.16871667495555501</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>700000</v>

</xml_diff>

<commit_message>
docs: add time unit to chart. feat: update js timer
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5A8F26-A555-DF42-9B7B-9C52426E96BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202258F5-84F1-F24E-B97D-BD32163B6B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -77,12 +77,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,9 +99,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,64 +317,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.1540444444444399E-3</c:v>
+                  <c:v>1.15404444444444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3280444444444401E-3</c:v>
+                  <c:v>2.3280444444444401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6934222222222198E-3</c:v>
+                  <c:v>3.6934222222222197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8577555555555504E-3</c:v>
+                  <c:v>4.8577555555555501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0637777777777704E-3</c:v>
+                  <c:v>6.0637777777777702</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5223333333333297E-3</c:v>
+                  <c:v>7.5223333333333295</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6793777777777695E-3</c:v>
+                  <c:v>8.6793777777777699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0194644444444401E-2</c:v>
+                  <c:v>10.1946444444444</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.10262E-2</c:v>
+                  <c:v>11.026199999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1747444444444401E-2</c:v>
+                  <c:v>11.747444444444401</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3117911111111101E-2</c:v>
+                  <c:v>13.1179111111111</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.43615111111111E-2</c:v>
+                  <c:v>14.361511111111099</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.61999111111111E-2</c:v>
+                  <c:v>16.199911111111099</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6842755555555498E-2</c:v>
+                  <c:v>16.842755555555499</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.8743355555555501E-2</c:v>
+                  <c:v>18.7433555555555</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.02561777777777E-2</c:v>
+                  <c:v>20.256177777777701</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2236555555555499E-2</c:v>
+                  <c:v>22.236555555555498</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3790155555555501E-2</c:v>
+                  <c:v>23.790155555555501</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5804244444444398E-2</c:v>
+                  <c:v>25.8042444444444</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8145955555555501E-2</c:v>
+                  <c:v>28.145955555555503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,64 +500,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.4022899777777699E-3</c:v>
+                  <c:v>1.40228997777777</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.82604637777777E-3</c:v>
+                  <c:v>2.8260463777777702</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3713101111111097E-3</c:v>
+                  <c:v>4.3713101111111099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8404372888888898E-3</c:v>
+                  <c:v>5.8404372888888894</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.9460814444444402E-3</c:v>
+                  <c:v>6.9460814444444399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3381473333333303E-3</c:v>
+                  <c:v>8.33814733333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.4671511999999992E-3</c:v>
+                  <c:v>9.4671512</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.14091658666666E-2</c:v>
+                  <c:v>11.4091658666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.26547619555555E-2</c:v>
+                  <c:v>12.6547619555555</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.34669127333333E-2</c:v>
+                  <c:v>13.466912733333299</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.48641465111111E-2</c:v>
+                  <c:v>14.8641465111111</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6428056977777699E-2</c:v>
+                  <c:v>16.4280569777777</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8853301177777702E-2</c:v>
+                  <c:v>18.853301177777702</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0155542911111098E-2</c:v>
+                  <c:v>20.155542911111098</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.2123518733333299E-2</c:v>
+                  <c:v>22.123518733333299</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3842707555555499E-2</c:v>
+                  <c:v>23.842707555555499</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.60826704888888E-2</c:v>
+                  <c:v>26.082670488888798</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.86139463333333E-2</c:v>
+                  <c:v>28.613946333333299</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.76800006666666E-2</c:v>
+                  <c:v>27.680000666666601</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0772209466666599E-2</c:v>
+                  <c:v>30.772209466666599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -690,64 +683,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>7.9028888888888899E-3</c:v>
+                  <c:v>7.9028888888888895</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.62671111111111E-2</c:v>
+                  <c:v>16.267111111111099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4160629629629601E-2</c:v>
+                  <c:v>24.1606296296296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2296259259259198E-2</c:v>
+                  <c:v>32.296259259259202</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1085814814814797E-2</c:v>
+                  <c:v>41.085814814814796</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9734740740740697E-2</c:v>
+                  <c:v>49.734740740740698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7665481481481401E-2</c:v>
+                  <c:v>57.6654814814814</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5998148148148097E-2</c:v>
+                  <c:v>65.998148148148104</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.5265777777777695E-2</c:v>
+                  <c:v>75.2657777777777</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.4995814814814802E-2</c:v>
+                  <c:v>84.995814814814807</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3621333333333306E-2</c:v>
+                  <c:v>93.621333333333311</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10444374074074</c:v>
+                  <c:v>104.44374074074</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.112842296296296</c:v>
+                  <c:v>112.842296296296</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.124860666666666</c:v>
+                  <c:v>124.86066666666599</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.135714148148148</c:v>
+                  <c:v>135.71414814814801</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.144590259259259</c:v>
+                  <c:v>144.590259259259</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.157631518518518</c:v>
+                  <c:v>157.63151851851799</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.16621792592592499</c:v>
+                  <c:v>166.21792592592499</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.179180444444444</c:v>
+                  <c:v>179.18044444444399</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.189683962962963</c:v>
+                  <c:v>189.68396296296299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,64 +866,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.23438432666666E-2</c:v>
+                  <c:v>12.3438432666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.49548595555555E-2</c:v>
+                  <c:v>24.954859555555501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8015178755555497E-2</c:v>
+                  <c:v>38.015178755555496</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.11074833777777E-2</c:v>
+                  <c:v>51.107483377777697</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.4151942911111107E-2</c:v>
+                  <c:v>64.151942911111107</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9637473755555493E-2</c:v>
+                  <c:v>79.63747375555549</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3039540288888806E-2</c:v>
+                  <c:v>93.039540288888801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.105885694488888</c:v>
+                  <c:v>105.88569448888801</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.118766064311111</c:v>
+                  <c:v>118.76606431111101</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13244145706666599</c:v>
+                  <c:v>132.441457066666</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.147738226333333</c:v>
+                  <c:v>147.73822633333299</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.16462669966666599</c:v>
+                  <c:v>164.62669966666598</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18337699462222201</c:v>
+                  <c:v>183.37699462222201</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.193701255444444</c:v>
+                  <c:v>193.701255444444</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.210247808222222</c:v>
+                  <c:v>210.24780822222201</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.22070003924444401</c:v>
+                  <c:v>220.70003924444401</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.23658160077777701</c:v>
+                  <c:v>236.581600777777</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25061169626666602</c:v>
+                  <c:v>250.61169626666603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.26514206868888901</c:v>
+                  <c:v>265.14206868888903</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.27515977077777698</c:v>
+                  <c:v>275.159770777777</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1056,64 +1049,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>7.8472962962962897E-3</c:v>
+                  <c:v>7.8472962962962898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6073037037037E-2</c:v>
+                  <c:v>16.073037037037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.38613703703703E-2</c:v>
+                  <c:v>23.861370370370299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1255481481481398E-2</c:v>
+                  <c:v>31.255481481481397</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9560333333333302E-2</c:v>
+                  <c:v>39.560333333333304</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0029074074073997E-2</c:v>
+                  <c:v>50.029074074073996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5935407407407399E-2</c:v>
+                  <c:v>55.935407407407396</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.4216296296296299E-2</c:v>
+                  <c:v>64.216296296296292</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.3974333333333295E-2</c:v>
+                  <c:v>73.974333333333291</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.3467185185185103E-2</c:v>
+                  <c:v>83.467185185185102</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.4506185185185096E-2</c:v>
+                  <c:v>94.506185185185089</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.11450092592592501</c:v>
+                  <c:v>114.500925925925</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.11425796296296201</c:v>
+                  <c:v>114.25796296296201</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.121193111111111</c:v>
+                  <c:v>121.19311111111101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.134029888888888</c:v>
+                  <c:v>134.029888888888</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.14265662962962899</c:v>
+                  <c:v>142.65662962962898</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.154057851851851</c:v>
+                  <c:v>154.05785185185101</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.162910851851851</c:v>
+                  <c:v>162.91085185185099</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.17444692592592501</c:v>
+                  <c:v>174.446925925925</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.18438303703703701</c:v>
+                  <c:v>184.38303703703701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1239,64 +1232,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.20945642888888E-2</c:v>
+                  <c:v>12.094564288888801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4201441644444401E-2</c:v>
+                  <c:v>24.201441644444401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6627184399999999E-2</c:v>
+                  <c:v>36.627184399999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9392725311111003E-2</c:v>
+                  <c:v>49.392725311111001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.1969233688888799E-2</c:v>
+                  <c:v>61.969233688888799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5429640999999895E-2</c:v>
+                  <c:v>75.42964099999989</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.9336647666666602E-2</c:v>
+                  <c:v>89.336647666666607</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.102615948822222</c:v>
+                  <c:v>102.61594882222199</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.113187225777777</c:v>
+                  <c:v>113.187225777777</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12756304697777701</c:v>
+                  <c:v>127.56304697777701</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14113324488888801</c:v>
+                  <c:v>141.13324488888802</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.157276132155555</c:v>
+                  <c:v>157.27613215555499</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.16871667495555501</c:v>
+                  <c:v>168.71667495555502</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.186122918333333</c:v>
+                  <c:v>186.12291833333299</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.19587684193333299</c:v>
+                  <c:v>195.876841933333</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2078488688</c:v>
+                  <c:v>207.84886879999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.22296346071111101</c:v>
+                  <c:v>222.963460711111</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.23950266511111101</c:v>
+                  <c:v>239.50266511111101</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.25774343220000001</c:v>
+                  <c:v>257.74343220000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.26794210208888802</c:v>
+                  <c:v>267.94210208888802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,28 +1421,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>3.5976296296296299E-3</c:v>
+                  <c:v>3.5976296296296297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6475814814814801E-2</c:v>
+                  <c:v>16.4758148148148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0443629629629503E-2</c:v>
+                  <c:v>40.443629629629505</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3447925925925903E-2</c:v>
+                  <c:v>73.447925925925901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.112558592592592</c:v>
+                  <c:v>112.55859259259201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16151374074074001</c:v>
+                  <c:v>161.51374074074002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.22285903703703699</c:v>
+                  <c:v>222.85903703703698</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.29516307407407399</c:v>
+                  <c:v>295.16307407407402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1585,7 +1578,6 @@
         <c:axId val="1752059088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.30000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1624,7 +1616,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Run Time</a:t>
+                  <a:t>Run Time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3844,9 +3836,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EC2C70-D28D-5649-B065-1682BAD693A3}">
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:N22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="162" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="83" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -3857,7 +3849,7 @@
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -3880,363 +3872,366 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>50000</v>
       </c>
-      <c r="C3" s="1">
-        <v>1.1540444444444399E-3</v>
+      <c r="C3">
+        <v>1.15404444444444</v>
       </c>
       <c r="D3">
-        <v>1.4022899777777699E-3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>7.9028888888888899E-3</v>
+        <v>1.40228997777777</v>
+      </c>
+      <c r="E3">
+        <v>7.9028888888888895</v>
       </c>
       <c r="F3">
-        <v>1.23438432666666E-2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>7.8472962962962897E-3</v>
+        <v>12.3438432666666</v>
+      </c>
+      <c r="G3">
+        <v>7.8472962962962898</v>
       </c>
       <c r="H3">
-        <v>1.20945642888888E-2</v>
+        <v>12.094564288888801</v>
       </c>
       <c r="I3">
-        <v>3.5976296296296299E-3</v>
+        <v>3.5976296296296297</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3+50000</f>
         <v>100000</v>
       </c>
-      <c r="C4" s="1">
-        <v>2.3280444444444401E-3</v>
+      <c r="C4">
+        <v>2.3280444444444401</v>
       </c>
       <c r="D4">
-        <v>2.82604637777777E-3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1.62671111111111E-2</v>
+        <v>2.8260463777777702</v>
+      </c>
+      <c r="E4">
+        <v>16.267111111111099</v>
       </c>
       <c r="F4">
-        <v>2.49548595555555E-2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1.6073037037037E-2</v>
+        <v>24.954859555555501</v>
+      </c>
+      <c r="G4">
+        <v>16.073037037037</v>
       </c>
       <c r="H4">
-        <v>2.4201441644444401E-2</v>
+        <v>24.201441644444401</v>
       </c>
       <c r="I4">
-        <v>1.6475814814814801E-2</v>
+        <v>16.4758148148148</v>
+      </c>
+      <c r="N4">
+        <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" ref="B5:B22" si="0">B4+50000</f>
         <v>150000</v>
       </c>
-      <c r="C5" s="1">
-        <v>3.6934222222222198E-3</v>
+      <c r="C5">
+        <v>3.6934222222222197</v>
       </c>
       <c r="D5">
-        <v>4.3713101111111097E-3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2.4160629629629601E-2</v>
+        <v>4.3713101111111099</v>
+      </c>
+      <c r="E5">
+        <v>24.1606296296296</v>
       </c>
       <c r="F5">
-        <v>3.8015178755555497E-2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2.38613703703703E-2</v>
+        <v>38.015178755555496</v>
+      </c>
+      <c r="G5">
+        <v>23.861370370370299</v>
       </c>
       <c r="H5">
-        <v>3.6627184399999999E-2</v>
+        <v>36.627184399999997</v>
       </c>
       <c r="I5">
-        <v>4.0443629629629503E-2</v>
+        <v>40.443629629629505</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
-      <c r="C6" s="1">
-        <v>4.8577555555555504E-3</v>
+      <c r="C6">
+        <v>4.8577555555555501</v>
       </c>
       <c r="D6">
-        <v>5.8404372888888898E-3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3.2296259259259198E-2</v>
+        <v>5.8404372888888894</v>
+      </c>
+      <c r="E6">
+        <v>32.296259259259202</v>
       </c>
       <c r="F6">
-        <v>5.11074833777777E-2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3.1255481481481398E-2</v>
+        <v>51.107483377777697</v>
+      </c>
+      <c r="G6">
+        <v>31.255481481481397</v>
       </c>
       <c r="H6">
-        <v>4.9392725311111003E-2</v>
+        <v>49.392725311111001</v>
       </c>
       <c r="I6">
-        <v>7.3447925925925903E-2</v>
+        <v>73.447925925925901</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>250000</v>
       </c>
-      <c r="C7" s="1">
-        <v>6.0637777777777704E-3</v>
+      <c r="C7">
+        <v>6.0637777777777702</v>
       </c>
       <c r="D7">
-        <v>6.9460814444444402E-3</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4.1085814814814797E-2</v>
+        <v>6.9460814444444399</v>
+      </c>
+      <c r="E7">
+        <v>41.085814814814796</v>
       </c>
       <c r="F7">
-        <v>6.4151942911111107E-2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>3.9560333333333302E-2</v>
+        <v>64.151942911111107</v>
+      </c>
+      <c r="G7">
+        <v>39.560333333333304</v>
       </c>
       <c r="H7">
-        <v>6.1969233688888799E-2</v>
+        <v>61.969233688888799</v>
       </c>
       <c r="I7">
-        <v>0.112558592592592</v>
+        <v>112.55859259259201</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
-      <c r="C8" s="1">
-        <v>7.5223333333333297E-3</v>
+      <c r="C8">
+        <v>7.5223333333333295</v>
       </c>
       <c r="D8">
-        <v>8.3381473333333303E-3</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4.9734740740740697E-2</v>
+        <v>8.33814733333333</v>
+      </c>
+      <c r="E8">
+        <v>49.734740740740698</v>
       </c>
       <c r="F8">
-        <v>7.9637473755555493E-2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>5.0029074074073997E-2</v>
+        <v>79.63747375555549</v>
+      </c>
+      <c r="G8">
+        <v>50.029074074073996</v>
       </c>
       <c r="H8">
-        <v>7.5429640999999895E-2</v>
+        <v>75.42964099999989</v>
       </c>
       <c r="I8">
-        <v>0.16151374074074001</v>
+        <v>161.51374074074002</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>350000</v>
       </c>
-      <c r="C9" s="1">
-        <v>8.6793777777777695E-3</v>
+      <c r="C9">
+        <v>8.6793777777777699</v>
       </c>
       <c r="D9">
-        <v>9.4671511999999992E-3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5.7665481481481401E-2</v>
+        <v>9.4671512</v>
+      </c>
+      <c r="E9">
+        <v>57.6654814814814</v>
       </c>
       <c r="F9">
-        <v>9.3039540288888806E-2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>5.5935407407407399E-2</v>
+        <v>93.039540288888801</v>
+      </c>
+      <c r="G9">
+        <v>55.935407407407396</v>
       </c>
       <c r="H9">
-        <v>8.9336647666666602E-2</v>
+        <v>89.336647666666607</v>
       </c>
       <c r="I9">
-        <v>0.22285903703703699</v>
+        <v>222.85903703703698</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="C10" s="1">
-        <v>1.0194644444444401E-2</v>
+      <c r="C10">
+        <v>10.1946444444444</v>
       </c>
       <c r="D10">
-        <v>1.14091658666666E-2</v>
-      </c>
-      <c r="E10" s="1">
-        <v>6.5998148148148097E-2</v>
+        <v>11.4091658666666</v>
+      </c>
+      <c r="E10">
+        <v>65.998148148148104</v>
       </c>
       <c r="F10">
-        <v>0.105885694488888</v>
-      </c>
-      <c r="G10" s="1">
-        <v>6.4216296296296299E-2</v>
+        <v>105.88569448888801</v>
+      </c>
+      <c r="G10">
+        <v>64.216296296296292</v>
       </c>
       <c r="H10">
-        <v>0.102615948822222</v>
+        <v>102.61594882222199</v>
       </c>
       <c r="I10">
-        <v>0.29516307407407399</v>
+        <v>295.16307407407402</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>450000</v>
       </c>
-      <c r="C11" s="1">
-        <v>1.10262E-2</v>
+      <c r="C11">
+        <v>11.026199999999999</v>
       </c>
       <c r="D11">
-        <v>1.26547619555555E-2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>7.5265777777777695E-2</v>
+        <v>12.6547619555555</v>
+      </c>
+      <c r="E11">
+        <v>75.2657777777777</v>
       </c>
       <c r="F11">
-        <v>0.118766064311111</v>
-      </c>
-      <c r="G11" s="1">
-        <v>7.3974333333333295E-2</v>
+        <v>118.76606431111101</v>
+      </c>
+      <c r="G11">
+        <v>73.974333333333291</v>
       </c>
       <c r="H11">
-        <v>0.113187225777777</v>
+        <v>113.187225777777</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="C12" s="1">
-        <v>1.1747444444444401E-2</v>
+      <c r="C12">
+        <v>11.747444444444401</v>
       </c>
       <c r="D12">
-        <v>1.34669127333333E-2</v>
-      </c>
-      <c r="E12" s="1">
-        <v>8.4995814814814802E-2</v>
+        <v>13.466912733333299</v>
+      </c>
+      <c r="E12">
+        <v>84.995814814814807</v>
       </c>
       <c r="F12">
-        <v>0.13244145706666599</v>
-      </c>
-      <c r="G12" s="1">
-        <v>8.3467185185185103E-2</v>
+        <v>132.441457066666</v>
+      </c>
+      <c r="G12">
+        <v>83.467185185185102</v>
       </c>
       <c r="H12">
-        <v>0.12756304697777701</v>
+        <v>127.56304697777701</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>550000</v>
       </c>
-      <c r="C13" s="1">
-        <v>1.3117911111111101E-2</v>
+      <c r="C13">
+        <v>13.1179111111111</v>
       </c>
       <c r="D13">
-        <v>1.48641465111111E-2</v>
-      </c>
-      <c r="E13" s="1">
-        <v>9.3621333333333306E-2</v>
+        <v>14.8641465111111</v>
+      </c>
+      <c r="E13">
+        <v>93.621333333333311</v>
       </c>
       <c r="F13">
-        <v>0.147738226333333</v>
-      </c>
-      <c r="G13" s="1">
-        <v>9.4506185185185096E-2</v>
+        <v>147.73822633333299</v>
+      </c>
+      <c r="G13">
+        <v>94.506185185185089</v>
       </c>
       <c r="H13">
-        <v>0.14113324488888801</v>
+        <v>141.13324488888802</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>600000</v>
       </c>
-      <c r="C14" s="1">
-        <v>1.43615111111111E-2</v>
+      <c r="C14">
+        <v>14.361511111111099</v>
       </c>
       <c r="D14">
-        <v>1.6428056977777699E-2</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.10444374074074</v>
+        <v>16.4280569777777</v>
+      </c>
+      <c r="E14">
+        <v>104.44374074074</v>
       </c>
       <c r="F14">
-        <v>0.16462669966666599</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.11450092592592501</v>
+        <v>164.62669966666598</v>
+      </c>
+      <c r="G14">
+        <v>114.500925925925</v>
       </c>
       <c r="H14">
-        <v>0.157276132155555</v>
+        <v>157.27613215555499</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>650000</v>
       </c>
-      <c r="C15" s="1">
-        <v>1.61999111111111E-2</v>
+      <c r="C15">
+        <v>16.199911111111099</v>
       </c>
       <c r="D15">
-        <v>1.8853301177777702E-2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.112842296296296</v>
+        <v>18.853301177777702</v>
+      </c>
+      <c r="E15">
+        <v>112.842296296296</v>
       </c>
       <c r="F15">
-        <v>0.18337699462222201</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0.11425796296296201</v>
+        <v>183.37699462222201</v>
+      </c>
+      <c r="G15">
+        <v>114.25796296296201</v>
       </c>
       <c r="H15">
-        <v>0.16871667495555501</v>
+        <v>168.71667495555502</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="C16" s="1">
-        <v>1.6842755555555498E-2</v>
+      <c r="C16">
+        <v>16.842755555555499</v>
       </c>
       <c r="D16">
-        <v>2.0155542911111098E-2</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.124860666666666</v>
+        <v>20.155542911111098</v>
+      </c>
+      <c r="E16">
+        <v>124.86066666666599</v>
       </c>
       <c r="F16">
-        <v>0.193701255444444</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.121193111111111</v>
+        <v>193.701255444444</v>
+      </c>
+      <c r="G16">
+        <v>121.19311111111101</v>
       </c>
       <c r="H16">
-        <v>0.186122918333333</v>
+        <v>186.12291833333299</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
@@ -4244,23 +4239,23 @@
         <f t="shared" si="0"/>
         <v>750000</v>
       </c>
-      <c r="C17" s="1">
-        <v>1.8743355555555501E-2</v>
+      <c r="C17">
+        <v>18.7433555555555</v>
       </c>
       <c r="D17">
-        <v>2.2123518733333299E-2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.135714148148148</v>
+        <v>22.123518733333299</v>
+      </c>
+      <c r="E17">
+        <v>135.71414814814801</v>
       </c>
       <c r="F17">
-        <v>0.210247808222222</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.134029888888888</v>
+        <v>210.24780822222201</v>
+      </c>
+      <c r="G17">
+        <v>134.029888888888</v>
       </c>
       <c r="H17">
-        <v>0.19587684193333299</v>
+        <v>195.876841933333</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -4268,23 +4263,23 @@
         <f t="shared" si="0"/>
         <v>800000</v>
       </c>
-      <c r="C18" s="1">
-        <v>2.02561777777777E-2</v>
+      <c r="C18">
+        <v>20.256177777777701</v>
       </c>
       <c r="D18">
-        <v>2.3842707555555499E-2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0.144590259259259</v>
+        <v>23.842707555555499</v>
+      </c>
+      <c r="E18">
+        <v>144.590259259259</v>
       </c>
       <c r="F18">
-        <v>0.22070003924444401</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.14265662962962899</v>
+        <v>220.70003924444401</v>
+      </c>
+      <c r="G18">
+        <v>142.65662962962898</v>
       </c>
       <c r="H18">
-        <v>0.2078488688</v>
+        <v>207.84886879999999</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -4292,23 +4287,23 @@
         <f t="shared" si="0"/>
         <v>850000</v>
       </c>
-      <c r="C19" s="1">
-        <v>2.2236555555555499E-2</v>
+      <c r="C19">
+        <v>22.236555555555498</v>
       </c>
       <c r="D19">
-        <v>2.60826704888888E-2</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.157631518518518</v>
+        <v>26.082670488888798</v>
+      </c>
+      <c r="E19">
+        <v>157.63151851851799</v>
       </c>
       <c r="F19">
-        <v>0.23658160077777701</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0.154057851851851</v>
+        <v>236.581600777777</v>
+      </c>
+      <c r="G19">
+        <v>154.05785185185101</v>
       </c>
       <c r="H19">
-        <v>0.22296346071111101</v>
+        <v>222.963460711111</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
@@ -4316,23 +4311,23 @@
         <f t="shared" si="0"/>
         <v>900000</v>
       </c>
-      <c r="C20" s="1">
-        <v>2.3790155555555501E-2</v>
+      <c r="C20">
+        <v>23.790155555555501</v>
       </c>
       <c r="D20">
-        <v>2.86139463333333E-2</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.16621792592592499</v>
+        <v>28.613946333333299</v>
+      </c>
+      <c r="E20">
+        <v>166.21792592592499</v>
       </c>
       <c r="F20">
-        <v>0.25061169626666602</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0.162910851851851</v>
+        <v>250.61169626666603</v>
+      </c>
+      <c r="G20">
+        <v>162.91085185185099</v>
       </c>
       <c r="H20">
-        <v>0.23950266511111101</v>
+        <v>239.50266511111101</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
@@ -4340,23 +4335,23 @@
         <f t="shared" si="0"/>
         <v>950000</v>
       </c>
-      <c r="C21" s="1">
-        <v>2.5804244444444398E-2</v>
+      <c r="C21">
+        <v>25.8042444444444</v>
       </c>
       <c r="D21">
-        <v>2.76800006666666E-2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.179180444444444</v>
+        <v>27.680000666666601</v>
+      </c>
+      <c r="E21">
+        <v>179.18044444444399</v>
       </c>
       <c r="F21">
-        <v>0.26514206868888901</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0.17444692592592501</v>
+        <v>265.14206868888903</v>
+      </c>
+      <c r="G21">
+        <v>174.446925925925</v>
       </c>
       <c r="H21">
-        <v>0.25774343220000001</v>
+        <v>257.74343220000003</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
@@ -4364,23 +4359,23 @@
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="C22" s="1">
-        <v>2.8145955555555501E-2</v>
+      <c r="C22">
+        <v>28.145955555555503</v>
       </c>
       <c r="D22">
-        <v>3.0772209466666599E-2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.189683962962963</v>
+        <v>30.772209466666599</v>
+      </c>
+      <c r="E22">
+        <v>189.68396296296299</v>
       </c>
       <c r="F22">
-        <v>0.27515977077777698</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0.18438303703703701</v>
+        <v>275.159770777777</v>
+      </c>
+      <c r="G22">
+        <v>184.38303703703701</v>
       </c>
       <c r="H22">
-        <v>0.26794210208888802</v>
+        <v>267.94210208888802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: plot link corrected
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2599D8-4AAA-5142-9EF4-A18D09F92673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8AE93E-52DB-6448-9F42-9A88BE252384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="2" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
@@ -16304,7 +16304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BD8F9E-1DE2-FD48-A0FF-3C810CF2B391}">
   <dimension ref="B2:M152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: add native vs own reverse method comparison in js
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8AE93E-52DB-6448-9F42-9A88BE252384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21F2C0B-5354-9A45-901E-40ABC5B8F1DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="2" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="3" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
   <sheets>
     <sheet name="Shuffle" sheetId="1" r:id="rId1"/>
     <sheet name="Sort" sheetId="2" r:id="rId2"/>
-    <sheet name="Reverse" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="reverse1" sheetId="3" r:id="rId3"/>
+    <sheet name="reverse2" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="21">
   <si>
     <t>Ruby_Shuffle</t>
   </si>
@@ -94,12 +95,18 @@
   <si>
     <t>timer.js:18</t>
   </si>
+  <si>
+    <t>nodeJS_reverse_mac</t>
+  </si>
+  <si>
+    <t>own-v1_reverse_mac</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +123,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFAAAB25"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -140,9 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2485,7 +2499,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$C$2</c:f>
+              <c:f>reverse1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2520,7 +2534,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$B$3:$B$32</c:f>
+              <c:f>reverse1!$B$3:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2619,7 +2633,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$C$3:$C$32</c:f>
+              <c:f>reverse1!$C$3:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2728,7 +2742,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$D$2</c:f>
+              <c:f>reverse1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2763,7 +2777,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$B$3:$B$32</c:f>
+              <c:f>reverse1!$B$3:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2862,7 +2876,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$D$3:$D$32</c:f>
+              <c:f>reverse1!$D$3:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2971,7 +2985,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$I$2</c:f>
+              <c:f>reverse1!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3006,7 +3020,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -3465,7 +3479,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$I$3:$I$152</c:f>
+              <c:f>reverse1!$I$3:$I$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -3934,7 +3948,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$J$2</c:f>
+              <c:f>reverse1!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3969,7 +3983,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -4428,7 +4442,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$J$3:$J$152</c:f>
+              <c:f>reverse1!$J$3:$J$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -4897,7 +4911,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$K$2</c:f>
+              <c:f>reverse1!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4932,7 +4946,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -5391,7 +5405,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$K$3:$K$152</c:f>
+              <c:f>reverse1!$K$3:$K$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -5860,7 +5874,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$F$2</c:f>
+              <c:f>reverse1!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5895,7 +5909,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$B$3:$B$32</c:f>
+              <c:f>reverse1!$B$3:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -5994,7 +6008,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$F$3:$F$32</c:f>
+              <c:f>reverse1!$F$3:$F$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -6103,7 +6117,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$L$2</c:f>
+              <c:f>reverse1!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6144,7 +6158,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -6603,7 +6617,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$L$3:$L$152</c:f>
+              <c:f>reverse1!$L$3:$L$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -7072,7 +7086,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$E$2</c:f>
+              <c:f>reverse1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7113,7 +7127,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$B$3:$B$32</c:f>
+              <c:f>reverse1!$B$3:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -7212,7 +7226,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$E$3:$E$32</c:f>
+              <c:f>reverse1!$E$3:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -7321,7 +7335,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$M$2</c:f>
+              <c:f>reverse1!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7362,7 +7376,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -7821,7 +7835,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$M$3:$M$152</c:f>
+              <c:f>reverse1!$M$3:$M$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -8707,7 +8721,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$C$2</c:f>
+              <c:f>reverse1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8742,7 +8756,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$B$3:$B$32</c:f>
+              <c:f>reverse1!$B$3:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8841,7 +8855,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$C$3:$C$32</c:f>
+              <c:f>reverse1!$C$3:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -8950,7 +8964,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$D$2</c:f>
+              <c:f>reverse1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8985,7 +8999,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$B$3:$B$32</c:f>
+              <c:f>reverse1!$B$3:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -9084,7 +9098,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$D$3:$D$32</c:f>
+              <c:f>reverse1!$D$3:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -9193,7 +9207,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$I$2</c:f>
+              <c:f>reverse1!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9228,7 +9242,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -9687,7 +9701,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$I$3:$I$152</c:f>
+              <c:f>reverse1!$I$3:$I$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -10156,7 +10170,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$J$2</c:f>
+              <c:f>reverse1!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10191,7 +10205,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -10650,7 +10664,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$J$3:$J$152</c:f>
+              <c:f>reverse1!$J$3:$J$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -11119,7 +11133,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$K$2</c:f>
+              <c:f>reverse1!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11154,7 +11168,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$H$3:$H$152</c:f>
+              <c:f>reverse1!$H$3:$H$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -11613,7 +11627,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$K$3:$K$152</c:f>
+              <c:f>reverse1!$K$3:$K$152</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
@@ -12082,7 +12096,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Reverse!$E$2</c:f>
+              <c:f>reverse1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12123,7 +12137,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Reverse!$B$3:$B$32</c:f>
+              <c:f>reverse1!$B$3:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -12222,7 +12236,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Reverse!$E$3:$E$32</c:f>
+              <c:f>reverse1!$E$3:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -12650,6 +12664,781 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+              <a:t>Chart Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10053114590374579"/>
+          <c:y val="0.13510164973528074"/>
+          <c:w val="0.80495959466783595"/>
+          <c:h val="0.64069625462183843"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>reverse2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nodeJS_reverse_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>reverse2!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>reverse2!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5.8898342152436502E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1149223066038501E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.64694434238804E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1791723039415099E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.71833336187733E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1593943635622602E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6756777515014001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3084222823381403E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8758389221297299E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5449778007136401E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.1310333510239901E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.6149057199557604E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.9713389691379297E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.7554222610261694E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.2535000311003706E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.5532000081406698E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.31624443166785E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.6126498033603E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.8709277394744999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.10660494574242101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0816-5B41-BC58-75877A0D362E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>reverse2!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>own-v1_reverse_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>reverse2!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>reverse2!$D$3:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.8788667172193499E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6995110412438699E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4171054727501299E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4363222155306002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9593056192000702E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.3494000120295406E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.105413000202841</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.120231388757626</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13526338794165099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.146121667491065</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.160922832373115</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17908166680071</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.18972583239277199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.20494733295506901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.21880650106403499</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.233332666671938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25293794439898598</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.270062777731153</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.27826966635055</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.29146194499399902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0816-5B41-BC58-75877A0D362E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1505303248"/>
+        <c:axId val="1505304928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1505303248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>Array Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1505304928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1505304928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>Run Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1505303248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26858432139138061"/>
+          <c:y val="0.90752687115358643"/>
+          <c:w val="0.47464847056530929"/>
+          <c:h val="8.3464075570896856E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12771,6 +13560,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -14874,6 +15703,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15254,6 +16599,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7542A9DB-47CB-E843-B684-5ED29013E1AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16304,8 +17690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BD8F9E-1DE2-FD48-A0FF-3C810CF2B391}">
   <dimension ref="B2:M152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20008,10 +21394,273 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1762653-C395-8048-983D-A4C069CDBDAD}">
+  <dimension ref="B2:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.8898342152436502E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.8788667172193499E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <f>B3+5000</f>
+        <v>10000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.1149223066038501E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.6995110412438699E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <f t="shared" ref="B5:B22" si="0">B4+5000</f>
+        <v>15000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.64694434238804E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5.4171054727501299E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.1791723039415099E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.4363222155306002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.71833336187733E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.9593056192000702E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.1593943635622602E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>9.3494000120295406E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.6756777515014001E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.105413000202841</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4.3084222823381403E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.120231388757626</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>45000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4.8758389221297299E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.13526338794165099</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5.5449778007136401E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.146121667491065</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>55000</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6.1310333510239901E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.160922832373115</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.6149057199557604E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.17908166680071</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7.9713389691379297E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.18972583239277199</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>70000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7.7554222610261694E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.20494733295506901</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>75000</v>
+      </c>
+      <c r="C17" s="2">
+        <v>8.2535000311003706E-2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.21880650106403499</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="C18" s="2">
+        <v>8.5532000081406698E-2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.233332666671938</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>85000</v>
+      </c>
+      <c r="C19" s="2">
+        <v>9.31624443166785E-2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.25293794439898598</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+      <c r="C20" s="2">
+        <v>9.6126498033603E-2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.270062777731153</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>95000</v>
+      </c>
+      <c r="C21" s="2">
+        <v>9.8709277394744999E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.27826966635055</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.10660494574242101</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.29146194499399902</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873D95BF-D23C-644A-9B7B-A0E7AE44E7F3}">
   <dimension ref="A1:R150"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R1" sqref="R1:R150"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: add throw away runs. Reduce max array size and resolution
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21F2C0B-5354-9A45-901E-40ABC5B8F1DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358969AD-444E-8540-B58F-6EA37396B7DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" activeTab="3" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="3" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
   <sheets>
     <sheet name="Shuffle" sheetId="1" r:id="rId1"/>
@@ -3484,454 +3484,454 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
                 <c:pt idx="0">
-                  <c:v>1.65192219946119E-2</c:v>
+                  <c:v>2.1154250483959899E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6741556185814997E-2</c:v>
+                  <c:v>4.1609874460846102E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9989332978924097E-2</c:v>
+                  <c:v>3.9775499608367598E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2832444301909802E-2</c:v>
+                  <c:v>5.3126689046621302E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0375777797566497E-2</c:v>
+                  <c:v>6.4531625714152996E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9418166453639601E-2</c:v>
+                  <c:v>6.9532250054180594E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.6582444417807705E-2</c:v>
+                  <c:v>7.6579438522457993E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.7434110749098903E-2</c:v>
+                  <c:v>8.7750438600778496E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.103699610672063</c:v>
+                  <c:v>9.8237999714910901E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.112765499908063</c:v>
+                  <c:v>0.10925512574613</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.122282667292488</c:v>
+                  <c:v>0.12516206270083699</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13525855561925301</c:v>
+                  <c:v>0.127371250186115</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.14186933284832301</c:v>
+                  <c:v>0.14221718674525599</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.152899666999777</c:v>
+                  <c:v>0.155403499491512</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.16398572197390901</c:v>
+                  <c:v>0.16445687552914001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.174337555550866</c:v>
+                  <c:v>0.17444856185466001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.185257555089063</c:v>
+                  <c:v>0.18688512500375501</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.198314944282174</c:v>
+                  <c:v>0.19804312614724001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.207088889347182</c:v>
+                  <c:v>0.20776350004598401</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.21795538854267801</c:v>
+                  <c:v>0.217996062245219</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.23580177790588799</c:v>
+                  <c:v>0.228582374285906</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.23989100029898999</c:v>
+                  <c:v>0.24134500185027699</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.25105499952203603</c:v>
+                  <c:v>0.258339312393218</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.26169955647653997</c:v>
+                  <c:v>0.27673525083810002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.28076816660662401</c:v>
+                  <c:v>0.27936912514269302</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.27567249991827503</c:v>
+                  <c:v>0.28894506255164698</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.29453094427784199</c:v>
+                  <c:v>0.30232049990445298</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.30670361055268103</c:v>
+                  <c:v>0.31637181201949699</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.30463700058559501</c:v>
+                  <c:v>0.32132274983450698</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.31897322212656298</c:v>
+                  <c:v>0.328818999230861</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.335588833524121</c:v>
+                  <c:v>0.35090656299144002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.34544855542480901</c:v>
+                  <c:v>0.36370181152596998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.36436033331685502</c:v>
+                  <c:v>0.37182837445288802</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.36917938850819998</c:v>
+                  <c:v>0.39172093570232303</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.37215911121004103</c:v>
+                  <c:v>0.39265649951994402</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.38841388809184202</c:v>
+                  <c:v>0.40224818745627999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.39870888843304497</c:v>
+                  <c:v>0.41913743782788498</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.398507944204741</c:v>
+                  <c:v>0.44802825106307798</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.42161077799068503</c:v>
+                  <c:v>0.45671699987724401</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.45855361140436501</c:v>
+                  <c:v>0.46248949924483801</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.47183594438764698</c:v>
+                  <c:v>0.48339949967339602</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.47680811087290398</c:v>
+                  <c:v>0.478339249268174</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.49395338942607198</c:v>
+                  <c:v>0.495697874110192</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.50581522223850095</c:v>
+                  <c:v>0.50081262318417397</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.51915055534078003</c:v>
+                  <c:v>0.52699243789538697</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.51764361167119599</c:v>
+                  <c:v>0.52963187498971798</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.54527844405836501</c:v>
+                  <c:v>0.53135731071233705</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.54937505535781295</c:v>
+                  <c:v>0.55346756149083298</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.59842027765181305</c:v>
+                  <c:v>0.58196600060909898</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.59515772242512899</c:v>
+                  <c:v>0.58562649972736802</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.60738555652399795</c:v>
+                  <c:v>0.59332968713715595</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.61161377798351901</c:v>
+                  <c:v>0.60989662585780002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.62744916602969103</c:v>
+                  <c:v>0.62941162614151802</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.65664727758202202</c:v>
+                  <c:v>0.65847231168299902</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.65469522194729901</c:v>
+                  <c:v>0.64366231206804503</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.66398927755653803</c:v>
+                  <c:v>0.64640106214210302</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.67323100028766503</c:v>
+                  <c:v>0.68013862473890097</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.71820933371782303</c:v>
+                  <c:v>0.69856343790888697</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.69090472182465901</c:v>
+                  <c:v>0.68299287464469605</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.73486249976687901</c:v>
+                  <c:v>0.721210563089698</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.72236872195369595</c:v>
+                  <c:v>0.72887293761595995</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.77505500055849497</c:v>
+                  <c:v>0.74672987358644605</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.75990438813136596</c:v>
+                  <c:v>0.75056487461552002</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.82948949995140198</c:v>
+                  <c:v>0.80153800081461601</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.78583499934110301</c:v>
+                  <c:v>0.79019256262108595</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.84491361139549104</c:v>
+                  <c:v>0.80484918784350101</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.811335722398426</c:v>
+                  <c:v>0.82444006390869595</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.88879766646358704</c:v>
+                  <c:v>0.84068050095811397</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.83744222256872303</c:v>
+                  <c:v>0.84409362403675903</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.83555377792153096</c:v>
+                  <c:v>0.860603000037372</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.91792288857201698</c:v>
+                  <c:v>0.87704375106841304</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.85683472268283301</c:v>
+                  <c:v>0.86880862526595504</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.92206922276980297</c:v>
+                  <c:v>0.92467824975028601</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.87719394494262004</c:v>
+                  <c:v>0.878106687683612</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.96720411111083204</c:v>
+                  <c:v>0.91236000042408705</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.899489333232243</c:v>
+                  <c:v>0.89544493565335803</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.99032133341663398</c:v>
+                  <c:v>0.95345456199720502</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.92280316642589</c:v>
+                  <c:v>0.91085156193003003</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.00779483322468</c:v>
+                  <c:v>0.989647249691188</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.97174866704477203</c:v>
+                  <c:v>0.97376206237822704</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.02890194435086</c:v>
+                  <c:v>1.0315268123522401</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.0652831668655001</c:v>
+                  <c:v>1.03320712503045</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.09856305540435</c:v>
+                  <c:v>1.05896968767046</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.1128907218161499</c:v>
+                  <c:v>1.0717105632647801</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.17172700001133</c:v>
+                  <c:v>1.0887696859426701</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.15806916666527</c:v>
+                  <c:v>1.11381506221368</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.06420583319332</c:v>
+                  <c:v>1.0617330619134</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.13822727733188</c:v>
+                  <c:v>1.1172992512583699</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.04233694407675</c:v>
+                  <c:v>1.0598551868460999</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.2002873340000699</c:v>
+                  <c:v>1.1480260002426801</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.0503385557482601</c:v>
+                  <c:v>1.0775930006057</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.1917405006372199</c:v>
+                  <c:v>1.15175243932753</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.0653614999933301</c:v>
+                  <c:v>1.1060021254234</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.2313667777925701</c:v>
+                  <c:v>1.1750489370897399</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.09875211140347</c:v>
+                  <c:v>1.1417620629072101</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.25887533297969</c:v>
+                  <c:v>1.2161118127405599</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.2151582783295001</c:v>
+                  <c:v>1.2504325625486601</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.25264494493603</c:v>
+                  <c:v>1.23164212564006</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.3365032221708</c:v>
+                  <c:v>1.26111306156963</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.29315849993791</c:v>
+                  <c:v>1.2899310616776301</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.33646083271337</c:v>
+                  <c:v>1.26966424891725</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.2705005556344899</c:v>
+                  <c:v>1.2419091253541401</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.33116816687915</c:v>
+                  <c:v>1.2942723133601199</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.24674188863072</c:v>
+                  <c:v>1.2016283748671399</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1.3812169451266501</c:v>
+                  <c:v>1.3854302503168501</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.2087348335318999</c:v>
+                  <c:v>1.2040255004539999</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.41294138940672</c:v>
+                  <c:v>1.3439333741553099</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.2161969439022999</c:v>
+                  <c:v>1.2299765618517899</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.4282873330844701</c:v>
+                  <c:v>1.39935700036585</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.2767278336816299</c:v>
+                  <c:v>1.25695087620988</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1.4874513888110701</c:v>
+                  <c:v>1.47827893588691</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1.29863299967514</c:v>
+                  <c:v>1.2872142493724801</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1.5245358890129399</c:v>
+                  <c:v>1.5170100615359801</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1.54560600014196</c:v>
+                  <c:v>1.5911656874231901</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.5359668334325101</c:v>
+                  <c:v>1.50943518662825</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1.59086999980111</c:v>
+                  <c:v>1.5279893744736901</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1.5617407218863499</c:v>
+                  <c:v>1.5115798134356699</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>1.59447000051538</c:v>
+                  <c:v>1.52659987518563</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1.3940732775049001</c:v>
+                  <c:v>1.4287933125160599</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>1.63363555529051</c:v>
+                  <c:v>1.5650997501797901</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1.40429827777875</c:v>
+                  <c:v>1.42840662552043</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1.64669394410318</c:v>
+                  <c:v>1.58606418827548</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>1.3811274444063499</c:v>
+                  <c:v>1.4357484383508501</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1.6596602778881699</c:v>
+                  <c:v>1.6223783139139401</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>1.40439088890949</c:v>
+                  <c:v>1.48612949904054</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>1.6904112220638301</c:v>
+                  <c:v>1.6645513754337999</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1.4447390553024</c:v>
+                  <c:v>1.5379989375360299</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>1.7042882223096101</c:v>
+                  <c:v>1.6482201870530799</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>1.6943401669462499</c:v>
+                  <c:v>1.6616218732669901</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1.7375244444443101</c:v>
+                  <c:v>1.7317581879906301</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1.9059758331212699</c:v>
+                  <c:v>1.77275406243279</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>1.82115272246301</c:v>
+                  <c:v>1.7379474383778799</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>1.78205744404759</c:v>
+                  <c:v>1.7401566253975</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>1.5876966112603701</c:v>
+                  <c:v>1.7272279383614599</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>1.79450838847292</c:v>
+                  <c:v>1.7727095629088501</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>1.60297011087338</c:v>
+                  <c:v>1.6175416875630599</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>1.8280026115890999</c:v>
+                  <c:v>1.79891450051218</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>1.5774916108283701</c:v>
+                  <c:v>1.6368558132089599</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>1.8409437218474001</c:v>
+                  <c:v>1.77758537512272</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>1.5796587218840901</c:v>
+                  <c:v>1.65796218812465</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>1.9275448885228801</c:v>
+                  <c:v>1.83635300118476</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>1.6350606112844399</c:v>
+                  <c:v>1.66436700103804</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>1.9188066114568001</c:v>
+                  <c:v>1.87462399946525</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>1.66594450010193</c:v>
+                  <c:v>1.71441499982029</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>1.95562722264892</c:v>
+                  <c:v>1.9158713137730901</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>2.0274828887648</c:v>
+                  <c:v>1.92541893757879</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>1.96881344397034</c:v>
+                  <c:v>1.9498613746836699</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>2.0283092775692499</c:v>
+                  <c:v>1.96982187591493</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>2.0176236112084598</c:v>
+                  <c:v>1.99480787478387</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>2.01672127739422</c:v>
+                  <c:v>1.9824372502043801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9706,454 +9706,454 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="150"/>
                 <c:pt idx="0">
-                  <c:v>1.65192219946119E-2</c:v>
+                  <c:v>2.1154250483959899E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6741556185814997E-2</c:v>
+                  <c:v>4.1609874460846102E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9989332978924097E-2</c:v>
+                  <c:v>3.9775499608367598E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2832444301909802E-2</c:v>
+                  <c:v>5.3126689046621302E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0375777797566497E-2</c:v>
+                  <c:v>6.4531625714152996E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9418166453639601E-2</c:v>
+                  <c:v>6.9532250054180594E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.6582444417807705E-2</c:v>
+                  <c:v>7.6579438522457993E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.7434110749098903E-2</c:v>
+                  <c:v>8.7750438600778496E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.103699610672063</c:v>
+                  <c:v>9.8237999714910901E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.112765499908063</c:v>
+                  <c:v>0.10925512574613</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.122282667292488</c:v>
+                  <c:v>0.12516206270083699</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13525855561925301</c:v>
+                  <c:v>0.127371250186115</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.14186933284832301</c:v>
+                  <c:v>0.14221718674525599</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.152899666999777</c:v>
+                  <c:v>0.155403499491512</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.16398572197390901</c:v>
+                  <c:v>0.16445687552914001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.174337555550866</c:v>
+                  <c:v>0.17444856185466001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.185257555089063</c:v>
+                  <c:v>0.18688512500375501</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.198314944282174</c:v>
+                  <c:v>0.19804312614724001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.207088889347182</c:v>
+                  <c:v>0.20776350004598401</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.21795538854267801</c:v>
+                  <c:v>0.217996062245219</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.23580177790588799</c:v>
+                  <c:v>0.228582374285906</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.23989100029898999</c:v>
+                  <c:v>0.24134500185027699</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.25105499952203603</c:v>
+                  <c:v>0.258339312393218</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.26169955647653997</c:v>
+                  <c:v>0.27673525083810002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.28076816660662401</c:v>
+                  <c:v>0.27936912514269302</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.27567249991827503</c:v>
+                  <c:v>0.28894506255164698</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.29453094427784199</c:v>
+                  <c:v>0.30232049990445298</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.30670361055268103</c:v>
+                  <c:v>0.31637181201949699</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.30463700058559501</c:v>
+                  <c:v>0.32132274983450698</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.31897322212656298</c:v>
+                  <c:v>0.328818999230861</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.335588833524121</c:v>
+                  <c:v>0.35090656299144002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.34544855542480901</c:v>
+                  <c:v>0.36370181152596998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.36436033331685502</c:v>
+                  <c:v>0.37182837445288802</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.36917938850819998</c:v>
+                  <c:v>0.39172093570232303</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.37215911121004103</c:v>
+                  <c:v>0.39265649951994402</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.38841388809184202</c:v>
+                  <c:v>0.40224818745627999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.39870888843304497</c:v>
+                  <c:v>0.41913743782788498</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.398507944204741</c:v>
+                  <c:v>0.44802825106307798</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.42161077799068503</c:v>
+                  <c:v>0.45671699987724401</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.45855361140436501</c:v>
+                  <c:v>0.46248949924483801</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.47183594438764698</c:v>
+                  <c:v>0.48339949967339602</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.47680811087290398</c:v>
+                  <c:v>0.478339249268174</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.49395338942607198</c:v>
+                  <c:v>0.495697874110192</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.50581522223850095</c:v>
+                  <c:v>0.50081262318417397</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.51915055534078003</c:v>
+                  <c:v>0.52699243789538697</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.51764361167119599</c:v>
+                  <c:v>0.52963187498971798</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.54527844405836501</c:v>
+                  <c:v>0.53135731071233705</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.54937505535781295</c:v>
+                  <c:v>0.55346756149083298</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.59842027765181305</c:v>
+                  <c:v>0.58196600060909898</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.59515772242512899</c:v>
+                  <c:v>0.58562649972736802</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.60738555652399795</c:v>
+                  <c:v>0.59332968713715595</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.61161377798351901</c:v>
+                  <c:v>0.60989662585780002</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.62744916602969103</c:v>
+                  <c:v>0.62941162614151802</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.65664727758202202</c:v>
+                  <c:v>0.65847231168299902</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.65469522194729901</c:v>
+                  <c:v>0.64366231206804503</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.66398927755653803</c:v>
+                  <c:v>0.64640106214210302</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.67323100028766503</c:v>
+                  <c:v>0.68013862473890097</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.71820933371782303</c:v>
+                  <c:v>0.69856343790888697</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.69090472182465901</c:v>
+                  <c:v>0.68299287464469605</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.73486249976687901</c:v>
+                  <c:v>0.721210563089698</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.72236872195369595</c:v>
+                  <c:v>0.72887293761595995</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.77505500055849497</c:v>
+                  <c:v>0.74672987358644605</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.75990438813136596</c:v>
+                  <c:v>0.75056487461552002</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.82948949995140198</c:v>
+                  <c:v>0.80153800081461601</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.78583499934110301</c:v>
+                  <c:v>0.79019256262108595</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.84491361139549104</c:v>
+                  <c:v>0.80484918784350101</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.811335722398426</c:v>
+                  <c:v>0.82444006390869595</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.88879766646358704</c:v>
+                  <c:v>0.84068050095811397</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.83744222256872303</c:v>
+                  <c:v>0.84409362403675903</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.83555377792153096</c:v>
+                  <c:v>0.860603000037372</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.91792288857201698</c:v>
+                  <c:v>0.87704375106841304</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.85683472268283301</c:v>
+                  <c:v>0.86880862526595504</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.92206922276980297</c:v>
+                  <c:v>0.92467824975028601</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.87719394494262004</c:v>
+                  <c:v>0.878106687683612</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.96720411111083204</c:v>
+                  <c:v>0.91236000042408705</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.899489333232243</c:v>
+                  <c:v>0.89544493565335803</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.99032133341663398</c:v>
+                  <c:v>0.95345456199720502</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.92280316642589</c:v>
+                  <c:v>0.91085156193003003</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.00779483322468</c:v>
+                  <c:v>0.989647249691188</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.97174866704477203</c:v>
+                  <c:v>0.97376206237822704</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.02890194435086</c:v>
+                  <c:v>1.0315268123522401</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.0652831668655001</c:v>
+                  <c:v>1.03320712503045</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.09856305540435</c:v>
+                  <c:v>1.05896968767046</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.1128907218161499</c:v>
+                  <c:v>1.0717105632647801</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.17172700001133</c:v>
+                  <c:v>1.0887696859426701</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.15806916666527</c:v>
+                  <c:v>1.11381506221368</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.06420583319332</c:v>
+                  <c:v>1.0617330619134</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.13822727733188</c:v>
+                  <c:v>1.1172992512583699</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.04233694407675</c:v>
+                  <c:v>1.0598551868460999</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.2002873340000699</c:v>
+                  <c:v>1.1480260002426801</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.0503385557482601</c:v>
+                  <c:v>1.0775930006057</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.1917405006372199</c:v>
+                  <c:v>1.15175243932753</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.0653614999933301</c:v>
+                  <c:v>1.1060021254234</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.2313667777925701</c:v>
+                  <c:v>1.1750489370897399</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.09875211140347</c:v>
+                  <c:v>1.1417620629072101</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.25887533297969</c:v>
+                  <c:v>1.2161118127405599</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.2151582783295001</c:v>
+                  <c:v>1.2504325625486601</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.25264494493603</c:v>
+                  <c:v>1.23164212564006</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.3365032221708</c:v>
+                  <c:v>1.26111306156963</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.29315849993791</c:v>
+                  <c:v>1.2899310616776301</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.33646083271337</c:v>
+                  <c:v>1.26966424891725</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.2705005556344899</c:v>
+                  <c:v>1.2419091253541401</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.33116816687915</c:v>
+                  <c:v>1.2942723133601199</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.24674188863072</c:v>
+                  <c:v>1.2016283748671399</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1.3812169451266501</c:v>
+                  <c:v>1.3854302503168501</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.2087348335318999</c:v>
+                  <c:v>1.2040255004539999</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.41294138940672</c:v>
+                  <c:v>1.3439333741553099</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.2161969439022999</c:v>
+                  <c:v>1.2299765618517899</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.4282873330844701</c:v>
+                  <c:v>1.39935700036585</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.2767278336816299</c:v>
+                  <c:v>1.25695087620988</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1.4874513888110701</c:v>
+                  <c:v>1.47827893588691</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1.29863299967514</c:v>
+                  <c:v>1.2872142493724801</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1.5245358890129399</c:v>
+                  <c:v>1.5170100615359801</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1.54560600014196</c:v>
+                  <c:v>1.5911656874231901</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.5359668334325101</c:v>
+                  <c:v>1.50943518662825</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1.59086999980111</c:v>
+                  <c:v>1.5279893744736901</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1.5617407218863499</c:v>
+                  <c:v>1.5115798134356699</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>1.59447000051538</c:v>
+                  <c:v>1.52659987518563</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1.3940732775049001</c:v>
+                  <c:v>1.4287933125160599</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>1.63363555529051</c:v>
+                  <c:v>1.5650997501797901</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1.40429827777875</c:v>
+                  <c:v>1.42840662552043</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1.64669394410318</c:v>
+                  <c:v>1.58606418827548</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>1.3811274444063499</c:v>
+                  <c:v>1.4357484383508501</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1.6596602778881699</c:v>
+                  <c:v>1.6223783139139401</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>1.40439088890949</c:v>
+                  <c:v>1.48612949904054</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>1.6904112220638301</c:v>
+                  <c:v>1.6645513754337999</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1.4447390553024</c:v>
+                  <c:v>1.5379989375360299</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>1.7042882223096101</c:v>
+                  <c:v>1.6482201870530799</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>1.6943401669462499</c:v>
+                  <c:v>1.6616218732669901</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1.7375244444443101</c:v>
+                  <c:v>1.7317581879906301</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1.9059758331212699</c:v>
+                  <c:v>1.77275406243279</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>1.82115272246301</c:v>
+                  <c:v>1.7379474383778799</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>1.78205744404759</c:v>
+                  <c:v>1.7401566253975</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>1.5876966112603701</c:v>
+                  <c:v>1.7272279383614599</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>1.79450838847292</c:v>
+                  <c:v>1.7727095629088501</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>1.60297011087338</c:v>
+                  <c:v>1.6175416875630599</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>1.8280026115890999</c:v>
+                  <c:v>1.79891450051218</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>1.5774916108283701</c:v>
+                  <c:v>1.6368558132089599</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>1.8409437218474001</c:v>
+                  <c:v>1.77758537512272</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>1.5796587218840901</c:v>
+                  <c:v>1.65796218812465</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>1.9275448885228801</c:v>
+                  <c:v>1.83635300118476</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>1.6350606112844399</c:v>
+                  <c:v>1.66436700103804</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>1.9188066114568001</c:v>
+                  <c:v>1.87462399946525</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>1.66594450010193</c:v>
+                  <c:v>1.71441499982029</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>1.95562722264892</c:v>
+                  <c:v>1.9158713137730901</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>2.0274828887648</c:v>
+                  <c:v>1.92541893757879</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>1.96881344397034</c:v>
+                  <c:v>1.9498613746836699</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>2.0283092775692499</c:v>
+                  <c:v>1.96982187591493</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>2.0176236112084598</c:v>
+                  <c:v>1.99480787478387</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>2.01672127739422</c:v>
+                  <c:v>1.9824372502043801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12699,7 +12699,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" sz="1800" baseline="0"/>
-              <a:t>Chart Title</a:t>
+              <a:t>JavaScript Reverse - Own vs Native Methods</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -12789,10 +12789,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>reverse2!$B$3:$B$22</c:f>
+              <c:f>reverse2!$B$3:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -12852,75 +12852,195 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>reverse2!$C$3:$C$22</c:f>
+              <c:f>reverse2!$C$3:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>5.8898342152436502E-3</c:v>
+                  <c:v>1.1196186766028401E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1149223066038501E-2</c:v>
+                  <c:v>1.6369812190532601E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.64694434238804E-2</c:v>
+                  <c:v>2.43306229822337E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1791723039415099E-2</c:v>
+                  <c:v>2.67914389260113E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.71833336187733E-2</c:v>
+                  <c:v>3.3644374459981898E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1593943635622602E-2</c:v>
+                  <c:v>3.9811500348150702E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6756777515014001E-2</c:v>
+                  <c:v>4.5923313125967903E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3084222823381403E-2</c:v>
+                  <c:v>4.6517625451087903E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.8758389221297299E-2</c:v>
+                  <c:v>5.2169687580317203E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5449778007136401E-2</c:v>
+                  <c:v>5.4724812973290599E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.1310333510239901E-2</c:v>
+                  <c:v>6.3656813465058804E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.6149057199557604E-2</c:v>
+                  <c:v>6.6259999759495203E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.9713389691379297E-2</c:v>
+                  <c:v>7.1303311735391603E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.7554222610261694E-2</c:v>
+                  <c:v>7.6617248356342302E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.2535000311003706E-2</c:v>
+                  <c:v>8.2056937273591701E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.5532000081406698E-2</c:v>
+                  <c:v>8.7459499947726699E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.31624443166785E-2</c:v>
+                  <c:v>9.2769123613834298E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.6126498033603E-2</c:v>
+                  <c:v>0.101034186314791</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.8709277394744999E-2</c:v>
+                  <c:v>0.10300812497735</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.10660494574242101</c:v>
+                  <c:v>0.10915737459435999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.108693374320864</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.11760218674317</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.12547562457621</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.12737143691629099</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.13276643725112</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.141481875441968</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.151696812361478</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.15343825053423599</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.153845812194049</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.160094062332063</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.16467187600210301</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.17532849963754399</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.17773874988779401</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.18532768683508</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.18569199973717301</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.19636581279337401</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.201803875621408</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.20804581325501201</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.21241356246173301</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.218072936870157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12972,10 +13092,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>reverse2!$B$3:$B$22</c:f>
+              <c:f>reverse2!$B$3:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>5000</c:v>
                 </c:pt>
@@ -13035,75 +13155,195 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>reverse2!$D$3:$D$22</c:f>
+              <c:f>reverse2!$D$3:$D$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>2.8788667172193499E-2</c:v>
+                  <c:v>1.6376437153667201E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6995110412438699E-2</c:v>
+                  <c:v>3.2153374515473801E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4171054727501299E-2</c:v>
+                  <c:v>4.5387312769889797E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4363222155306002E-2</c:v>
+                  <c:v>5.7279061991721301E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.9593056192000702E-2</c:v>
+                  <c:v>7.3285875376313897E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3494000120295406E-2</c:v>
+                  <c:v>8.7966187391430098E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.105413000202841</c:v>
+                  <c:v>0.105177499353885</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.120231388757626</c:v>
+                  <c:v>0.117016687523573</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13526338794165099</c:v>
+                  <c:v>0.13605537498369799</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.146121667491065</c:v>
+                  <c:v>0.15006937505677301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.160922832373115</c:v>
+                  <c:v>0.16492412565275999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.17908166680071</c:v>
+                  <c:v>0.18001306336372999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18972583239277199</c:v>
+                  <c:v>0.19478281354531601</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.20494733295506901</c:v>
+                  <c:v>0.21016493625938801</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.21880650106403499</c:v>
+                  <c:v>0.22472974937409099</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.233332666671938</c:v>
+                  <c:v>0.23368493607267701</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25293794439898598</c:v>
+                  <c:v>0.25480700051411898</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.270062777731153</c:v>
+                  <c:v>0.26838706200942303</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.27826966635055</c:v>
+                  <c:v>0.27895549964159699</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.29146194499399902</c:v>
+                  <c:v>0.29991768766194499</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.31161593692377199</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.323901999276131</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.343023498542606</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.350884687621146</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.365783376619219</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.38357606157660401</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.41171668889001001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.42007593810558302</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.42149556241929498</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.436957125551998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.45125900069251601</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.471608936786651</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.49377443781122499</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.48778856405988302</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.51640306320041396</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.53925943747162797</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.55409681238233999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.57646674942225196</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.58828618843108405</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.60639425041154005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13111,7 +13351,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0816-5B41-BC58-75877A0D362E}"/>
+              <c16:uniqueId val="{00000000-3B31-4C49-AB80-0E860BCBBE49}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13360,10 +13600,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26858432139138061"/>
-          <c:y val="0.90752687115358643"/>
-          <c:w val="0.47464847056530929"/>
-          <c:h val="8.3464075570896856E-2"/>
+          <c:x val="0.28275809730436757"/>
+          <c:y val="0.92277192938932906"/>
+          <c:w val="0.44951343352043777"/>
+          <c:h val="5.6901313996772528E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -16604,15 +16844,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:colOff>669739</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90127</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>597647</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>96051</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17690,8 +17930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BD8F9E-1DE2-FD48-A0FF-3C810CF2B391}">
   <dimension ref="B2:M152"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView showGridLines="0" topLeftCell="K1" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17749,8 +17989,8 @@
       <c r="H3">
         <v>10000</v>
       </c>
-      <c r="I3">
-        <v>1.65192219946119E-2</v>
+      <c r="I3" s="2">
+        <v>2.1154250483959899E-2</v>
       </c>
       <c r="J3">
         <v>8.9562777801701302E-3</v>
@@ -17787,8 +18027,8 @@
         <f>H3+10000</f>
         <v>20000</v>
       </c>
-      <c r="I4">
-        <v>3.6741556185814997E-2</v>
+      <c r="I4" s="2">
+        <v>4.1609874460846102E-2</v>
       </c>
       <c r="J4">
         <v>1.6776444448623799E-2</v>
@@ -17825,8 +18065,8 @@
         <f t="shared" ref="H5:H68" si="1">H4+10000</f>
         <v>30000</v>
       </c>
-      <c r="I5">
-        <v>3.9989332978924097E-2</v>
+      <c r="I5" s="2">
+        <v>3.9775499608367598E-2</v>
       </c>
       <c r="J5">
         <v>2.4572111113229701E-2</v>
@@ -17863,8 +18103,8 @@
         <f t="shared" si="1"/>
         <v>40000</v>
       </c>
-      <c r="I6">
-        <v>5.2832444301909802E-2</v>
+      <c r="I6" s="2">
+        <v>5.3126689046621302E-2</v>
       </c>
       <c r="J6">
         <v>3.1841166666708803E-2</v>
@@ -17901,8 +18141,8 @@
         <f t="shared" si="1"/>
         <v>50000</v>
       </c>
-      <c r="I7">
-        <v>6.0375777797566497E-2</v>
+      <c r="I7" s="2">
+        <v>6.4531625714152996E-2</v>
       </c>
       <c r="J7">
         <v>3.9617444443542302E-2</v>
@@ -17939,8 +18179,8 @@
         <f t="shared" si="1"/>
         <v>60000</v>
       </c>
-      <c r="I8">
-        <v>6.9418166453639601E-2</v>
+      <c r="I8" s="2">
+        <v>6.9532250054180594E-2</v>
       </c>
       <c r="J8">
         <v>4.7108166668395901E-2</v>
@@ -17977,8 +18217,8 @@
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="I9">
-        <v>7.6582444417807705E-2</v>
+      <c r="I9" s="2">
+        <v>7.6579438522457993E-2</v>
       </c>
       <c r="J9">
         <v>5.4665111112020201E-2</v>
@@ -18015,8 +18255,8 @@
         <f t="shared" si="1"/>
         <v>80000</v>
       </c>
-      <c r="I10">
-        <v>8.7434110749098903E-2</v>
+      <c r="I10" s="2">
+        <v>8.7750438600778496E-2</v>
       </c>
       <c r="J10">
         <v>6.1942500004079103E-2</v>
@@ -18053,8 +18293,8 @@
         <f t="shared" si="1"/>
         <v>90000</v>
       </c>
-      <c r="I11">
-        <v>0.103699610672063</v>
+      <c r="I11" s="2">
+        <v>9.8237999714910901E-2</v>
       </c>
       <c r="J11">
         <v>6.9440500003919506E-2</v>
@@ -18091,8 +18331,8 @@
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-      <c r="I12">
-        <v>0.112765499908063</v>
+      <c r="I12" s="2">
+        <v>0.10925512574613</v>
       </c>
       <c r="J12">
         <v>7.6833444443764096E-2</v>
@@ -18129,8 +18369,8 @@
         <f t="shared" si="1"/>
         <v>110000</v>
       </c>
-      <c r="I13">
-        <v>0.122282667292488</v>
+      <c r="I13" s="2">
+        <v>0.12516206270083699</v>
       </c>
       <c r="J13">
         <v>8.5207055562124004E-2</v>
@@ -18167,8 +18407,8 @@
         <f t="shared" si="1"/>
         <v>120000</v>
       </c>
-      <c r="I14">
-        <v>0.13525855561925301</v>
+      <c r="I14" s="2">
+        <v>0.127371250186115</v>
       </c>
       <c r="J14">
         <v>9.1661777774182399E-2</v>
@@ -18205,8 +18445,8 @@
         <f t="shared" si="1"/>
         <v>130000</v>
       </c>
-      <c r="I15">
-        <v>0.14186933284832301</v>
+      <c r="I15" s="2">
+        <v>0.14221718674525599</v>
       </c>
       <c r="J15">
         <v>9.9159388891873895E-2</v>
@@ -18243,8 +18483,8 @@
         <f t="shared" si="1"/>
         <v>140000</v>
       </c>
-      <c r="I16">
-        <v>0.152899666999777</v>
+      <c r="I16" s="2">
+        <v>0.155403499491512</v>
       </c>
       <c r="J16">
         <v>0.10655249999965399</v>
@@ -18281,8 +18521,8 @@
         <f t="shared" si="1"/>
         <v>150000</v>
       </c>
-      <c r="I17">
-        <v>0.16398572197390901</v>
+      <c r="I17" s="2">
+        <v>0.16445687552914001</v>
       </c>
       <c r="J17">
         <v>0.11571683333022501</v>
@@ -18319,8 +18559,8 @@
         <f t="shared" si="1"/>
         <v>160000</v>
       </c>
-      <c r="I18">
-        <v>0.174337555550866</v>
+      <c r="I18" s="2">
+        <v>0.17444856185466001</v>
       </c>
       <c r="J18">
         <v>0.1212836111097</v>
@@ -18357,8 +18597,8 @@
         <f t="shared" si="1"/>
         <v>170000</v>
       </c>
-      <c r="I19">
-        <v>0.185257555089063</v>
+      <c r="I19" s="2">
+        <v>0.18688512500375501</v>
       </c>
       <c r="J19">
         <v>0.12938838889304899</v>
@@ -18395,8 +18635,8 @@
         <f t="shared" si="1"/>
         <v>180000</v>
       </c>
-      <c r="I20">
-        <v>0.198314944282174</v>
+      <c r="I20" s="2">
+        <v>0.19804312614724001</v>
       </c>
       <c r="J20">
         <v>0.13623450000240001</v>
@@ -18433,8 +18673,8 @@
         <f t="shared" si="1"/>
         <v>190000</v>
       </c>
-      <c r="I21">
-        <v>0.207088889347182</v>
+      <c r="I21" s="2">
+        <v>0.20776350004598401</v>
       </c>
       <c r="J21">
         <v>0.147257055555302</v>
@@ -18471,8 +18711,8 @@
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
-      <c r="I22">
-        <v>0.21795538854267801</v>
+      <c r="I22" s="2">
+        <v>0.217996062245219</v>
       </c>
       <c r="J22">
         <v>0.15194055555265401</v>
@@ -18509,8 +18749,8 @@
         <f t="shared" si="1"/>
         <v>210000</v>
       </c>
-      <c r="I23">
-        <v>0.23580177790588799</v>
+      <c r="I23" s="2">
+        <v>0.228582374285906</v>
       </c>
       <c r="J23">
         <v>0.16078122221774199</v>
@@ -18547,8 +18787,8 @@
         <f t="shared" si="1"/>
         <v>220000</v>
       </c>
-      <c r="I24">
-        <v>0.23989100029898999</v>
+      <c r="I24" s="2">
+        <v>0.24134500185027699</v>
       </c>
       <c r="J24">
         <v>0.16667638889015901</v>
@@ -18585,8 +18825,8 @@
         <f t="shared" si="1"/>
         <v>230000</v>
       </c>
-      <c r="I25">
-        <v>0.25105499952203603</v>
+      <c r="I25" s="2">
+        <v>0.258339312393218</v>
       </c>
       <c r="J25">
         <v>0.17482333333464301</v>
@@ -18623,8 +18863,8 @@
         <f t="shared" si="1"/>
         <v>240000</v>
       </c>
-      <c r="I26">
-        <v>0.26169955647653997</v>
+      <c r="I26" s="2">
+        <v>0.27673525083810002</v>
       </c>
       <c r="J26">
         <v>0.18144222221841699</v>
@@ -18661,8 +18901,8 @@
         <f t="shared" si="1"/>
         <v>250000</v>
       </c>
-      <c r="I27">
-        <v>0.28076816660662401</v>
+      <c r="I27" s="2">
+        <v>0.27936912514269302</v>
       </c>
       <c r="J27">
         <v>0.18952394444204401</v>
@@ -18699,8 +18939,8 @@
         <f t="shared" si="1"/>
         <v>260000</v>
       </c>
-      <c r="I28">
-        <v>0.27567249991827503</v>
+      <c r="I28" s="2">
+        <v>0.28894506255164698</v>
       </c>
       <c r="J28">
         <v>0.20475816666213201</v>
@@ -18737,8 +18977,8 @@
         <f t="shared" si="1"/>
         <v>270000</v>
       </c>
-      <c r="I29">
-        <v>0.29453094427784199</v>
+      <c r="I29" s="2">
+        <v>0.30232049990445298</v>
       </c>
       <c r="J29">
         <v>0.20946633333126799</v>
@@ -18775,8 +19015,8 @@
         <f t="shared" si="1"/>
         <v>280000</v>
       </c>
-      <c r="I30">
-        <v>0.30670361055268103</v>
+      <c r="I30" s="2">
+        <v>0.31637181201949699</v>
       </c>
       <c r="J30">
         <v>0.21149933333152901</v>
@@ -18813,8 +19053,8 @@
         <f t="shared" si="1"/>
         <v>290000</v>
       </c>
-      <c r="I31">
-        <v>0.30463700058559501</v>
+      <c r="I31" s="2">
+        <v>0.32132274983450698</v>
       </c>
       <c r="J31">
         <v>0.220633833332815</v>
@@ -18851,8 +19091,8 @@
         <f t="shared" si="1"/>
         <v>300000</v>
       </c>
-      <c r="I32">
-        <v>0.31897322212656298</v>
+      <c r="I32" s="2">
+        <v>0.328818999230861</v>
       </c>
       <c r="J32">
         <v>0.22789444444545801</v>
@@ -18872,8 +19112,8 @@
         <f t="shared" si="1"/>
         <v>310000</v>
       </c>
-      <c r="I33">
-        <v>0.335588833524121</v>
+      <c r="I33" s="2">
+        <v>0.35090656299144002</v>
       </c>
       <c r="J33">
         <v>0.24107905555704001</v>
@@ -18893,8 +19133,8 @@
         <f t="shared" si="1"/>
         <v>320000</v>
       </c>
-      <c r="I34">
-        <v>0.34544855542480901</v>
+      <c r="I34" s="2">
+        <v>0.36370181152596998</v>
       </c>
       <c r="J34">
         <v>0.24116794444529999</v>
@@ -18914,8 +19154,8 @@
         <f t="shared" si="1"/>
         <v>330000</v>
       </c>
-      <c r="I35">
-        <v>0.36436033331685502</v>
+      <c r="I35" s="2">
+        <v>0.37182837445288802</v>
       </c>
       <c r="J35">
         <v>0.248605722225167</v>
@@ -18935,8 +19175,8 @@
         <f t="shared" si="1"/>
         <v>340000</v>
       </c>
-      <c r="I36">
-        <v>0.36917938850819998</v>
+      <c r="I36" s="2">
+        <v>0.39172093570232303</v>
       </c>
       <c r="J36">
         <v>0.25626355555302999</v>
@@ -18956,8 +19196,8 @@
         <f t="shared" si="1"/>
         <v>350000</v>
       </c>
-      <c r="I37">
-        <v>0.37215911121004103</v>
+      <c r="I37" s="2">
+        <v>0.39265649951994402</v>
       </c>
       <c r="J37">
         <v>0.270054833334547</v>
@@ -18977,8 +19217,8 @@
         <f t="shared" si="1"/>
         <v>360000</v>
       </c>
-      <c r="I38">
-        <v>0.38841388809184202</v>
+      <c r="I38" s="2">
+        <v>0.40224818745627999</v>
       </c>
       <c r="J38">
         <v>0.27111594444916798</v>
@@ -18998,8 +19238,8 @@
         <f t="shared" si="1"/>
         <v>370000</v>
       </c>
-      <c r="I39">
-        <v>0.39870888843304497</v>
+      <c r="I39" s="2">
+        <v>0.41913743782788498</v>
       </c>
       <c r="J39">
         <v>0.292327999999138</v>
@@ -19019,8 +19259,8 @@
         <f t="shared" si="1"/>
         <v>380000</v>
       </c>
-      <c r="I40">
-        <v>0.398507944204741</v>
+      <c r="I40" s="2">
+        <v>0.44802825106307798</v>
       </c>
       <c r="J40">
         <v>0.28860450000340399</v>
@@ -19040,8 +19280,8 @@
         <f t="shared" si="1"/>
         <v>390000</v>
       </c>
-      <c r="I41">
-        <v>0.42161077799068503</v>
+      <c r="I41" s="2">
+        <v>0.45671699987724401</v>
       </c>
       <c r="J41">
         <v>0.30630772221936903</v>
@@ -19061,8 +19301,8 @@
         <f t="shared" si="1"/>
         <v>400000</v>
       </c>
-      <c r="I42">
-        <v>0.45855361140436501</v>
+      <c r="I42" s="2">
+        <v>0.46248949924483801</v>
       </c>
       <c r="J42">
         <v>0.30454349999814001</v>
@@ -19082,8 +19322,8 @@
         <f t="shared" si="1"/>
         <v>410000</v>
       </c>
-      <c r="I43">
-        <v>0.47183594438764698</v>
+      <c r="I43" s="2">
+        <v>0.48339949967339602</v>
       </c>
       <c r="J43">
         <v>0.32077744444379402</v>
@@ -19103,8 +19343,8 @@
         <f t="shared" si="1"/>
         <v>420000</v>
       </c>
-      <c r="I44">
-        <v>0.47680811087290398</v>
+      <c r="I44" s="2">
+        <v>0.478339249268174</v>
       </c>
       <c r="J44">
         <v>0.32061900000068499</v>
@@ -19124,8 +19364,8 @@
         <f t="shared" si="1"/>
         <v>430000</v>
       </c>
-      <c r="I45">
-        <v>0.49395338942607198</v>
+      <c r="I45" s="2">
+        <v>0.495697874110192</v>
       </c>
       <c r="J45">
         <v>0.32634183333397598</v>
@@ -19145,8 +19385,8 @@
         <f t="shared" si="1"/>
         <v>440000</v>
       </c>
-      <c r="I46">
-        <v>0.50581522223850095</v>
+      <c r="I46" s="2">
+        <v>0.50081262318417397</v>
       </c>
       <c r="J46">
         <v>0.331448555552116</v>
@@ -19166,8 +19406,8 @@
         <f t="shared" si="1"/>
         <v>450000</v>
       </c>
-      <c r="I47">
-        <v>0.51915055534078003</v>
+      <c r="I47" s="2">
+        <v>0.52699243789538697</v>
       </c>
       <c r="J47">
         <v>0.34322211111106699</v>
@@ -19187,8 +19427,8 @@
         <f t="shared" si="1"/>
         <v>460000</v>
       </c>
-      <c r="I48">
-        <v>0.51764361167119599</v>
+      <c r="I48" s="2">
+        <v>0.52963187498971798</v>
       </c>
       <c r="J48">
         <v>0.35620872222029398</v>
@@ -19208,8 +19448,8 @@
         <f t="shared" si="1"/>
         <v>470000</v>
       </c>
-      <c r="I49">
-        <v>0.54527844405836501</v>
+      <c r="I49" s="2">
+        <v>0.53135731071233705</v>
       </c>
       <c r="J49">
         <v>0.355546666669801</v>
@@ -19229,8 +19469,8 @@
         <f t="shared" si="1"/>
         <v>480000</v>
       </c>
-      <c r="I50">
-        <v>0.54937505535781295</v>
+      <c r="I50" s="2">
+        <v>0.55346756149083298</v>
       </c>
       <c r="J50">
         <v>0.36580122222787598</v>
@@ -19250,8 +19490,8 @@
         <f t="shared" si="1"/>
         <v>490000</v>
       </c>
-      <c r="I51">
-        <v>0.59842027765181305</v>
+      <c r="I51" s="2">
+        <v>0.58196600060909898</v>
       </c>
       <c r="J51">
         <v>0.37769644444213302</v>
@@ -19271,8 +19511,8 @@
         <f t="shared" si="1"/>
         <v>500000</v>
       </c>
-      <c r="I52">
-        <v>0.59515772242512899</v>
+      <c r="I52" s="2">
+        <v>0.58562649972736802</v>
       </c>
       <c r="J52">
         <v>0.39821666666507</v>
@@ -19292,8 +19532,8 @@
         <f t="shared" si="1"/>
         <v>510000</v>
       </c>
-      <c r="I53">
-        <v>0.60738555652399795</v>
+      <c r="I53" s="2">
+        <v>0.59332968713715595</v>
       </c>
       <c r="J53">
         <v>0.38916399999450502</v>
@@ -19313,8 +19553,8 @@
         <f t="shared" si="1"/>
         <v>520000</v>
       </c>
-      <c r="I54">
-        <v>0.61161377798351901</v>
+      <c r="I54" s="2">
+        <v>0.60989662585780002</v>
       </c>
       <c r="J54">
         <v>0.40514472222356601</v>
@@ -19334,8 +19574,8 @@
         <f t="shared" si="1"/>
         <v>530000</v>
       </c>
-      <c r="I55">
-        <v>0.62744916602969103</v>
+      <c r="I55" s="2">
+        <v>0.62941162614151802</v>
       </c>
       <c r="J55">
         <v>0.40971588888593602</v>
@@ -19355,8 +19595,8 @@
         <f t="shared" si="1"/>
         <v>540000</v>
       </c>
-      <c r="I56">
-        <v>0.65664727758202202</v>
+      <c r="I56" s="2">
+        <v>0.65847231168299902</v>
       </c>
       <c r="J56">
         <v>0.41131899999648602</v>
@@ -19376,8 +19616,8 @@
         <f t="shared" si="1"/>
         <v>550000</v>
       </c>
-      <c r="I57">
-        <v>0.65469522194729901</v>
+      <c r="I57" s="2">
+        <v>0.64366231206804503</v>
       </c>
       <c r="J57">
         <v>0.43238505555523699</v>
@@ -19397,8 +19637,8 @@
         <f t="shared" si="1"/>
         <v>560000</v>
       </c>
-      <c r="I58">
-        <v>0.66398927755653803</v>
+      <c r="I58" s="2">
+        <v>0.64640106214210302</v>
       </c>
       <c r="J58">
         <v>0.432678111109352</v>
@@ -19418,8 +19658,8 @@
         <f t="shared" si="1"/>
         <v>570000</v>
       </c>
-      <c r="I59">
-        <v>0.67323100028766503</v>
+      <c r="I59" s="2">
+        <v>0.68013862473890097</v>
       </c>
       <c r="J59">
         <v>0.4459895000004</v>
@@ -19439,8 +19679,8 @@
         <f t="shared" si="1"/>
         <v>580000</v>
       </c>
-      <c r="I60">
-        <v>0.71820933371782303</v>
+      <c r="I60" s="2">
+        <v>0.69856343790888697</v>
       </c>
       <c r="J60">
         <v>0.46014016666837598</v>
@@ -19460,8 +19700,8 @@
         <f t="shared" si="1"/>
         <v>590000</v>
       </c>
-      <c r="I61">
-        <v>0.69090472182465901</v>
+      <c r="I61" s="2">
+        <v>0.68299287464469605</v>
       </c>
       <c r="J61">
         <v>0.45963672222246199</v>
@@ -19481,8 +19721,8 @@
         <f t="shared" si="1"/>
         <v>600000</v>
       </c>
-      <c r="I62">
-        <v>0.73486249976687901</v>
+      <c r="I62" s="2">
+        <v>0.721210563089698</v>
       </c>
       <c r="J62">
         <v>0.47001788889206603</v>
@@ -19502,8 +19742,8 @@
         <f t="shared" si="1"/>
         <v>610000</v>
       </c>
-      <c r="I63">
-        <v>0.72236872195369595</v>
+      <c r="I63" s="2">
+        <v>0.72887293761595995</v>
       </c>
       <c r="J63">
         <v>0.46709733333166997</v>
@@ -19523,8 +19763,8 @@
         <f t="shared" si="1"/>
         <v>620000</v>
       </c>
-      <c r="I64">
-        <v>0.77505500055849497</v>
+      <c r="I64" s="2">
+        <v>0.74672987358644605</v>
       </c>
       <c r="J64">
         <v>0.49560088888716097</v>
@@ -19544,8 +19784,8 @@
         <f t="shared" si="1"/>
         <v>630000</v>
       </c>
-      <c r="I65">
-        <v>0.75990438813136596</v>
+      <c r="I65" s="2">
+        <v>0.75056487461552002</v>
       </c>
       <c r="J65">
         <v>0.50706222222167197</v>
@@ -19565,8 +19805,8 @@
         <f t="shared" si="1"/>
         <v>640000</v>
       </c>
-      <c r="I66">
-        <v>0.82948949995140198</v>
+      <c r="I66" s="2">
+        <v>0.80153800081461601</v>
       </c>
       <c r="J66">
         <v>0.51011105555355396</v>
@@ -19586,8 +19826,8 @@
         <f t="shared" si="1"/>
         <v>650000</v>
       </c>
-      <c r="I67">
-        <v>0.78583499934110301</v>
+      <c r="I67" s="2">
+        <v>0.79019256262108595</v>
       </c>
       <c r="J67">
         <v>0.51294550000036698</v>
@@ -19607,8 +19847,8 @@
         <f t="shared" si="1"/>
         <v>660000</v>
       </c>
-      <c r="I68">
-        <v>0.84491361139549104</v>
+      <c r="I68" s="2">
+        <v>0.80484918784350101</v>
       </c>
       <c r="J68">
         <v>0.49965194444262601</v>
@@ -19628,8 +19868,8 @@
         <f t="shared" ref="H69:H132" si="2">H68+10000</f>
         <v>670000</v>
       </c>
-      <c r="I69">
-        <v>0.811335722398426</v>
+      <c r="I69" s="2">
+        <v>0.82444006390869595</v>
       </c>
       <c r="J69">
         <v>0.52772038889330897</v>
@@ -19649,8 +19889,8 @@
         <f t="shared" si="2"/>
         <v>680000</v>
       </c>
-      <c r="I70">
-        <v>0.88879766646358704</v>
+      <c r="I70" s="2">
+        <v>0.84068050095811397</v>
       </c>
       <c r="J70">
         <v>0.53776661111138901</v>
@@ -19670,8 +19910,8 @@
         <f t="shared" si="2"/>
         <v>690000</v>
       </c>
-      <c r="I71">
-        <v>0.83744222256872303</v>
+      <c r="I71" s="2">
+        <v>0.84409362403675903</v>
       </c>
       <c r="J71">
         <v>0.54047261110584499</v>
@@ -19691,8 +19931,8 @@
         <f t="shared" si="2"/>
         <v>700000</v>
       </c>
-      <c r="I72">
-        <v>0.83555377792153096</v>
+      <c r="I72" s="2">
+        <v>0.860603000037372</v>
       </c>
       <c r="J72">
         <v>0.55388399999679205</v>
@@ -19712,8 +19952,8 @@
         <f t="shared" si="2"/>
         <v>710000</v>
       </c>
-      <c r="I73">
-        <v>0.91792288857201698</v>
+      <c r="I73" s="2">
+        <v>0.87704375106841304</v>
       </c>
       <c r="J73">
         <v>0.56470511111223798</v>
@@ -19733,8 +19973,8 @@
         <f t="shared" si="2"/>
         <v>720000</v>
       </c>
-      <c r="I74">
-        <v>0.85683472268283301</v>
+      <c r="I74" s="2">
+        <v>0.86880862526595504</v>
       </c>
       <c r="J74">
         <v>0.553097055555554</v>
@@ -19754,8 +19994,8 @@
         <f t="shared" si="2"/>
         <v>730000</v>
       </c>
-      <c r="I75">
-        <v>0.92206922276980297</v>
+      <c r="I75" s="2">
+        <v>0.92467824975028601</v>
       </c>
       <c r="J75">
         <v>0.570997611111832</v>
@@ -19775,8 +20015,8 @@
         <f t="shared" si="2"/>
         <v>740000</v>
       </c>
-      <c r="I76">
-        <v>0.87719394494262004</v>
+      <c r="I76" s="2">
+        <v>0.878106687683612</v>
       </c>
       <c r="J76">
         <v>0.57331272222088703</v>
@@ -19796,8 +20036,8 @@
         <f t="shared" si="2"/>
         <v>750000</v>
       </c>
-      <c r="I77">
-        <v>0.96720411111083204</v>
+      <c r="I77" s="2">
+        <v>0.91236000042408705</v>
       </c>
       <c r="J77">
         <v>0.57543661111331901</v>
@@ -19817,8 +20057,8 @@
         <f t="shared" si="2"/>
         <v>760000</v>
       </c>
-      <c r="I78">
-        <v>0.899489333232243</v>
+      <c r="I78" s="2">
+        <v>0.89544493565335803</v>
       </c>
       <c r="J78">
         <v>0.57881272222180502</v>
@@ -19838,8 +20078,8 @@
         <f t="shared" si="2"/>
         <v>770000</v>
       </c>
-      <c r="I79">
-        <v>0.99032133341663398</v>
+      <c r="I79" s="2">
+        <v>0.95345456199720502</v>
       </c>
       <c r="J79">
         <v>0.59390683333104799</v>
@@ -19859,8 +20099,8 @@
         <f t="shared" si="2"/>
         <v>780000</v>
       </c>
-      <c r="I80">
-        <v>0.92280316642589</v>
+      <c r="I80" s="2">
+        <v>0.91085156193003003</v>
       </c>
       <c r="J80">
         <v>0.59783183333638501</v>
@@ -19880,8 +20120,8 @@
         <f t="shared" si="2"/>
         <v>790000</v>
       </c>
-      <c r="I81">
-        <v>1.00779483322468</v>
+      <c r="I81" s="2">
+        <v>0.989647249691188</v>
       </c>
       <c r="J81">
         <v>0.62471011111564501</v>
@@ -19901,8 +20141,8 @@
         <f t="shared" si="2"/>
         <v>800000</v>
       </c>
-      <c r="I82">
-        <v>0.97174866704477203</v>
+      <c r="I82" s="2">
+        <v>0.97376206237822704</v>
       </c>
       <c r="J82">
         <v>0.61927850000211004</v>
@@ -19922,8 +20162,8 @@
         <f t="shared" si="2"/>
         <v>810000</v>
       </c>
-      <c r="I83">
-        <v>1.02890194435086</v>
+      <c r="I83" s="2">
+        <v>1.0315268123522401</v>
       </c>
       <c r="J83">
         <v>0.62540022222027702</v>
@@ -19943,8 +20183,8 @@
         <f t="shared" si="2"/>
         <v>820000</v>
       </c>
-      <c r="I84">
-        <v>1.0652831668655001</v>
+      <c r="I84" s="2">
+        <v>1.03320712503045</v>
       </c>
       <c r="J84">
         <v>0.638380055558324</v>
@@ -19964,8 +20204,8 @@
         <f t="shared" si="2"/>
         <v>830000</v>
       </c>
-      <c r="I85">
-        <v>1.09856305540435</v>
+      <c r="I85" s="2">
+        <v>1.05896968767046</v>
       </c>
       <c r="J85">
         <v>0.64592805555245503</v>
@@ -19985,8 +20225,8 @@
         <f t="shared" si="2"/>
         <v>840000</v>
       </c>
-      <c r="I86">
-        <v>1.1128907218161499</v>
+      <c r="I86" s="2">
+        <v>1.0717105632647801</v>
       </c>
       <c r="J86">
         <v>0.66486022222670704</v>
@@ -20006,8 +20246,8 @@
         <f t="shared" si="2"/>
         <v>850000</v>
       </c>
-      <c r="I87">
-        <v>1.17172700001133</v>
+      <c r="I87" s="2">
+        <v>1.0887696859426701</v>
       </c>
       <c r="J87">
         <v>0.66770000000219099</v>
@@ -20027,8 +20267,8 @@
         <f t="shared" si="2"/>
         <v>860000</v>
       </c>
-      <c r="I88">
-        <v>1.15806916666527</v>
+      <c r="I88" s="2">
+        <v>1.11381506221368</v>
       </c>
       <c r="J88">
         <v>0.67633722221944403</v>
@@ -20048,8 +20288,8 @@
         <f t="shared" si="2"/>
         <v>870000</v>
       </c>
-      <c r="I89">
-        <v>1.06420583319332</v>
+      <c r="I89" s="2">
+        <v>1.0617330619134</v>
       </c>
       <c r="J89">
         <v>0.68776800000179905</v>
@@ -20069,8 +20309,8 @@
         <f t="shared" si="2"/>
         <v>880000</v>
       </c>
-      <c r="I90">
-        <v>1.13822727733188</v>
+      <c r="I90" s="2">
+        <v>1.1172992512583699</v>
       </c>
       <c r="J90">
         <v>0.69927333333341901</v>
@@ -20090,8 +20330,8 @@
         <f t="shared" si="2"/>
         <v>890000</v>
       </c>
-      <c r="I91">
-        <v>1.04233694407675</v>
+      <c r="I91" s="2">
+        <v>1.0598551868460999</v>
       </c>
       <c r="J91">
         <v>0.69272433333228201</v>
@@ -20111,8 +20351,8 @@
         <f t="shared" si="2"/>
         <v>900000</v>
       </c>
-      <c r="I92">
-        <v>1.2002873340000699</v>
+      <c r="I92" s="2">
+        <v>1.1480260002426801</v>
       </c>
       <c r="J92">
         <v>0.707018222216801</v>
@@ -20132,8 +20372,8 @@
         <f t="shared" si="2"/>
         <v>910000</v>
       </c>
-      <c r="I93">
-        <v>1.0503385557482601</v>
+      <c r="I93" s="2">
+        <v>1.0775930006057</v>
       </c>
       <c r="J93">
         <v>0.71080472222011903</v>
@@ -20153,8 +20393,8 @@
         <f t="shared" si="2"/>
         <v>920000</v>
       </c>
-      <c r="I94">
-        <v>1.1917405006372199</v>
+      <c r="I94" s="2">
+        <v>1.15175243932753</v>
       </c>
       <c r="J94">
         <v>0.72109205555655798</v>
@@ -20174,8 +20414,8 @@
         <f t="shared" si="2"/>
         <v>930000</v>
       </c>
-      <c r="I95">
-        <v>1.0653614999933301</v>
+      <c r="I95" s="2">
+        <v>1.1060021254234</v>
       </c>
       <c r="J95">
         <v>0.706444722221931</v>
@@ -20195,8 +20435,8 @@
         <f t="shared" si="2"/>
         <v>940000</v>
       </c>
-      <c r="I96">
-        <v>1.2313667777925701</v>
+      <c r="I96" s="2">
+        <v>1.1750489370897399</v>
       </c>
       <c r="J96">
         <v>0.74662227778106904</v>
@@ -20216,8 +20456,8 @@
         <f t="shared" si="2"/>
         <v>950000</v>
       </c>
-      <c r="I97">
-        <v>1.09875211140347</v>
+      <c r="I97" s="2">
+        <v>1.1417620629072101</v>
       </c>
       <c r="J97">
         <v>0.73557261110949501</v>
@@ -20237,8 +20477,8 @@
         <f t="shared" si="2"/>
         <v>960000</v>
       </c>
-      <c r="I98">
-        <v>1.25887533297969</v>
+      <c r="I98" s="2">
+        <v>1.2161118127405599</v>
       </c>
       <c r="J98">
         <v>0.73289655555628097</v>
@@ -20258,8 +20498,8 @@
         <f t="shared" si="2"/>
         <v>970000</v>
       </c>
-      <c r="I99">
-        <v>1.2151582783295001</v>
+      <c r="I99" s="2">
+        <v>1.2504325625486601</v>
       </c>
       <c r="J99">
         <v>0.76779238888896795</v>
@@ -20279,8 +20519,8 @@
         <f t="shared" si="2"/>
         <v>980000</v>
       </c>
-      <c r="I100">
-        <v>1.25264494493603</v>
+      <c r="I100" s="2">
+        <v>1.23164212564006</v>
       </c>
       <c r="J100">
         <v>0.77526866666772098</v>
@@ -20300,8 +20540,8 @@
         <f t="shared" si="2"/>
         <v>990000</v>
       </c>
-      <c r="I101">
-        <v>1.3365032221708</v>
+      <c r="I101" s="2">
+        <v>1.26111306156963</v>
       </c>
       <c r="J101">
         <v>0.78259377777835104</v>
@@ -20321,8 +20561,8 @@
         <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
-      <c r="I102">
-        <v>1.29315849993791</v>
+      <c r="I102" s="2">
+        <v>1.2899310616776301</v>
       </c>
       <c r="J102">
         <v>0.78872038888867801</v>
@@ -20342,8 +20582,8 @@
         <f t="shared" si="2"/>
         <v>1010000</v>
       </c>
-      <c r="I103">
-        <v>1.33646083271337</v>
+      <c r="I103" s="2">
+        <v>1.26966424891725</v>
       </c>
       <c r="J103">
         <v>0.78747361111163605</v>
@@ -20363,8 +20603,8 @@
         <f t="shared" si="2"/>
         <v>1020000</v>
       </c>
-      <c r="I104">
-        <v>1.2705005556344899</v>
+      <c r="I104" s="2">
+        <v>1.2419091253541401</v>
       </c>
       <c r="J104">
         <v>0.78500483333482396</v>
@@ -20384,8 +20624,8 @@
         <f t="shared" si="2"/>
         <v>1030000</v>
       </c>
-      <c r="I105">
-        <v>1.33116816687915</v>
+      <c r="I105" s="2">
+        <v>1.2942723133601199</v>
       </c>
       <c r="J105">
         <v>0.82691805554915998</v>
@@ -20405,8 +20645,8 @@
         <f t="shared" si="2"/>
         <v>1040000</v>
       </c>
-      <c r="I106">
-        <v>1.24674188863072</v>
+      <c r="I106" s="2">
+        <v>1.2016283748671399</v>
       </c>
       <c r="J106">
         <v>0.81122133333216495</v>
@@ -20426,8 +20666,8 @@
         <f t="shared" si="2"/>
         <v>1050000</v>
       </c>
-      <c r="I107">
-        <v>1.3812169451266501</v>
+      <c r="I107" s="2">
+        <v>1.3854302503168501</v>
       </c>
       <c r="J107">
         <v>0.82848861111657801</v>
@@ -20447,8 +20687,8 @@
         <f t="shared" si="2"/>
         <v>1060000</v>
       </c>
-      <c r="I108">
-        <v>1.2087348335318999</v>
+      <c r="I108" s="2">
+        <v>1.2040255004539999</v>
       </c>
       <c r="J108">
         <v>0.83134494444594598</v>
@@ -20468,8 +20708,8 @@
         <f t="shared" si="2"/>
         <v>1070000</v>
       </c>
-      <c r="I109">
-        <v>1.41294138940672</v>
+      <c r="I109" s="2">
+        <v>1.3439333741553099</v>
       </c>
       <c r="J109">
         <v>0.861744166665529</v>
@@ -20489,8 +20729,8 @@
         <f t="shared" si="2"/>
         <v>1080000</v>
       </c>
-      <c r="I110">
-        <v>1.2161969439022999</v>
+      <c r="I110" s="2">
+        <v>1.2299765618517899</v>
       </c>
       <c r="J110">
         <v>0.858155555555842</v>
@@ -20510,8 +20750,8 @@
         <f t="shared" si="2"/>
         <v>1090000</v>
       </c>
-      <c r="I111">
-        <v>1.4282873330844701</v>
+      <c r="I111" s="2">
+        <v>1.39935700036585</v>
       </c>
       <c r="J111">
         <v>0.85489911110845296</v>
@@ -20531,8 +20771,8 @@
         <f t="shared" si="2"/>
         <v>1100000</v>
       </c>
-      <c r="I112">
-        <v>1.2767278336816299</v>
+      <c r="I112" s="2">
+        <v>1.25695087620988</v>
       </c>
       <c r="J112">
         <v>0.86826938888730598</v>
@@ -20552,8 +20792,8 @@
         <f t="shared" si="2"/>
         <v>1110000</v>
       </c>
-      <c r="I113">
-        <v>1.4874513888110701</v>
+      <c r="I113" s="2">
+        <v>1.47827893588691</v>
       </c>
       <c r="J113">
         <v>0.86867561111123104</v>
@@ -20573,8 +20813,8 @@
         <f t="shared" si="2"/>
         <v>1120000</v>
       </c>
-      <c r="I114">
-        <v>1.29863299967514</v>
+      <c r="I114" s="2">
+        <v>1.2872142493724801</v>
       </c>
       <c r="J114">
         <v>0.88139755555473798</v>
@@ -20594,8 +20834,8 @@
         <f t="shared" si="2"/>
         <v>1130000</v>
       </c>
-      <c r="I115">
-        <v>1.5245358890129399</v>
+      <c r="I115" s="2">
+        <v>1.5170100615359801</v>
       </c>
       <c r="J115">
         <v>0.87969149999682605</v>
@@ -20615,8 +20855,8 @@
         <f t="shared" si="2"/>
         <v>1140000</v>
       </c>
-      <c r="I116">
-        <v>1.54560600014196</v>
+      <c r="I116" s="2">
+        <v>1.5911656874231901</v>
       </c>
       <c r="J116">
         <v>0.90000622222335802</v>
@@ -20636,8 +20876,8 @@
         <f t="shared" si="2"/>
         <v>1150000</v>
       </c>
-      <c r="I117">
-        <v>1.5359668334325101</v>
+      <c r="I117" s="2">
+        <v>1.50943518662825</v>
       </c>
       <c r="J117">
         <v>0.93082800000330301</v>
@@ -20657,8 +20897,8 @@
         <f t="shared" si="2"/>
         <v>1160000</v>
       </c>
-      <c r="I118">
-        <v>1.59086999980111</v>
+      <c r="I118" s="2">
+        <v>1.5279893744736901</v>
       </c>
       <c r="J118">
         <v>0.91665350000322199</v>
@@ -20678,8 +20918,8 @@
         <f t="shared" si="2"/>
         <v>1170000</v>
       </c>
-      <c r="I119">
-        <v>1.5617407218863499</v>
+      <c r="I119" s="2">
+        <v>1.5115798134356699</v>
       </c>
       <c r="J119">
         <v>0.90630511111359902</v>
@@ -20699,8 +20939,8 @@
         <f t="shared" si="2"/>
         <v>1180000</v>
       </c>
-      <c r="I120">
-        <v>1.59447000051538</v>
+      <c r="I120" s="2">
+        <v>1.52659987518563</v>
       </c>
       <c r="J120">
         <v>0.93462705555430103</v>
@@ -20720,8 +20960,8 @@
         <f t="shared" si="2"/>
         <v>1190000</v>
       </c>
-      <c r="I121">
-        <v>1.3940732775049001</v>
+      <c r="I121" s="2">
+        <v>1.4287933125160599</v>
       </c>
       <c r="J121">
         <v>0.94531611110950398</v>
@@ -20741,8 +20981,8 @@
         <f t="shared" si="2"/>
         <v>1200000</v>
       </c>
-      <c r="I122">
-        <v>1.63363555529051</v>
+      <c r="I122" s="2">
+        <v>1.5650997501797901</v>
       </c>
       <c r="J122">
         <v>0.93792805555696901</v>
@@ -20762,8 +21002,8 @@
         <f t="shared" si="2"/>
         <v>1210000</v>
       </c>
-      <c r="I123">
-        <v>1.40429827777875</v>
+      <c r="I123" s="2">
+        <v>1.42840662552043</v>
       </c>
       <c r="J123">
         <v>0.96557605555507398</v>
@@ -20783,8 +21023,8 @@
         <f t="shared" si="2"/>
         <v>1220000</v>
       </c>
-      <c r="I124">
-        <v>1.64669394410318</v>
+      <c r="I124" s="2">
+        <v>1.58606418827548</v>
       </c>
       <c r="J124">
         <v>0.95689016666922999</v>
@@ -20804,8 +21044,8 @@
         <f t="shared" si="2"/>
         <v>1230000</v>
       </c>
-      <c r="I125">
-        <v>1.3811274444063499</v>
+      <c r="I125" s="2">
+        <v>1.4357484383508501</v>
       </c>
       <c r="J125">
         <v>0.97275549999742195</v>
@@ -20825,8 +21065,8 @@
         <f t="shared" si="2"/>
         <v>1240000</v>
       </c>
-      <c r="I126">
-        <v>1.6596602778881699</v>
+      <c r="I126" s="2">
+        <v>1.6223783139139401</v>
       </c>
       <c r="J126">
         <v>0.98821544443974996</v>
@@ -20846,8 +21086,8 @@
         <f t="shared" si="2"/>
         <v>1250000</v>
       </c>
-      <c r="I127">
-        <v>1.40439088890949</v>
+      <c r="I127" s="2">
+        <v>1.48612949904054</v>
       </c>
       <c r="J127">
         <v>0.97722494444395902</v>
@@ -20867,8 +21107,8 @@
         <f t="shared" si="2"/>
         <v>1260000</v>
       </c>
-      <c r="I128">
-        <v>1.6904112220638301</v>
+      <c r="I128" s="2">
+        <v>1.6645513754337999</v>
       </c>
       <c r="J128">
         <v>0.97645372222015903</v>
@@ -20888,8 +21128,8 @@
         <f t="shared" si="2"/>
         <v>1270000</v>
       </c>
-      <c r="I129">
-        <v>1.4447390553024</v>
+      <c r="I129" s="2">
+        <v>1.5379989375360299</v>
       </c>
       <c r="J129">
         <v>1.00309733333415</v>
@@ -20909,8 +21149,8 @@
         <f t="shared" si="2"/>
         <v>1280000</v>
       </c>
-      <c r="I130">
-        <v>1.7042882223096101</v>
+      <c r="I130" s="2">
+        <v>1.6482201870530799</v>
       </c>
       <c r="J130">
         <v>1.00129316666667</v>
@@ -20930,8 +21170,8 @@
         <f t="shared" si="2"/>
         <v>1290000</v>
       </c>
-      <c r="I131">
-        <v>1.6943401669462499</v>
+      <c r="I131" s="2">
+        <v>1.6616218732669901</v>
       </c>
       <c r="J131">
         <v>1.01342738889151</v>
@@ -20951,8 +21191,8 @@
         <f t="shared" si="2"/>
         <v>1300000</v>
       </c>
-      <c r="I132">
-        <v>1.7375244444443101</v>
+      <c r="I132" s="2">
+        <v>1.7317581879906301</v>
       </c>
       <c r="J132">
         <v>1.0091198333328799</v>
@@ -20972,8 +21212,8 @@
         <f t="shared" ref="H133:H152" si="3">H132+10000</f>
         <v>1310000</v>
       </c>
-      <c r="I133">
-        <v>1.9059758331212699</v>
+      <c r="I133" s="2">
+        <v>1.77275406243279</v>
       </c>
       <c r="J133">
         <v>1.03638038888069</v>
@@ -20993,8 +21233,8 @@
         <f t="shared" si="3"/>
         <v>1320000</v>
       </c>
-      <c r="I134">
-        <v>1.82115272246301</v>
+      <c r="I134" s="2">
+        <v>1.7379474383778799</v>
       </c>
       <c r="J134">
         <v>1.03171655555423</v>
@@ -21014,8 +21254,8 @@
         <f t="shared" si="3"/>
         <v>1330000</v>
       </c>
-      <c r="I135">
-        <v>1.78205744404759</v>
+      <c r="I135" s="2">
+        <v>1.7401566253975</v>
       </c>
       <c r="J135">
         <v>1.1525941111095599</v>
@@ -21035,8 +21275,8 @@
         <f t="shared" si="3"/>
         <v>1340000</v>
       </c>
-      <c r="I136">
-        <v>1.5876966112603701</v>
+      <c r="I136" s="2">
+        <v>1.7272279383614599</v>
       </c>
       <c r="J136">
         <v>1.0467824444446401</v>
@@ -21056,8 +21296,8 @@
         <f t="shared" si="3"/>
         <v>1350000</v>
       </c>
-      <c r="I137">
-        <v>1.79450838847292</v>
+      <c r="I137" s="2">
+        <v>1.7727095629088501</v>
       </c>
       <c r="J137">
         <v>1.0728601111056999</v>
@@ -21077,8 +21317,8 @@
         <f t="shared" si="3"/>
         <v>1360000</v>
       </c>
-      <c r="I138">
-        <v>1.60297011087338</v>
+      <c r="I138" s="2">
+        <v>1.6175416875630599</v>
       </c>
       <c r="J138">
         <v>1.07161711111095</v>
@@ -21098,8 +21338,8 @@
         <f t="shared" si="3"/>
         <v>1370000</v>
       </c>
-      <c r="I139">
-        <v>1.8280026115890999</v>
+      <c r="I139" s="2">
+        <v>1.79891450051218</v>
       </c>
       <c r="J139">
         <v>1.0621756666676201</v>
@@ -21119,8 +21359,8 @@
         <f t="shared" si="3"/>
         <v>1380000</v>
       </c>
-      <c r="I140">
-        <v>1.5774916108283701</v>
+      <c r="I140" s="2">
+        <v>1.6368558132089599</v>
       </c>
       <c r="J140">
         <v>1.08328600000661</v>
@@ -21140,8 +21380,8 @@
         <f t="shared" si="3"/>
         <v>1390000</v>
       </c>
-      <c r="I141">
-        <v>1.8409437218474001</v>
+      <c r="I141" s="2">
+        <v>1.77758537512272</v>
       </c>
       <c r="J141">
         <v>1.0867001666613001</v>
@@ -21161,8 +21401,8 @@
         <f t="shared" si="3"/>
         <v>1400000</v>
       </c>
-      <c r="I142">
-        <v>1.5796587218840901</v>
+      <c r="I142" s="2">
+        <v>1.65796218812465</v>
       </c>
       <c r="J142">
         <v>1.11349483333793</v>
@@ -21182,8 +21422,8 @@
         <f t="shared" si="3"/>
         <v>1410000</v>
       </c>
-      <c r="I143">
-        <v>1.9275448885228801</v>
+      <c r="I143" s="2">
+        <v>1.83635300118476</v>
       </c>
       <c r="J143">
         <v>1.1262473888911899</v>
@@ -21203,8 +21443,8 @@
         <f t="shared" si="3"/>
         <v>1420000</v>
       </c>
-      <c r="I144">
-        <v>1.6350606112844399</v>
+      <c r="I144" s="2">
+        <v>1.66436700103804</v>
       </c>
       <c r="J144">
         <v>1.1230974444463</v>
@@ -21224,8 +21464,8 @@
         <f t="shared" si="3"/>
         <v>1430000</v>
       </c>
-      <c r="I145">
-        <v>1.9188066114568001</v>
+      <c r="I145" s="2">
+        <v>1.87462399946525</v>
       </c>
       <c r="J145">
         <v>1.1184692777799901</v>
@@ -21245,8 +21485,8 @@
         <f t="shared" si="3"/>
         <v>1440000</v>
       </c>
-      <c r="I146">
-        <v>1.66594450010193</v>
+      <c r="I146" s="2">
+        <v>1.71441499982029</v>
       </c>
       <c r="J146">
         <v>1.1477340555575199</v>
@@ -21266,8 +21506,8 @@
         <f t="shared" si="3"/>
         <v>1450000</v>
       </c>
-      <c r="I147">
-        <v>1.95562722264892</v>
+      <c r="I147" s="2">
+        <v>1.9158713137730901</v>
       </c>
       <c r="J147">
         <v>1.1402198333332001</v>
@@ -21287,8 +21527,8 @@
         <f t="shared" si="3"/>
         <v>1460000</v>
       </c>
-      <c r="I148">
-        <v>2.0274828887648</v>
+      <c r="I148" s="2">
+        <v>1.92541893757879</v>
       </c>
       <c r="J148">
         <v>1.1741095555577501</v>
@@ -21308,8 +21548,8 @@
         <f t="shared" si="3"/>
         <v>1470000</v>
       </c>
-      <c r="I149">
-        <v>1.96881344397034</v>
+      <c r="I149" s="2">
+        <v>1.9498613746836699</v>
       </c>
       <c r="J149">
         <v>1.14943383333027</v>
@@ -21329,8 +21569,8 @@
         <f t="shared" si="3"/>
         <v>1480000</v>
       </c>
-      <c r="I150">
-        <v>2.0283092775692499</v>
+      <c r="I150" s="2">
+        <v>1.96982187591493</v>
       </c>
       <c r="J150">
         <v>1.1912089444392899</v>
@@ -21350,8 +21590,8 @@
         <f t="shared" si="3"/>
         <v>1490000</v>
       </c>
-      <c r="I151">
-        <v>2.0176236112084598</v>
+      <c r="I151" s="2">
+        <v>1.99480787478387</v>
       </c>
       <c r="J151">
         <v>1.16541261110978</v>
@@ -21371,8 +21611,8 @@
         <f t="shared" si="3"/>
         <v>1500000</v>
       </c>
-      <c r="I152">
-        <v>2.01672127739422</v>
+      <c r="I152" s="2">
+        <v>1.9824372502043801</v>
       </c>
       <c r="J152">
         <v>1.1772243333349801</v>
@@ -21395,10 +21635,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1762653-C395-8048-983D-A4C069CDBDAD}">
-  <dimension ref="B2:D22"/>
+  <dimension ref="B2:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21416,10 +21656,10 @@
         <v>5000</v>
       </c>
       <c r="C3" s="2">
-        <v>5.8898342152436502E-3</v>
+        <v>1.1196186766028401E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>2.8788667172193499E-2</v>
+        <v>1.6376437153667201E-2</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -21428,22 +21668,22 @@
         <v>10000</v>
       </c>
       <c r="C4" s="2">
-        <v>1.1149223066038501E-2</v>
+        <v>1.6369812190532601E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>3.6995110412438699E-2</v>
+        <v>3.2153374515473801E-2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5">
-        <f t="shared" ref="B5:B22" si="0">B4+5000</f>
+        <f t="shared" ref="B5:B68" si="0">B4+5000</f>
         <v>15000</v>
       </c>
       <c r="C5" s="2">
-        <v>1.64694434238804E-2</v>
+        <v>2.43306229822337E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>5.4171054727501299E-2</v>
+        <v>4.5387312769889797E-2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -21452,10 +21692,10 @@
         <v>20000</v>
       </c>
       <c r="C6" s="2">
-        <v>2.1791723039415099E-2</v>
+        <v>2.67914389260113E-2</v>
       </c>
       <c r="D6" s="2">
-        <v>6.4363222155306002E-2</v>
+        <v>5.7279061991721301E-2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -21464,10 +21704,10 @@
         <v>25000</v>
       </c>
       <c r="C7" s="2">
-        <v>2.71833336187733E-2</v>
+        <v>3.3644374459981898E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>7.9593056192000702E-2</v>
+        <v>7.3285875376313897E-2</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -21476,10 +21716,10 @@
         <v>30000</v>
       </c>
       <c r="C8" s="2">
-        <v>3.1593943635622602E-2</v>
+        <v>3.9811500348150702E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>9.3494000120295406E-2</v>
+        <v>8.7966187391430098E-2</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -21488,10 +21728,10 @@
         <v>35000</v>
       </c>
       <c r="C9" s="2">
-        <v>3.6756777515014001E-2</v>
+        <v>4.5923313125967903E-2</v>
       </c>
       <c r="D9" s="2">
-        <v>0.105413000202841</v>
+        <v>0.105177499353885</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
@@ -21500,10 +21740,10 @@
         <v>40000</v>
       </c>
       <c r="C10" s="2">
-        <v>4.3084222823381403E-2</v>
+        <v>4.6517625451087903E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>0.120231388757626</v>
+        <v>0.117016687523573</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
@@ -21512,10 +21752,10 @@
         <v>45000</v>
       </c>
       <c r="C11" s="2">
-        <v>4.8758389221297299E-2</v>
+        <v>5.2169687580317203E-2</v>
       </c>
       <c r="D11" s="2">
-        <v>0.13526338794165099</v>
+        <v>0.13605537498369799</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
@@ -21524,10 +21764,10 @@
         <v>50000</v>
       </c>
       <c r="C12" s="2">
-        <v>5.5449778007136401E-2</v>
+        <v>5.4724812973290599E-2</v>
       </c>
       <c r="D12" s="2">
-        <v>0.146121667491065</v>
+        <v>0.15006937505677301</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
@@ -21536,10 +21776,10 @@
         <v>55000</v>
       </c>
       <c r="C13" s="2">
-        <v>6.1310333510239901E-2</v>
+        <v>6.3656813465058804E-2</v>
       </c>
       <c r="D13" s="2">
-        <v>0.160922832373115</v>
+        <v>0.16492412565275999</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
@@ -21548,10 +21788,10 @@
         <v>60000</v>
       </c>
       <c r="C14" s="2">
-        <v>6.6149057199557604E-2</v>
+        <v>6.6259999759495203E-2</v>
       </c>
       <c r="D14" s="2">
-        <v>0.17908166680071</v>
+        <v>0.18001306336372999</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
@@ -21560,10 +21800,10 @@
         <v>65000</v>
       </c>
       <c r="C15" s="2">
-        <v>7.9713389691379297E-2</v>
+        <v>7.1303311735391603E-2</v>
       </c>
       <c r="D15" s="2">
-        <v>0.18972583239277199</v>
+        <v>0.19478281354531601</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
@@ -21572,10 +21812,10 @@
         <v>70000</v>
       </c>
       <c r="C16" s="2">
-        <v>7.7554222610261694E-2</v>
+        <v>7.6617248356342302E-2</v>
       </c>
       <c r="D16" s="2">
-        <v>0.20494733295506901</v>
+        <v>0.21016493625938801</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -21584,10 +21824,10 @@
         <v>75000</v>
       </c>
       <c r="C17" s="2">
-        <v>8.2535000311003706E-2</v>
+        <v>8.2056937273591701E-2</v>
       </c>
       <c r="D17" s="2">
-        <v>0.21880650106403499</v>
+        <v>0.22472974937409099</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -21596,10 +21836,10 @@
         <v>80000</v>
       </c>
       <c r="C18" s="2">
-        <v>8.5532000081406698E-2</v>
+        <v>8.7459499947726699E-2</v>
       </c>
       <c r="D18" s="2">
-        <v>0.233332666671938</v>
+        <v>0.23368493607267701</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -21608,10 +21848,10 @@
         <v>85000</v>
       </c>
       <c r="C19" s="2">
-        <v>9.31624443166785E-2</v>
+        <v>9.2769123613834298E-2</v>
       </c>
       <c r="D19" s="2">
-        <v>0.25293794439898598</v>
+        <v>0.25480700051411898</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
@@ -21620,10 +21860,10 @@
         <v>90000</v>
       </c>
       <c r="C20" s="2">
-        <v>9.6126498033603E-2</v>
+        <v>0.101034186314791</v>
       </c>
       <c r="D20" s="2">
-        <v>0.270062777731153</v>
+        <v>0.26838706200942303</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
@@ -21632,10 +21872,10 @@
         <v>95000</v>
       </c>
       <c r="C21" s="2">
-        <v>9.8709277394744999E-2</v>
+        <v>0.10300812497735</v>
       </c>
       <c r="D21" s="2">
-        <v>0.27826966635055</v>
+        <v>0.27895549964159699</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
@@ -21644,11 +21884,371 @@
         <v>100000</v>
       </c>
       <c r="C22" s="2">
-        <v>0.10660494574242101</v>
+        <v>0.10915737459435999</v>
       </c>
       <c r="D22" s="2">
-        <v>0.29146194499399902</v>
-      </c>
+        <v>0.29991768766194499</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>105000</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.108693374320864</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.31161593692377199</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.11760218674317</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.323901999276131</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>115000</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.12547562457621</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.343023498542606</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>120000</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.12737143691629099</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.350884687621146</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>125000</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.13276643725112</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.365783376619219</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>130000</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.141481875441968</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.38357606157660401</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>135000</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.151696812361478</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.41171668889001001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>140000</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.15343825053423599</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.42007593810558302</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>145000</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.153845812194049</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.42149556241929498</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.160094062332063</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.436957125551998</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>155000</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.16467187600210301</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.45125900069251601</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>160000</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.17532849963754399</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.471608936786651</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>165000</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.17773874988779401</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.49377443781122499</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>170000</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.18532768683508</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.48778856405988302</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>175000</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.18569199973717301</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.51640306320041396</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>180000</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.19636581279337401</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.53925943747162797</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>185000</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.201803875621408</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.55409681238233999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>190000</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.20804581325501201</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.57646674942225196</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>195000</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.21241356246173301</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.58828618843108405</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.218072936870157</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.60639425041154005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: return value. force 'use_strict'
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358969AD-444E-8540-B58F-6EA37396B7DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263A3F50-F575-5D4E-96BC-78A2709B31A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="3" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
@@ -13226,124 +13226,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>1.6376437153667201E-2</c:v>
+                  <c:v>6.71600177884101E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2153374515473801E-2</c:v>
+                  <c:v>1.2699937447905501E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5387312769889797E-2</c:v>
+                  <c:v>1.8858748488128099E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7279061991721301E-2</c:v>
+                  <c:v>2.5420187041163399E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3285875376313897E-2</c:v>
+                  <c:v>3.1124314293265301E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.7966187391430098E-2</c:v>
+                  <c:v>3.7090062163770199E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.105177499353885</c:v>
+                  <c:v>4.3489749543368802E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.117016687523573</c:v>
+                  <c:v>4.9556624144315699E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13605537498369799</c:v>
+                  <c:v>5.6966374628245803E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15006937505677301</c:v>
+                  <c:v>6.2213686294853597E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16492412565275999</c:v>
+                  <c:v>6.7312001250684206E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.18001306336372999</c:v>
+                  <c:v>7.4702063575387001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.19478281354531601</c:v>
+                  <c:v>8.0799874849617398E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.21016493625938801</c:v>
+                  <c:v>8.7619563564658096E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.22472974937409099</c:v>
+                  <c:v>9.1546562500297995E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.23368493607267701</c:v>
+                  <c:v>9.7751937806606196E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25480700051411898</c:v>
+                  <c:v>0.105358435772359</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.26838706200942303</c:v>
+                  <c:v>0.111805189400911</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.27895549964159699</c:v>
+                  <c:v>0.115804060362279</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.29991768766194499</c:v>
+                  <c:v>0.122200375422835</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.31161593692377199</c:v>
+                  <c:v>0.12968800123780899</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.323901999276131</c:v>
+                  <c:v>0.13459349703043699</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.343023498542606</c:v>
+                  <c:v>0.139754874631762</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.350884687621146</c:v>
+                  <c:v>0.14541375357657599</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.365783376619219</c:v>
+                  <c:v>0.15673306211829099</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.38357606157660401</c:v>
+                  <c:v>0.15892268717288899</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.41171668889001001</c:v>
+                  <c:v>0.16712943464517499</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.42007593810558302</c:v>
+                  <c:v>0.17443787492811599</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.42149556241929498</c:v>
+                  <c:v>0.17766894027590699</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.436957125551998</c:v>
+                  <c:v>0.18855100031942101</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.45125900069251601</c:v>
+                  <c:v>0.18933543656021301</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.471608936786651</c:v>
+                  <c:v>0.20079049933701701</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.49377443781122499</c:v>
+                  <c:v>0.20100493915379</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.48778856405988302</c:v>
+                  <c:v>0.21251118741929501</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.51640306320041396</c:v>
+                  <c:v>0.22030294034629999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.53925943747162797</c:v>
+                  <c:v>0.21909443847835</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.55409681238233999</c:v>
+                  <c:v>0.22599750105291599</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.57646674942225196</c:v>
+                  <c:v>0.23703274969011501</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.58828618843108405</c:v>
+                  <c:v>0.24115225113928301</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.60639425041154005</c:v>
+                  <c:v>0.243429438211023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21638,7 +21638,7 @@
   <dimension ref="B2:D82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="D3" sqref="D3:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21659,7 +21659,7 @@
         <v>1.1196186766028401E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>1.6376437153667201E-2</v>
+        <v>6.71600177884101E-3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -21671,19 +21671,19 @@
         <v>1.6369812190532601E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>3.2153374515473801E-2</v>
+        <v>1.2699937447905501E-2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5">
-        <f t="shared" ref="B5:B68" si="0">B4+5000</f>
+        <f t="shared" ref="B5:B42" si="0">B4+5000</f>
         <v>15000</v>
       </c>
       <c r="C5" s="2">
         <v>2.43306229822337E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>4.5387312769889797E-2</v>
+        <v>1.8858748488128099E-2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -21695,7 +21695,7 @@
         <v>2.67914389260113E-2</v>
       </c>
       <c r="D6" s="2">
-        <v>5.7279061991721301E-2</v>
+        <v>2.5420187041163399E-2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -21707,7 +21707,7 @@
         <v>3.3644374459981898E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>7.3285875376313897E-2</v>
+        <v>3.1124314293265301E-2</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -21719,7 +21719,7 @@
         <v>3.9811500348150702E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>8.7966187391430098E-2</v>
+        <v>3.7090062163770199E-2</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -21731,7 +21731,7 @@
         <v>4.5923313125967903E-2</v>
       </c>
       <c r="D9" s="2">
-        <v>0.105177499353885</v>
+        <v>4.3489749543368802E-2</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
@@ -21743,7 +21743,7 @@
         <v>4.6517625451087903E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>0.117016687523573</v>
+        <v>4.9556624144315699E-2</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
@@ -21755,7 +21755,7 @@
         <v>5.2169687580317203E-2</v>
       </c>
       <c r="D11" s="2">
-        <v>0.13605537498369799</v>
+        <v>5.6966374628245803E-2</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
@@ -21767,7 +21767,7 @@
         <v>5.4724812973290599E-2</v>
       </c>
       <c r="D12" s="2">
-        <v>0.15006937505677301</v>
+        <v>6.2213686294853597E-2</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
@@ -21779,7 +21779,7 @@
         <v>6.3656813465058804E-2</v>
       </c>
       <c r="D13" s="2">
-        <v>0.16492412565275999</v>
+        <v>6.7312001250684206E-2</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
@@ -21791,7 +21791,7 @@
         <v>6.6259999759495203E-2</v>
       </c>
       <c r="D14" s="2">
-        <v>0.18001306336372999</v>
+        <v>7.4702063575387001E-2</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
@@ -21803,7 +21803,7 @@
         <v>7.1303311735391603E-2</v>
       </c>
       <c r="D15" s="2">
-        <v>0.19478281354531601</v>
+        <v>8.0799874849617398E-2</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
@@ -21815,7 +21815,7 @@
         <v>7.6617248356342302E-2</v>
       </c>
       <c r="D16" s="2">
-        <v>0.21016493625938801</v>
+        <v>8.7619563564658096E-2</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -21827,7 +21827,7 @@
         <v>8.2056937273591701E-2</v>
       </c>
       <c r="D17" s="2">
-        <v>0.22472974937409099</v>
+        <v>9.1546562500297995E-2</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -21839,7 +21839,7 @@
         <v>8.7459499947726699E-2</v>
       </c>
       <c r="D18" s="2">
-        <v>0.23368493607267701</v>
+        <v>9.7751937806606196E-2</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -21851,7 +21851,7 @@
         <v>9.2769123613834298E-2</v>
       </c>
       <c r="D19" s="2">
-        <v>0.25480700051411898</v>
+        <v>0.105358435772359</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
@@ -21863,7 +21863,7 @@
         <v>0.101034186314791</v>
       </c>
       <c r="D20" s="2">
-        <v>0.26838706200942303</v>
+        <v>0.111805189400911</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
@@ -21875,7 +21875,7 @@
         <v>0.10300812497735</v>
       </c>
       <c r="D21" s="2">
-        <v>0.27895549964159699</v>
+        <v>0.115804060362279</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
@@ -21887,7 +21887,7 @@
         <v>0.10915737459435999</v>
       </c>
       <c r="D22" s="2">
-        <v>0.29991768766194499</v>
+        <v>0.122200375422835</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
@@ -21899,7 +21899,7 @@
         <v>0.108693374320864</v>
       </c>
       <c r="D23" s="2">
-        <v>0.31161593692377199</v>
+        <v>0.12968800123780899</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
@@ -21911,7 +21911,7 @@
         <v>0.11760218674317</v>
       </c>
       <c r="D24" s="2">
-        <v>0.323901999276131</v>
+        <v>0.13459349703043699</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
@@ -21923,7 +21923,7 @@
         <v>0.12547562457621</v>
       </c>
       <c r="D25" s="2">
-        <v>0.343023498542606</v>
+        <v>0.139754874631762</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -21935,7 +21935,7 @@
         <v>0.12737143691629099</v>
       </c>
       <c r="D26" s="2">
-        <v>0.350884687621146</v>
+        <v>0.14541375357657599</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -21947,7 +21947,7 @@
         <v>0.13276643725112</v>
       </c>
       <c r="D27" s="2">
-        <v>0.365783376619219</v>
+        <v>0.15673306211829099</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
@@ -21959,7 +21959,7 @@
         <v>0.141481875441968</v>
       </c>
       <c r="D28" s="2">
-        <v>0.38357606157660401</v>
+        <v>0.15892268717288899</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
@@ -21971,7 +21971,7 @@
         <v>0.151696812361478</v>
       </c>
       <c r="D29" s="2">
-        <v>0.41171668889001001</v>
+        <v>0.16712943464517499</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
@@ -21983,7 +21983,7 @@
         <v>0.15343825053423599</v>
       </c>
       <c r="D30" s="2">
-        <v>0.42007593810558302</v>
+        <v>0.17443787492811599</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
@@ -21995,7 +21995,7 @@
         <v>0.153845812194049</v>
       </c>
       <c r="D31" s="2">
-        <v>0.42149556241929498</v>
+        <v>0.17766894027590699</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
@@ -22007,7 +22007,7 @@
         <v>0.160094062332063</v>
       </c>
       <c r="D32" s="2">
-        <v>0.436957125551998</v>
+        <v>0.18855100031942101</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -22019,7 +22019,7 @@
         <v>0.16467187600210301</v>
       </c>
       <c r="D33" s="2">
-        <v>0.45125900069251601</v>
+        <v>0.18933543656021301</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -22031,7 +22031,7 @@
         <v>0.17532849963754399</v>
       </c>
       <c r="D34" s="2">
-        <v>0.471608936786651</v>
+        <v>0.20079049933701701</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -22043,7 +22043,7 @@
         <v>0.17773874988779401</v>
       </c>
       <c r="D35" s="2">
-        <v>0.49377443781122499</v>
+        <v>0.20100493915379</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -22055,7 +22055,7 @@
         <v>0.18532768683508</v>
       </c>
       <c r="D36" s="2">
-        <v>0.48778856405988302</v>
+        <v>0.21251118741929501</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -22067,7 +22067,7 @@
         <v>0.18569199973717301</v>
       </c>
       <c r="D37" s="2">
-        <v>0.51640306320041396</v>
+        <v>0.22030294034629999</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
@@ -22079,7 +22079,7 @@
         <v>0.19636581279337401</v>
       </c>
       <c r="D38" s="2">
-        <v>0.53925943747162797</v>
+        <v>0.21909443847835</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -22091,7 +22091,7 @@
         <v>0.201803875621408</v>
       </c>
       <c r="D39" s="2">
-        <v>0.55409681238233999</v>
+        <v>0.22599750105291599</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -22103,7 +22103,7 @@
         <v>0.20804581325501201</v>
       </c>
       <c r="D40" s="2">
-        <v>0.57646674942225196</v>
+        <v>0.23703274969011501</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -22115,7 +22115,7 @@
         <v>0.21241356246173301</v>
       </c>
       <c r="D41" s="2">
-        <v>0.58828618843108405</v>
+        <v>0.24115225113928301</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -22127,7 +22127,7 @@
         <v>0.218072936870157</v>
       </c>
       <c r="D42" s="2">
-        <v>0.60639425041154005</v>
+        <v>0.243429438211023</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: add timings for own and native array sort methods
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D512575-CC97-5143-AC3B-13A0651DBB4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A4C77-B6C0-944A-B466-C4D987FA3F72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="3" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
   <sheets>
     <sheet name="Shuffle" sheetId="1" r:id="rId1"/>
     <sheet name="Sort" sheetId="2" r:id="rId2"/>
     <sheet name="reverse1" sheetId="3" r:id="rId3"/>
     <sheet name="reverse2" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
+    <sheet name="SortJS" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="22">
   <si>
     <t>Ruby_Shuffle</t>
   </si>
@@ -100,6 +101,9 @@
   </si>
   <si>
     <t>own-v1_reverse_mac</t>
+  </si>
+  <si>
+    <t>nodeJS_sort_mac</t>
   </si>
 </sst>
 </file>
@@ -13352,6 +13356,1021 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3B31-4C49-AB80-0E860BCBBE49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1505303248"/>
+        <c:axId val="1505304928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1505303248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>Array Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1505304928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1505304928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>Run Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1505303248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23043345073257326"/>
+          <c:y val="0.91236797328704222"/>
+          <c:w val="0.49375450074032901"/>
+          <c:h val="7.7227998142020721E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+              <a:t>JavaScript Reverse - Own vs Native Methods</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10053114590374579"/>
+          <c:y val="0.13510164973528074"/>
+          <c:w val="0.80495959466783595"/>
+          <c:h val="0.64069625462183843"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nodeJS_sort_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$C$3:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.12187631428241701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.210019376128911</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.269614748656749</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.438968188129365</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54755968600511495</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66297500114887897</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74745393730700005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.863141561858356</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98799843527376596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1082725636660999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.22623875085264</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.29503356013447</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.42520150076597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.54141630977392</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6086499989032701</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.7248529409989699</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.83331062551587</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9650127505883499</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0445866240188399</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1761859385296698</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2546268152072999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.4150560637935898</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4811960021033799</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.58932687714695</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.69499099720269</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.7773601878434402</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9496711874380699</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.0304327486082898</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.1212183125316999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.4173068134114102</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.4073553765192601</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.5309945605695199</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.6593865593895298</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.7487891847267698</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.87341756001114</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.9474486252292902</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.0971238119527698</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.1871026251465002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.3140698149800301</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.4648304982110796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F261-F743-8DBA-B19B281452DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>own-v1_reverse_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$D$3:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.21598993893712701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44471349753439399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70402950234711104</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93995587807148695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1384934382513101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.40842318814247</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6836156267672699</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9471496874466501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2235239390283801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3766261264681798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6145902471616802</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.93198106158524</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.1862418772652701</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.45903218351304</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.65179431252181</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.9927455633878699</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2502428106963599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5954261245205998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8610913129523396</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.8870891230180797</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.29215562716126</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.4247216852381799</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.6658528121188203</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.9754807492718101</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.2851543137803603</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.35092850029468</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.6577940015122197</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.9292340604588301</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.2016396885737697</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.5434015011414797</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.9579920005053202</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.9206572482362301</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.1251433100551296</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.6307578152045608</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.8071163110434991</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.2034498751163394</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.4497423721477301</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.7012956254184193</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.7889198763296008</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10.0051420619711</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F261-F743-8DBA-B19B281452DC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13840,6 +14859,46 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -16459,6 +17518,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -16880,6 +18455,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>253705</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>35386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>181612</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41310</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14A5B936-9A45-0944-A4FE-CA8931557295}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -17730,7 +19348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF7D883-2303-AA4F-89A1-5EE1247FC595}">
   <dimension ref="B3:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -21637,7 +23255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1762653-C395-8048-983D-A4C069CDBDAD}">
   <dimension ref="B2:E82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="125" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -22297,6 +23915,669 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEBD08F-A22D-004C-B028-B9A5649A9EF3}">
+  <dimension ref="B2:E82"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" zoomScale="141" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.12187631428241701</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.21598993893712701</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <f>B3+5000</f>
+        <v>10000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.210019376128911</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.44471349753439399</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <f t="shared" ref="B5:B42" si="0">B4+5000</f>
+        <v>15000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.269614748656749</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.70402950234711104</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.438968188129365</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.93995587807148695</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.54755968600511495</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.1384934382513101</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.66297500114887897</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.40842318814247</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.74745393730700005</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.6836156267672699</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.863141561858356</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.9471496874466501</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>45000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.98799843527376596</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2.2235239390283801</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.1082725636660999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.3766261264681798</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>55000</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.22623875085264</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.6145902471616802</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.29503356013447</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2.93198106158524</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.42520150076597</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3.1862418772652701</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>70000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.54141630977392</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3.45903218351304</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>75000</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.6086499989032701</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3.65179431252181</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.7248529409989699</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3.9927455633878699</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>85000</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.83331062551587</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4.2502428106963599</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.9650127505883499</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4.5954261245205998</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>95000</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2.0445866240188399</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4.8610913129523396</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2.1761859385296698</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4.8870891230180797</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>105000</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2.2546268152072999</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5.29215562716126</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2.4150560637935898</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5.4247216852381799</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>115000</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2.4811960021033799</v>
+      </c>
+      <c r="D25" s="2">
+        <v>5.6658528121188203</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>120000</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.58932687714695</v>
+      </c>
+      <c r="D26" s="2">
+        <v>5.9754807492718101</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>125000</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2.69499099720269</v>
+      </c>
+      <c r="D27" s="2">
+        <v>6.2851543137803603</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>130000</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.7773601878434402</v>
+      </c>
+      <c r="D28" s="2">
+        <v>6.35092850029468</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>135000</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2.9496711874380699</v>
+      </c>
+      <c r="D29" s="2">
+        <v>6.6577940015122197</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>140000</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3.0304327486082898</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6.9292340604588301</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>145000</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.1212183125316999</v>
+      </c>
+      <c r="D31" s="2">
+        <v>7.2016396885737697</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3.4173068134114102</v>
+      </c>
+      <c r="D32" s="2">
+        <v>7.5434015011414797</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>155000</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3.4073553765192601</v>
+      </c>
+      <c r="D33" s="2">
+        <v>7.9579920005053202</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>160000</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3.5309945605695199</v>
+      </c>
+      <c r="D34" s="2">
+        <v>7.9206572482362301</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>165000</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3.6593865593895298</v>
+      </c>
+      <c r="D35" s="2">
+        <v>8.1251433100551296</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>170000</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3.7487891847267698</v>
+      </c>
+      <c r="D36" s="2">
+        <v>8.6307578152045608</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>175000</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3.87341756001114</v>
+      </c>
+      <c r="D37" s="2">
+        <v>8.8071163110434991</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>180000</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3.9474486252292902</v>
+      </c>
+      <c r="D38" s="2">
+        <v>9.2034498751163394</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>185000</v>
+      </c>
+      <c r="C39" s="2">
+        <v>4.0971238119527698</v>
+      </c>
+      <c r="D39" s="2">
+        <v>9.4497423721477301</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>190000</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4.1871026251465002</v>
+      </c>
+      <c r="D40" s="2">
+        <v>9.7012956254184193</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>195000</v>
+      </c>
+      <c r="C41" s="2">
+        <v>4.3140698149800301</v>
+      </c>
+      <c r="D41" s="2">
+        <v>9.7889198763296008</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4.4648304982110796</v>
+      </c>
+      <c r="D42" s="2">
+        <v>10.0051420619711</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C82" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873D95BF-D23C-644A-9B7B-A0E7AE44E7F3}">
   <dimension ref="A1:R150"/>
   <sheetViews>

</xml_diff>

<commit_message>
docs: add sort plot to readme
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A4C77-B6C0-944A-B466-C4D987FA3F72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC92734-A19F-E247-BA87-A6D12588B5C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="23">
   <si>
     <t>Ruby_Shuffle</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>nodeJS_sort_mac</t>
+  </si>
+  <si>
+    <t>own-quicksort_mac</t>
   </si>
 </sst>
 </file>
@@ -14080,7 +14083,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>own-v1_reverse_mac</c:v>
+                  <c:v>own-quicksort_mac</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -23918,8 +23921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEBD08F-A22D-004C-B028-B9A5649A9EF3}">
   <dimension ref="B2:E82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23929,7 +23932,7 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: correct sort chart title
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC92734-A19F-E247-BA87-A6D12588B5C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEA55ED-0C25-7E4D-B3B8-B3F9D1FF52E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
@@ -13721,7 +13721,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" sz="1800" baseline="0"/>
-              <a:t>JavaScript Reverse - Own vs Native Methods</a:t>
+              <a:t>JavaScript Array Sort - Own vs Native Methods</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -23921,8 +23921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEBD08F-A22D-004C-B028-B9A5649A9EF3}">
   <dimension ref="B2:E82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" zoomScale="141" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: compare npm 'array-sort' module
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,27 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55FCFCE-F5C3-E24D-B51B-8E1FC78542C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61BADE0-B75D-1D47-BB17-116D904EAAF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="5" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
   <sheets>
     <sheet name="reverse1JS" sheetId="3" r:id="rId1"/>
     <sheet name="reverse2JS" sheetId="6" r:id="rId2"/>
     <sheet name="SortJS" sheetId="7" r:id="rId3"/>
     <sheet name="jsNativeSort.csv" sheetId="11" r:id="rId4"/>
-    <sheet name="customQuickSort.csv" sheetId="12" r:id="rId5"/>
-    <sheet name="jsNativeReverse.csv" sheetId="9" r:id="rId6"/>
-    <sheet name="customReverse1.csv" sheetId="10" r:id="rId7"/>
-    <sheet name="Shuffle" sheetId="1" r:id="rId8"/>
-    <sheet name="Sort" sheetId="2" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId10"/>
+    <sheet name="arraySortModule.csv" sheetId="13" r:id="rId5"/>
+    <sheet name="customQuickSort.csv" sheetId="12" r:id="rId6"/>
+    <sheet name="jsNativeReverse.csv" sheetId="9" r:id="rId7"/>
+    <sheet name="customReverse1.csv" sheetId="10" r:id="rId8"/>
+    <sheet name="Shuffle" sheetId="1" r:id="rId9"/>
+    <sheet name="Sort" sheetId="2" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="customQuickSort" localSheetId="4">'customQuickSort.csv'!$A$1:$B$41</definedName>
-    <definedName name="customReverse1" localSheetId="6">'customReverse1.csv'!$A$1:$B$41</definedName>
-    <definedName name="jsNativeReverse" localSheetId="5">jsNativeReverse.csv!$A$1:$B$41</definedName>
-    <definedName name="jsNativeSort" localSheetId="3">jsNativeSort.csv!$A$1:$B$41</definedName>
+    <definedName name="arraySortModule_1" localSheetId="4">arraySortModule.csv!$A$1:$B$41</definedName>
+    <definedName name="customQuickSort_1" localSheetId="5">'customQuickSort.csv'!$A$1:$B$41</definedName>
+    <definedName name="customReverse1" localSheetId="7">'customReverse1.csv'!$A$1:$B$41</definedName>
+    <definedName name="jsNativeReverse" localSheetId="6">jsNativeReverse.csv!$A$1:$B$41</definedName>
+    <definedName name="jsNativeSort_1" localSheetId="3">jsNativeSort.csv!$A$1:$B$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,15 +51,23 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{A0802B38-761C-3F49-8430-7914B7A12B6F}" name="customQuickSort" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customQuickSort.csv" tab="0" comma="1">
+  <connection id="1" xr16:uid="{2669F9B4-4E49-2D4E-89EE-F2687A004E3D}" name="arraySortModule" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/arraySortModule.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{213ABC1B-D4DE-5947-BFE0-24F20803A464}" name="customReverse1" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="2" xr16:uid="{AEEB8A18-EF97-2842-9A1D-B553F804E5ED}" name="customQuickSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customQuickSort.csv" tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" xr16:uid="{213ABC1B-D4DE-5947-BFE0-24F20803A464}" name="customReverse1" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customReverse1.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -65,7 +75,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{9C73BBB2-53E6-3E40-9352-6501CDC56324}" name="jsNativeReverse" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="4" xr16:uid="{9C73BBB2-53E6-3E40-9352-6501CDC56324}" name="jsNativeReverse" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/jsNativeReverse.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -73,8 +83,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{E22469A4-4930-ED40-A969-86359748CB5B}" name="jsNativeSort" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/jsNativeSort.csv" tab="0" comma="1">
+  <connection id="5" xr16:uid="{E76F3574-ECC5-1A46-8FC9-3D2B01FA329A}" name="jsNativeSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/jsNativeSort.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -85,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="26">
   <si>
     <t>Ruby_Shuffle</t>
   </si>
@@ -160,6 +170,9 @@
   </si>
   <si>
     <t>custom_quicksort_mac</t>
+  </si>
+  <si>
+    <t>npm-array-sort_module_mac</t>
   </si>
 </sst>
 </file>
@@ -11771,124 +11784,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.1199979968369</c:v>
+                  <c:v>0.102104179561138</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20063475146889601</c:v>
+                  <c:v>0.18288007006049101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.261109128594398</c:v>
+                  <c:v>0.26449694484472203</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43670225515961603</c:v>
+                  <c:v>0.44295200332999202</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54477911442518201</c:v>
+                  <c:v>0.54009718447923605</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.64931999519467298</c:v>
+                  <c:v>0.64845924451947201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.764678884297609</c:v>
+                  <c:v>0.74817012250423398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86618981137871698</c:v>
+                  <c:v>0.85550755634903897</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.96688568219542503</c:v>
+                  <c:v>0.96094468608498496</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.07931518927216</c:v>
+                  <c:v>1.09424675256013</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1851388737559301</c:v>
+                  <c:v>1.1908555626869199</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2909123152494399</c:v>
+                  <c:v>1.3038464970886701</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.41042612493038</c:v>
+                  <c:v>1.41307693347334</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5051705017685799</c:v>
+                  <c:v>1.5018486306071199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.62348287180066</c:v>
+                  <c:v>1.6071853749453999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.72499694302678</c:v>
+                  <c:v>1.72906507179141</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.8473305590450699</c:v>
+                  <c:v>1.8329610005021</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.9544373229145999</c:v>
+                  <c:v>1.9289744459092599</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0875138118863101</c:v>
+                  <c:v>2.07904719188809</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1874821782112099</c:v>
+                  <c:v>2.1664838194847098</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2938996888697099</c:v>
+                  <c:v>2.27309099584817</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.39359518885612</c:v>
+                  <c:v>2.3939069323241702</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.5150051303207799</c:v>
+                  <c:v>2.4993582032620898</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.6451878175139401</c:v>
+                  <c:v>2.5731642507016601</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7360225617885501</c:v>
+                  <c:v>2.6972448788583199</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.8532086908817198</c:v>
+                  <c:v>2.81661182269454</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.9287724979221799</c:v>
+                  <c:v>2.8874612487852498</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.0759288184344702</c:v>
+                  <c:v>3.0497043095529</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.2083752006292299</c:v>
+                  <c:v>3.1712031289935099</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.3299876227974798</c:v>
+                  <c:v>3.3488848209381099</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.41366206482052</c:v>
+                  <c:v>3.3672025650739599</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.5766049996018401</c:v>
+                  <c:v>3.4657886773347801</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.6716839969158102</c:v>
+                  <c:v>3.6366016864776598</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.7504634335636999</c:v>
+                  <c:v>3.7163554951548501</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.89176605641841</c:v>
+                  <c:v>3.8447315655648699</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.97317218780517</c:v>
+                  <c:v>3.9402064457535699</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.1001307480037203</c:v>
+                  <c:v>4.0289232470095104</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.2197454385459396</c:v>
+                  <c:v>4.1664040572941303</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.3330923765897698</c:v>
+                  <c:v>4.33424437791109</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.4430988095700696</c:v>
+                  <c:v>4.4016934260725904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12074,124 +12087,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.221586633473634</c:v>
+                  <c:v>0.224419370293617</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46199505403637797</c:v>
+                  <c:v>0.48534169048070902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73074813187122301</c:v>
+                  <c:v>0.70382000878453199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96426095068454698</c:v>
+                  <c:v>0.944891057908535</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.18974462896585</c:v>
+                  <c:v>1.1797451823949801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4454148709774</c:v>
+                  <c:v>1.44095319136977</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6753259301185599</c:v>
+                  <c:v>1.6711024269461601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9470981918275301</c:v>
+                  <c:v>1.94047862663865</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.25918631628155</c:v>
+                  <c:v>2.2459357976913399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4528659954666998</c:v>
+                  <c:v>2.4170888029038902</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.73197524622082</c:v>
+                  <c:v>2.6943588666617799</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0792190730571698</c:v>
+                  <c:v>3.0461016856133898</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.24573050439357</c:v>
+                  <c:v>3.2180449254810801</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.5009155534207799</c:v>
+                  <c:v>3.4659693166613499</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.74848449230194</c:v>
+                  <c:v>3.73576307296752</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.0660851895809103</c:v>
+                  <c:v>4.04451049119234</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.3421271219849498</c:v>
+                  <c:v>4.2967164963483802</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.6957743838429398</c:v>
+                  <c:v>4.6426041908562103</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.92130456492304</c:v>
+                  <c:v>4.8864714354276604</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.0852276235818801</c:v>
+                  <c:v>5.1012060046195904</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.4002521187066996</c:v>
+                  <c:v>5.4195951931178499</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.6862730532884598</c:v>
+                  <c:v>5.6902301907539297</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.8699241280555698</c:v>
+                  <c:v>5.8280169405043099</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.2431466840207497</c:v>
+                  <c:v>6.1095849797129604</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.5644953623414004</c:v>
+                  <c:v>6.4049805589020199</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.7295807525515503</c:v>
+                  <c:v>6.5553994998335803</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.9686236269771999</c:v>
+                  <c:v>6.8206861875951201</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.3471433818340302</c:v>
+                  <c:v>7.1622718758881003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.6388465650379596</c:v>
+                  <c:v>7.4341810569167102</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.82126894220709</c:v>
+                  <c:v>7.6537613719701696</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8.2384492494165897</c:v>
+                  <c:v>8.1159730702638608</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.4374661296605993</c:v>
+                  <c:v>8.2242235504090697</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.6387074440717697</c:v>
+                  <c:v>8.4505550004541803</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>9.0221693217754293</c:v>
+                  <c:v>8.88100038096308</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.4006117470562405</c:v>
+                  <c:v>9.1215629912912792</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.7380985505878908</c:v>
+                  <c:v>9.5587001852691102</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.7194906361400992</c:v>
+                  <c:v>9.9733838215470296</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>10.0323565527796</c:v>
+                  <c:v>10.198628738522499</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>10.1223034486174</c:v>
+                  <c:v>10.228653751313599</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10.339805189520099</c:v>
+                  <c:v>10.415818195789999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12200,6 +12213,309 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F261-F743-8DBA-B19B281452DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>npm-array-sort_module_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$E$3:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.112655509263277</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22397561743855399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33785206452012001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52848924696445398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66075130552053396</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78948049619793803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91676411405205704</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.05848781391978</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1791832409799099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3122853115200901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.45074712857604</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.60746737197041</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7320846840739199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9626933634281101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9835802540183001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.11196393892169</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2421319298446099</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4141624271869602</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5126983150839801</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.6471459977328702</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.7636468708515101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.90731174871325</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.04968574270606</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.1576443202793598</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2568029984831801</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.4399440549314</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.5874574966728598</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.69811506569385</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.8563339971005899</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.9518458060920199</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.0669074393808797</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.2685754373669598</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.3928043693304</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.4732246883213502</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.6336993761360601</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.7830456905066896</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.8871905095875201</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.0735971890389902</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.1893460005521703</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.3516968116164199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-76CC-6E4D-AF97-8C75E6ED8E3C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12450,8 +12766,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.23043345073257326"/>
           <c:y val="0.91236797328704222"/>
-          <c:w val="0.49375450074032901"/>
-          <c:h val="7.7227998142020721E-2"/>
+          <c:w val="0.24360180382627272"/>
+          <c:h val="8.7632026712957764E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -18555,19 +18871,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeSort" connectionId="4" xr16:uid="{52324B67-03AC-4C4E-93E8-ED184E25AD42}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeSort_1" refreshOnLoad="1" connectionId="5" xr16:uid="{BBCF7482-98FD-AD4A-9712-69ACE12AE351}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customQuickSort" connectionId="1" xr16:uid="{6B1255BA-882D-024C-8FD5-228D90B15207}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="arraySortModule_1" refreshOnLoad="1" connectionId="1" xr16:uid="{6229A45F-E8FB-5D4E-887A-3055FCD7FF12}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeReverse" refreshOnLoad="1" connectionId="3" xr16:uid="{56AAB590-BEC7-2A4A-83EF-8F6D8BE5A81F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customQuickSort_1" refreshOnLoad="1" connectionId="2" xr16:uid="{73741D56-D32B-A845-966F-3B86276DBDD5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customReverse1" refreshOnLoad="1" connectionId="2" xr16:uid="{F973722E-3E43-7B4F-B612-A86E25BA9E65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeReverse" refreshOnLoad="1" connectionId="4" xr16:uid="{56AAB590-BEC7-2A4A-83EF-8F6D8BE5A81F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customReverse1" refreshOnLoad="1" connectionId="3" xr16:uid="{F973722E-3E43-7B4F-B612-A86E25BA9E65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22573,6 +22893,206 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF7D883-2303-AA4F-89A1-5EE1247FC595}">
+  <dimension ref="B3:C23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>50000</v>
+      </c>
+      <c r="C4">
+        <v>9.3356444444444402E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <f>B4+50000</f>
+        <v>100000</v>
+      </c>
+      <c r="C5">
+        <v>1.9268066666666601E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <f t="shared" ref="B6:B23" si="0">B5+50000</f>
+        <v>150000</v>
+      </c>
+      <c r="C6">
+        <v>3.0407311111111099E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="C7">
+        <v>4.1367466666666602E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>250000</v>
+      </c>
+      <c r="C8">
+        <v>5.2428288888888799E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="C9">
+        <v>6.4871799999999993E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>350000</v>
+      </c>
+      <c r="C10">
+        <v>8.0576155555555501E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>400000</v>
+      </c>
+      <c r="C11">
+        <v>9.1186400000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>450000</v>
+      </c>
+      <c r="C12">
+        <v>0.111102022222222</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>500000</v>
+      </c>
+      <c r="C13">
+        <v>0.112598044444444</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>550000</v>
+      </c>
+      <c r="C14">
+        <v>0.124821622222222</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+      <c r="C15">
+        <v>0.13755588888888801</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>650000</v>
+      </c>
+      <c r="C16">
+        <v>0.152608111111111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>700000</v>
+      </c>
+      <c r="C17">
+        <v>0.15943162222222201</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>750000</v>
+      </c>
+      <c r="C18">
+        <v>0.17657208888888801</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>800000</v>
+      </c>
+      <c r="C19">
+        <v>0.18930424444444399</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>850000</v>
+      </c>
+      <c r="C20">
+        <v>0.19828582222222199</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>900000</v>
+      </c>
+      <c r="C21">
+        <v>0.214428955555555</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>950000</v>
+      </c>
+      <c r="C22">
+        <v>0.22844199999999901</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="C23">
+        <v>0.239597088888888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873D95BF-D23C-644A-9B7B-A0E7AE44E7F3}">
   <dimension ref="A1:R150"/>
   <sheetViews>
@@ -27573,8 +28093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEBD08F-A22D-004C-B028-B9A5649A9EF3}">
   <dimension ref="B2:E82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27586,6 +28106,9 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3">
@@ -27593,13 +28116,16 @@
       </c>
       <c r="C3" s="2">
         <f>jsNativeSort.csv!B2</f>
-        <v>0.1199979968369</v>
+        <v>0.102104179561138</v>
       </c>
       <c r="D3" s="2">
         <f>'customQuickSort.csv'!B2</f>
-        <v>0.221586633473634</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>0.224419370293617</v>
+      </c>
+      <c r="E3" s="2">
+        <f>arraySortModule.csv!B2</f>
+        <v>0.112655509263277</v>
+      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4">
@@ -27608,13 +28134,16 @@
       </c>
       <c r="C4" s="2">
         <f>jsNativeSort.csv!B3</f>
-        <v>0.20063475146889601</v>
+        <v>0.18288007006049101</v>
       </c>
       <c r="D4" s="2">
         <f>'customQuickSort.csv'!B3</f>
-        <v>0.46199505403637797</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>0.48534169048070902</v>
+      </c>
+      <c r="E4" s="2">
+        <f>arraySortModule.csv!B3</f>
+        <v>0.22397561743855399</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5">
@@ -27623,13 +28152,16 @@
       </c>
       <c r="C5" s="2">
         <f>jsNativeSort.csv!B4</f>
-        <v>0.261109128594398</v>
+        <v>0.26449694484472203</v>
       </c>
       <c r="D5" s="2">
         <f>'customQuickSort.csv'!B4</f>
-        <v>0.73074813187122301</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>0.70382000878453199</v>
+      </c>
+      <c r="E5" s="2">
+        <f>arraySortModule.csv!B4</f>
+        <v>0.33785206452012001</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6">
@@ -27638,13 +28170,16 @@
       </c>
       <c r="C6" s="2">
         <f>jsNativeSort.csv!B5</f>
-        <v>0.43670225515961603</v>
+        <v>0.44295200332999202</v>
       </c>
       <c r="D6" s="2">
         <f>'customQuickSort.csv'!B5</f>
-        <v>0.96426095068454698</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>0.944891057908535</v>
+      </c>
+      <c r="E6" s="2">
+        <f>arraySortModule.csv!B5</f>
+        <v>0.52848924696445398</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7">
@@ -27653,13 +28188,16 @@
       </c>
       <c r="C7" s="2">
         <f>jsNativeSort.csv!B6</f>
-        <v>0.54477911442518201</v>
+        <v>0.54009718447923605</v>
       </c>
       <c r="D7" s="2">
         <f>'customQuickSort.csv'!B6</f>
-        <v>1.18974462896585</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>1.1797451823949801</v>
+      </c>
+      <c r="E7" s="2">
+        <f>arraySortModule.csv!B6</f>
+        <v>0.66075130552053396</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8">
@@ -27668,13 +28206,16 @@
       </c>
       <c r="C8" s="2">
         <f>jsNativeSort.csv!B7</f>
-        <v>0.64931999519467298</v>
+        <v>0.64845924451947201</v>
       </c>
       <c r="D8" s="2">
         <f>'customQuickSort.csv'!B7</f>
-        <v>1.4454148709774</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>1.44095319136977</v>
+      </c>
+      <c r="E8" s="2">
+        <f>arraySortModule.csv!B7</f>
+        <v>0.78948049619793803</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9">
@@ -27683,13 +28224,16 @@
       </c>
       <c r="C9" s="2">
         <f>jsNativeSort.csv!B8</f>
-        <v>0.764678884297609</v>
+        <v>0.74817012250423398</v>
       </c>
       <c r="D9" s="2">
         <f>'customQuickSort.csv'!B8</f>
-        <v>1.6753259301185599</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>1.6711024269461601</v>
+      </c>
+      <c r="E9" s="2">
+        <f>arraySortModule.csv!B8</f>
+        <v>0.91676411405205704</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10">
@@ -27698,13 +28242,16 @@
       </c>
       <c r="C10" s="2">
         <f>jsNativeSort.csv!B9</f>
-        <v>0.86618981137871698</v>
+        <v>0.85550755634903897</v>
       </c>
       <c r="D10" s="2">
         <f>'customQuickSort.csv'!B9</f>
-        <v>1.9470981918275301</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>1.94047862663865</v>
+      </c>
+      <c r="E10" s="2">
+        <f>arraySortModule.csv!B9</f>
+        <v>1.05848781391978</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11">
@@ -27713,13 +28260,16 @@
       </c>
       <c r="C11" s="2">
         <f>jsNativeSort.csv!B10</f>
-        <v>0.96688568219542503</v>
+        <v>0.96094468608498496</v>
       </c>
       <c r="D11" s="2">
         <f>'customQuickSort.csv'!B10</f>
-        <v>2.25918631628155</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>2.2459357976913399</v>
+      </c>
+      <c r="E11" s="2">
+        <f>arraySortModule.csv!B10</f>
+        <v>1.1791832409799099</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12">
@@ -27728,13 +28278,16 @@
       </c>
       <c r="C12" s="2">
         <f>jsNativeSort.csv!B11</f>
-        <v>1.07931518927216</v>
+        <v>1.09424675256013</v>
       </c>
       <c r="D12" s="2">
         <f>'customQuickSort.csv'!B11</f>
-        <v>2.4528659954666998</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>2.4170888029038902</v>
+      </c>
+      <c r="E12" s="2">
+        <f>arraySortModule.csv!B11</f>
+        <v>1.3122853115200901</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13">
@@ -27743,13 +28296,16 @@
       </c>
       <c r="C13" s="2">
         <f>jsNativeSort.csv!B12</f>
-        <v>1.1851388737559301</v>
+        <v>1.1908555626869199</v>
       </c>
       <c r="D13" s="2">
         <f>'customQuickSort.csv'!B12</f>
-        <v>2.73197524622082</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>2.6943588666617799</v>
+      </c>
+      <c r="E13" s="2">
+        <f>arraySortModule.csv!B12</f>
+        <v>1.45074712857604</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14">
@@ -27758,13 +28314,16 @@
       </c>
       <c r="C14" s="2">
         <f>jsNativeSort.csv!B13</f>
-        <v>1.2909123152494399</v>
+        <v>1.3038464970886701</v>
       </c>
       <c r="D14" s="2">
         <f>'customQuickSort.csv'!B13</f>
-        <v>3.0792190730571698</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>3.0461016856133898</v>
+      </c>
+      <c r="E14" s="2">
+        <f>arraySortModule.csv!B13</f>
+        <v>1.60746737197041</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15">
@@ -27773,13 +28332,16 @@
       </c>
       <c r="C15" s="2">
         <f>jsNativeSort.csv!B14</f>
-        <v>1.41042612493038</v>
+        <v>1.41307693347334</v>
       </c>
       <c r="D15" s="2">
         <f>'customQuickSort.csv'!B14</f>
-        <v>3.24573050439357</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>3.2180449254810801</v>
+      </c>
+      <c r="E15" s="2">
+        <f>arraySortModule.csv!B14</f>
+        <v>1.7320846840739199</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16">
@@ -27788,13 +28350,16 @@
       </c>
       <c r="C16" s="2">
         <f>jsNativeSort.csv!B15</f>
-        <v>1.5051705017685799</v>
+        <v>1.5018486306071199</v>
       </c>
       <c r="D16" s="2">
         <f>'customQuickSort.csv'!B15</f>
-        <v>3.5009155534207799</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>3.4659693166613499</v>
+      </c>
+      <c r="E16" s="2">
+        <f>arraySortModule.csv!B15</f>
+        <v>1.9626933634281101</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17">
@@ -27803,13 +28368,16 @@
       </c>
       <c r="C17" s="2">
         <f>jsNativeSort.csv!B16</f>
-        <v>1.62348287180066</v>
+        <v>1.6071853749453999</v>
       </c>
       <c r="D17" s="2">
         <f>'customQuickSort.csv'!B16</f>
-        <v>3.74848449230194</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>3.73576307296752</v>
+      </c>
+      <c r="E17" s="2">
+        <f>arraySortModule.csv!B16</f>
+        <v>1.9835802540183001</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18">
@@ -27818,13 +28386,16 @@
       </c>
       <c r="C18" s="2">
         <f>jsNativeSort.csv!B17</f>
-        <v>1.72499694302678</v>
+        <v>1.72906507179141</v>
       </c>
       <c r="D18" s="2">
         <f>'customQuickSort.csv'!B17</f>
-        <v>4.0660851895809103</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>4.04451049119234</v>
+      </c>
+      <c r="E18" s="2">
+        <f>arraySortModule.csv!B17</f>
+        <v>2.11196393892169</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19">
@@ -27833,13 +28404,16 @@
       </c>
       <c r="C19" s="2">
         <f>jsNativeSort.csv!B18</f>
-        <v>1.8473305590450699</v>
+        <v>1.8329610005021</v>
       </c>
       <c r="D19" s="2">
         <f>'customQuickSort.csv'!B18</f>
-        <v>4.3421271219849498</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>4.2967164963483802</v>
+      </c>
+      <c r="E19" s="2">
+        <f>arraySortModule.csv!B18</f>
+        <v>2.2421319298446099</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20">
@@ -27848,13 +28422,16 @@
       </c>
       <c r="C20" s="2">
         <f>jsNativeSort.csv!B19</f>
-        <v>1.9544373229145999</v>
+        <v>1.9289744459092599</v>
       </c>
       <c r="D20" s="2">
         <f>'customQuickSort.csv'!B19</f>
-        <v>4.6957743838429398</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>4.6426041908562103</v>
+      </c>
+      <c r="E20" s="2">
+        <f>arraySortModule.csv!B19</f>
+        <v>2.4141624271869602</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21">
@@ -27863,13 +28440,16 @@
       </c>
       <c r="C21" s="2">
         <f>jsNativeSort.csv!B20</f>
-        <v>2.0875138118863101</v>
+        <v>2.07904719188809</v>
       </c>
       <c r="D21" s="2">
         <f>'customQuickSort.csv'!B20</f>
-        <v>4.92130456492304</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>4.8864714354276604</v>
+      </c>
+      <c r="E21" s="2">
+        <f>arraySortModule.csv!B20</f>
+        <v>2.5126983150839801</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22">
@@ -27878,13 +28458,16 @@
       </c>
       <c r="C22" s="2">
         <f>jsNativeSort.csv!B21</f>
-        <v>2.1874821782112099</v>
+        <v>2.1664838194847098</v>
       </c>
       <c r="D22" s="2">
         <f>'customQuickSort.csv'!B21</f>
-        <v>5.0852276235818801</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>5.1012060046195904</v>
+      </c>
+      <c r="E22" s="2">
+        <f>arraySortModule.csv!B21</f>
+        <v>2.6471459977328702</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23">
@@ -27893,13 +28476,16 @@
       </c>
       <c r="C23" s="2">
         <f>jsNativeSort.csv!B22</f>
-        <v>2.2938996888697099</v>
+        <v>2.27309099584817</v>
       </c>
       <c r="D23" s="2">
         <f>'customQuickSort.csv'!B22</f>
-        <v>5.4002521187066996</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>5.4195951931178499</v>
+      </c>
+      <c r="E23" s="2">
+        <f>arraySortModule.csv!B22</f>
+        <v>2.7636468708515101</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24">
@@ -27908,13 +28494,16 @@
       </c>
       <c r="C24" s="2">
         <f>jsNativeSort.csv!B23</f>
-        <v>2.39359518885612</v>
+        <v>2.3939069323241702</v>
       </c>
       <c r="D24" s="2">
         <f>'customQuickSort.csv'!B23</f>
-        <v>5.6862730532884598</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>5.6902301907539297</v>
+      </c>
+      <c r="E24" s="2">
+        <f>arraySortModule.csv!B23</f>
+        <v>2.90731174871325</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25">
@@ -27923,13 +28512,16 @@
       </c>
       <c r="C25" s="2">
         <f>jsNativeSort.csv!B24</f>
-        <v>2.5150051303207799</v>
+        <v>2.4993582032620898</v>
       </c>
       <c r="D25" s="2">
         <f>'customQuickSort.csv'!B24</f>
-        <v>5.8699241280555698</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>5.8280169405043099</v>
+      </c>
+      <c r="E25" s="2">
+        <f>arraySortModule.csv!B24</f>
+        <v>3.04968574270606</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26">
@@ -27938,13 +28530,16 @@
       </c>
       <c r="C26" s="2">
         <f>jsNativeSort.csv!B25</f>
-        <v>2.6451878175139401</v>
+        <v>2.5731642507016601</v>
       </c>
       <c r="D26" s="2">
         <f>'customQuickSort.csv'!B25</f>
-        <v>6.2431466840207497</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>6.1095849797129604</v>
+      </c>
+      <c r="E26" s="2">
+        <f>arraySortModule.csv!B25</f>
+        <v>3.1576443202793598</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27">
@@ -27953,13 +28548,16 @@
       </c>
       <c r="C27" s="2">
         <f>jsNativeSort.csv!B26</f>
-        <v>2.7360225617885501</v>
+        <v>2.6972448788583199</v>
       </c>
       <c r="D27" s="2">
         <f>'customQuickSort.csv'!B26</f>
-        <v>6.5644953623414004</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>6.4049805589020199</v>
+      </c>
+      <c r="E27" s="2">
+        <f>arraySortModule.csv!B26</f>
+        <v>3.2568029984831801</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28">
@@ -27968,13 +28566,16 @@
       </c>
       <c r="C28" s="2">
         <f>jsNativeSort.csv!B27</f>
-        <v>2.8532086908817198</v>
+        <v>2.81661182269454</v>
       </c>
       <c r="D28" s="2">
         <f>'customQuickSort.csv'!B27</f>
-        <v>6.7295807525515503</v>
-      </c>
-      <c r="E28" s="2"/>
+        <v>6.5553994998335803</v>
+      </c>
+      <c r="E28" s="2">
+        <f>arraySortModule.csv!B27</f>
+        <v>3.4399440549314</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29">
@@ -27983,13 +28584,16 @@
       </c>
       <c r="C29" s="2">
         <f>jsNativeSort.csv!B28</f>
-        <v>2.9287724979221799</v>
+        <v>2.8874612487852498</v>
       </c>
       <c r="D29" s="2">
         <f>'customQuickSort.csv'!B28</f>
-        <v>6.9686236269771999</v>
-      </c>
-      <c r="E29" s="2"/>
+        <v>6.8206861875951201</v>
+      </c>
+      <c r="E29" s="2">
+        <f>arraySortModule.csv!B28</f>
+        <v>3.5874574966728598</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30">
@@ -27998,13 +28602,16 @@
       </c>
       <c r="C30" s="2">
         <f>jsNativeSort.csv!B29</f>
-        <v>3.0759288184344702</v>
+        <v>3.0497043095529</v>
       </c>
       <c r="D30" s="2">
         <f>'customQuickSort.csv'!B29</f>
-        <v>7.3471433818340302</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>7.1622718758881003</v>
+      </c>
+      <c r="E30" s="2">
+        <f>arraySortModule.csv!B29</f>
+        <v>3.69811506569385</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31">
@@ -28013,13 +28620,16 @@
       </c>
       <c r="C31" s="2">
         <f>jsNativeSort.csv!B30</f>
-        <v>3.2083752006292299</v>
+        <v>3.1712031289935099</v>
       </c>
       <c r="D31" s="2">
         <f>'customQuickSort.csv'!B30</f>
-        <v>7.6388465650379596</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>7.4341810569167102</v>
+      </c>
+      <c r="E31" s="2">
+        <f>arraySortModule.csv!B30</f>
+        <v>3.8563339971005899</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32">
@@ -28028,13 +28638,16 @@
       </c>
       <c r="C32" s="2">
         <f>jsNativeSort.csv!B31</f>
-        <v>3.3299876227974798</v>
+        <v>3.3488848209381099</v>
       </c>
       <c r="D32" s="2">
         <f>'customQuickSort.csv'!B31</f>
-        <v>7.82126894220709</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>7.6537613719701696</v>
+      </c>
+      <c r="E32" s="2">
+        <f>arraySortModule.csv!B31</f>
+        <v>3.9518458060920199</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33">
@@ -28043,13 +28656,16 @@
       </c>
       <c r="C33" s="2">
         <f>jsNativeSort.csv!B32</f>
-        <v>3.41366206482052</v>
+        <v>3.3672025650739599</v>
       </c>
       <c r="D33" s="2">
         <f>'customQuickSort.csv'!B32</f>
-        <v>8.2384492494165897</v>
-      </c>
-      <c r="E33" s="2"/>
+        <v>8.1159730702638608</v>
+      </c>
+      <c r="E33" s="2">
+        <f>arraySortModule.csv!B32</f>
+        <v>4.0669074393808797</v>
+      </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34">
@@ -28058,13 +28674,16 @@
       </c>
       <c r="C34" s="2">
         <f>jsNativeSort.csv!B33</f>
-        <v>3.5766049996018401</v>
+        <v>3.4657886773347801</v>
       </c>
       <c r="D34" s="2">
         <f>'customQuickSort.csv'!B33</f>
-        <v>8.4374661296605993</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>8.2242235504090697</v>
+      </c>
+      <c r="E34" s="2">
+        <f>arraySortModule.csv!B33</f>
+        <v>4.2685754373669598</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35">
@@ -28073,13 +28692,16 @@
       </c>
       <c r="C35" s="2">
         <f>jsNativeSort.csv!B34</f>
-        <v>3.6716839969158102</v>
+        <v>3.6366016864776598</v>
       </c>
       <c r="D35" s="2">
         <f>'customQuickSort.csv'!B34</f>
-        <v>8.6387074440717697</v>
-      </c>
-      <c r="E35" s="2"/>
+        <v>8.4505550004541803</v>
+      </c>
+      <c r="E35" s="2">
+        <f>arraySortModule.csv!B34</f>
+        <v>4.3928043693304</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36">
@@ -28088,13 +28710,16 @@
       </c>
       <c r="C36" s="2">
         <f>jsNativeSort.csv!B35</f>
-        <v>3.7504634335636999</v>
+        <v>3.7163554951548501</v>
       </c>
       <c r="D36" s="2">
         <f>'customQuickSort.csv'!B35</f>
-        <v>9.0221693217754293</v>
-      </c>
-      <c r="E36" s="2"/>
+        <v>8.88100038096308</v>
+      </c>
+      <c r="E36" s="2">
+        <f>arraySortModule.csv!B35</f>
+        <v>4.4732246883213502</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37">
@@ -28103,13 +28728,16 @@
       </c>
       <c r="C37" s="2">
         <f>jsNativeSort.csv!B36</f>
-        <v>3.89176605641841</v>
+        <v>3.8447315655648699</v>
       </c>
       <c r="D37" s="2">
         <f>'customQuickSort.csv'!B36</f>
-        <v>9.4006117470562405</v>
-      </c>
-      <c r="E37" s="2"/>
+        <v>9.1215629912912792</v>
+      </c>
+      <c r="E37" s="2">
+        <f>arraySortModule.csv!B36</f>
+        <v>4.6336993761360601</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38">
@@ -28118,13 +28746,16 @@
       </c>
       <c r="C38" s="2">
         <f>jsNativeSort.csv!B37</f>
-        <v>3.97317218780517</v>
+        <v>3.9402064457535699</v>
       </c>
       <c r="D38" s="2">
         <f>'customQuickSort.csv'!B37</f>
-        <v>9.7380985505878908</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>9.5587001852691102</v>
+      </c>
+      <c r="E38" s="2">
+        <f>arraySortModule.csv!B37</f>
+        <v>4.7830456905066896</v>
+      </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39">
@@ -28133,13 +28764,16 @@
       </c>
       <c r="C39" s="2">
         <f>jsNativeSort.csv!B38</f>
-        <v>4.1001307480037203</v>
+        <v>4.0289232470095104</v>
       </c>
       <c r="D39" s="2">
         <f>'customQuickSort.csv'!B38</f>
-        <v>9.7194906361400992</v>
-      </c>
-      <c r="E39" s="2"/>
+        <v>9.9733838215470296</v>
+      </c>
+      <c r="E39" s="2">
+        <f>arraySortModule.csv!B38</f>
+        <v>4.8871905095875201</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40">
@@ -28148,13 +28782,16 @@
       </c>
       <c r="C40" s="2">
         <f>jsNativeSort.csv!B39</f>
-        <v>4.2197454385459396</v>
+        <v>4.1664040572941303</v>
       </c>
       <c r="D40" s="2">
         <f>'customQuickSort.csv'!B39</f>
-        <v>10.0323565527796</v>
-      </c>
-      <c r="E40" s="2"/>
+        <v>10.198628738522499</v>
+      </c>
+      <c r="E40" s="2">
+        <f>arraySortModule.csv!B39</f>
+        <v>5.0735971890389902</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41">
@@ -28163,13 +28800,16 @@
       </c>
       <c r="C41" s="2">
         <f>jsNativeSort.csv!B40</f>
-        <v>4.3330923765897698</v>
+        <v>4.33424437791109</v>
       </c>
       <c r="D41" s="2">
         <f>'customQuickSort.csv'!B40</f>
-        <v>10.1223034486174</v>
-      </c>
-      <c r="E41" s="2"/>
+        <v>10.228653751313599</v>
+      </c>
+      <c r="E41" s="2">
+        <f>arraySortModule.csv!B40</f>
+        <v>5.1893460005521703</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42">
@@ -28178,13 +28818,16 @@
       </c>
       <c r="C42" s="2">
         <f>jsNativeSort.csv!B41</f>
-        <v>4.4430988095700696</v>
+        <v>4.4016934260725904</v>
       </c>
       <c r="D42" s="2">
         <f>'customQuickSort.csv'!B41</f>
-        <v>10.339805189520099</v>
-      </c>
-      <c r="E42" s="2"/>
+        <v>10.415818195789999</v>
+      </c>
+      <c r="E42" s="2">
+        <f>arraySortModule.csv!B41</f>
+        <v>5.3516968116164199</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C43" s="2"/>
@@ -28317,7 +28960,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28339,7 +28982,7 @@
         <v>5000</v>
       </c>
       <c r="B2">
-        <v>0.1199979968369</v>
+        <v>0.102104179561138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -28347,7 +28990,7 @@
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>0.20063475146889601</v>
+        <v>0.18288007006049101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -28355,7 +28998,7 @@
         <v>15000</v>
       </c>
       <c r="B4">
-        <v>0.261109128594398</v>
+        <v>0.26449694484472203</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -28363,7 +29006,7 @@
         <v>20000</v>
       </c>
       <c r="B5">
-        <v>0.43670225515961603</v>
+        <v>0.44295200332999202</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -28371,7 +29014,7 @@
         <v>25000</v>
       </c>
       <c r="B6">
-        <v>0.54477911442518201</v>
+        <v>0.54009718447923605</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -28379,7 +29022,7 @@
         <v>30000</v>
       </c>
       <c r="B7">
-        <v>0.64931999519467298</v>
+        <v>0.64845924451947201</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -28387,7 +29030,7 @@
         <v>35000</v>
       </c>
       <c r="B8">
-        <v>0.764678884297609</v>
+        <v>0.74817012250423398</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -28395,7 +29038,7 @@
         <v>40000</v>
       </c>
       <c r="B9">
-        <v>0.86618981137871698</v>
+        <v>0.85550755634903897</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -28403,7 +29046,7 @@
         <v>45000</v>
       </c>
       <c r="B10">
-        <v>0.96688568219542503</v>
+        <v>0.96094468608498496</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -28411,7 +29054,7 @@
         <v>50000</v>
       </c>
       <c r="B11">
-        <v>1.07931518927216</v>
+        <v>1.09424675256013</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -28419,7 +29062,7 @@
         <v>55000</v>
       </c>
       <c r="B12">
-        <v>1.1851388737559301</v>
+        <v>1.1908555626869199</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -28427,7 +29070,7 @@
         <v>60000</v>
       </c>
       <c r="B13">
-        <v>1.2909123152494399</v>
+        <v>1.3038464970886701</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -28435,7 +29078,7 @@
         <v>65000</v>
       </c>
       <c r="B14">
-        <v>1.41042612493038</v>
+        <v>1.41307693347334</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -28443,7 +29086,7 @@
         <v>70000</v>
       </c>
       <c r="B15">
-        <v>1.5051705017685799</v>
+        <v>1.5018486306071199</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -28451,7 +29094,7 @@
         <v>75000</v>
       </c>
       <c r="B16">
-        <v>1.62348287180066</v>
+        <v>1.6071853749453999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -28459,7 +29102,7 @@
         <v>80000</v>
       </c>
       <c r="B17">
-        <v>1.72499694302678</v>
+        <v>1.72906507179141</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -28467,7 +29110,7 @@
         <v>85000</v>
       </c>
       <c r="B18">
-        <v>1.8473305590450699</v>
+        <v>1.8329610005021</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -28475,7 +29118,7 @@
         <v>90000</v>
       </c>
       <c r="B19">
-        <v>1.9544373229145999</v>
+        <v>1.9289744459092599</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -28483,7 +29126,7 @@
         <v>95000</v>
       </c>
       <c r="B20">
-        <v>2.0875138118863101</v>
+        <v>2.07904719188809</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -28491,7 +29134,7 @@
         <v>100000</v>
       </c>
       <c r="B21">
-        <v>2.1874821782112099</v>
+        <v>2.1664838194847098</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -28499,7 +29142,7 @@
         <v>105000</v>
       </c>
       <c r="B22">
-        <v>2.2938996888697099</v>
+        <v>2.27309099584817</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -28507,7 +29150,7 @@
         <v>110000</v>
       </c>
       <c r="B23">
-        <v>2.39359518885612</v>
+        <v>2.3939069323241702</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -28515,7 +29158,7 @@
         <v>115000</v>
       </c>
       <c r="B24">
-        <v>2.5150051303207799</v>
+        <v>2.4993582032620898</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -28523,7 +29166,7 @@
         <v>120000</v>
       </c>
       <c r="B25">
-        <v>2.6451878175139401</v>
+        <v>2.5731642507016601</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -28531,7 +29174,7 @@
         <v>125000</v>
       </c>
       <c r="B26">
-        <v>2.7360225617885501</v>
+        <v>2.6972448788583199</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -28539,7 +29182,7 @@
         <v>130000</v>
       </c>
       <c r="B27">
-        <v>2.8532086908817198</v>
+        <v>2.81661182269454</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -28547,7 +29190,7 @@
         <v>135000</v>
       </c>
       <c r="B28">
-        <v>2.9287724979221799</v>
+        <v>2.8874612487852498</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -28555,7 +29198,7 @@
         <v>140000</v>
       </c>
       <c r="B29">
-        <v>3.0759288184344702</v>
+        <v>3.0497043095529</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -28563,7 +29206,7 @@
         <v>145000</v>
       </c>
       <c r="B30">
-        <v>3.2083752006292299</v>
+        <v>3.1712031289935099</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -28571,7 +29214,7 @@
         <v>150000</v>
       </c>
       <c r="B31">
-        <v>3.3299876227974798</v>
+        <v>3.3488848209381099</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -28579,7 +29222,7 @@
         <v>155000</v>
       </c>
       <c r="B32">
-        <v>3.41366206482052</v>
+        <v>3.3672025650739599</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -28587,7 +29230,7 @@
         <v>160000</v>
       </c>
       <c r="B33">
-        <v>3.5766049996018401</v>
+        <v>3.4657886773347801</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -28595,7 +29238,7 @@
         <v>165000</v>
       </c>
       <c r="B34">
-        <v>3.6716839969158102</v>
+        <v>3.6366016864776598</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -28603,7 +29246,7 @@
         <v>170000</v>
       </c>
       <c r="B35">
-        <v>3.7504634335636999</v>
+        <v>3.7163554951548501</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -28611,7 +29254,7 @@
         <v>175000</v>
       </c>
       <c r="B36">
-        <v>3.89176605641841</v>
+        <v>3.8447315655648699</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -28619,7 +29262,7 @@
         <v>180000</v>
       </c>
       <c r="B37">
-        <v>3.97317218780517</v>
+        <v>3.9402064457535699</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -28627,7 +29270,7 @@
         <v>185000</v>
       </c>
       <c r="B38">
-        <v>4.1001307480037203</v>
+        <v>4.0289232470095104</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -28635,7 +29278,7 @@
         <v>190000</v>
       </c>
       <c r="B39">
-        <v>4.2197454385459396</v>
+        <v>4.1664040572941303</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -28643,7 +29286,7 @@
         <v>195000</v>
       </c>
       <c r="B40">
-        <v>4.3330923765897698</v>
+        <v>4.33424437791109</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -28651,7 +29294,7 @@
         <v>200000</v>
       </c>
       <c r="B41">
-        <v>4.4430988095700696</v>
+        <v>4.4016934260725904</v>
       </c>
     </row>
   </sheetData>
@@ -28660,11 +29303,356 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEBB81E-0061-5F4B-A5E8-AFD40BDCA62B}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5000</v>
+      </c>
+      <c r="B2">
+        <v>0.112655509263277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>0.22397561743855399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4">
+        <v>0.33785206452012001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20000</v>
+      </c>
+      <c r="B5">
+        <v>0.52848924696445398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>25000</v>
+      </c>
+      <c r="B6">
+        <v>0.66075130552053396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>30000</v>
+      </c>
+      <c r="B7">
+        <v>0.78948049619793803</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>35000</v>
+      </c>
+      <c r="B8">
+        <v>0.91676411405205704</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>40000</v>
+      </c>
+      <c r="B9">
+        <v>1.05848781391978</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>45000</v>
+      </c>
+      <c r="B10">
+        <v>1.1791832409799099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>50000</v>
+      </c>
+      <c r="B11">
+        <v>1.3122853115200901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>55000</v>
+      </c>
+      <c r="B12">
+        <v>1.45074712857604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>60000</v>
+      </c>
+      <c r="B13">
+        <v>1.60746737197041</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>65000</v>
+      </c>
+      <c r="B14">
+        <v>1.7320846840739199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>70000</v>
+      </c>
+      <c r="B15">
+        <v>1.9626933634281101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>75000</v>
+      </c>
+      <c r="B16">
+        <v>1.9835802540183001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80000</v>
+      </c>
+      <c r="B17">
+        <v>2.11196393892169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>85000</v>
+      </c>
+      <c r="B18">
+        <v>2.2421319298446099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>90000</v>
+      </c>
+      <c r="B19">
+        <v>2.4141624271869602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>95000</v>
+      </c>
+      <c r="B20">
+        <v>2.5126983150839801</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>100000</v>
+      </c>
+      <c r="B21">
+        <v>2.6471459977328702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>105000</v>
+      </c>
+      <c r="B22">
+        <v>2.7636468708515101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>110000</v>
+      </c>
+      <c r="B23">
+        <v>2.90731174871325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>115000</v>
+      </c>
+      <c r="B24">
+        <v>3.04968574270606</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>120000</v>
+      </c>
+      <c r="B25">
+        <v>3.1576443202793598</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>125000</v>
+      </c>
+      <c r="B26">
+        <v>3.2568029984831801</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>130000</v>
+      </c>
+      <c r="B27">
+        <v>3.4399440549314</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>135000</v>
+      </c>
+      <c r="B28">
+        <v>3.5874574966728598</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>140000</v>
+      </c>
+      <c r="B29">
+        <v>3.69811506569385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>145000</v>
+      </c>
+      <c r="B30">
+        <v>3.8563339971005899</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>150000</v>
+      </c>
+      <c r="B31">
+        <v>3.9518458060920199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>155000</v>
+      </c>
+      <c r="B32">
+        <v>4.0669074393808797</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>160000</v>
+      </c>
+      <c r="B33">
+        <v>4.2685754373669598</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>165000</v>
+      </c>
+      <c r="B34">
+        <v>4.3928043693304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>170000</v>
+      </c>
+      <c r="B35">
+        <v>4.4732246883213502</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>175000</v>
+      </c>
+      <c r="B36">
+        <v>4.6336993761360601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>180000</v>
+      </c>
+      <c r="B37">
+        <v>4.7830456905066896</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>185000</v>
+      </c>
+      <c r="B38">
+        <v>4.8871905095875201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>190000</v>
+      </c>
+      <c r="B39">
+        <v>5.0735971890389902</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>195000</v>
+      </c>
+      <c r="B40">
+        <v>5.1893460005521703</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>200000</v>
+      </c>
+      <c r="B41">
+        <v>5.3516968116164199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3A630D-BCBD-EA48-90F0-EE0016EF0A47}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28686,7 +29674,7 @@
         <v>5000</v>
       </c>
       <c r="B2">
-        <v>0.221586633473634</v>
+        <v>0.224419370293617</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -28694,7 +29682,7 @@
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>0.46199505403637797</v>
+        <v>0.48534169048070902</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -28702,7 +29690,7 @@
         <v>15000</v>
       </c>
       <c r="B4">
-        <v>0.73074813187122301</v>
+        <v>0.70382000878453199</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -28710,7 +29698,7 @@
         <v>20000</v>
       </c>
       <c r="B5">
-        <v>0.96426095068454698</v>
+        <v>0.944891057908535</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -28718,7 +29706,7 @@
         <v>25000</v>
       </c>
       <c r="B6">
-        <v>1.18974462896585</v>
+        <v>1.1797451823949801</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -28726,7 +29714,7 @@
         <v>30000</v>
       </c>
       <c r="B7">
-        <v>1.4454148709774</v>
+        <v>1.44095319136977</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -28734,7 +29722,7 @@
         <v>35000</v>
       </c>
       <c r="B8">
-        <v>1.6753259301185599</v>
+        <v>1.6711024269461601</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -28742,7 +29730,7 @@
         <v>40000</v>
       </c>
       <c r="B9">
-        <v>1.9470981918275301</v>
+        <v>1.94047862663865</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -28750,7 +29738,7 @@
         <v>45000</v>
       </c>
       <c r="B10">
-        <v>2.25918631628155</v>
+        <v>2.2459357976913399</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -28758,7 +29746,7 @@
         <v>50000</v>
       </c>
       <c r="B11">
-        <v>2.4528659954666998</v>
+        <v>2.4170888029038902</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -28766,7 +29754,7 @@
         <v>55000</v>
       </c>
       <c r="B12">
-        <v>2.73197524622082</v>
+        <v>2.6943588666617799</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -28774,7 +29762,7 @@
         <v>60000</v>
       </c>
       <c r="B13">
-        <v>3.0792190730571698</v>
+        <v>3.0461016856133898</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -28782,7 +29770,7 @@
         <v>65000</v>
       </c>
       <c r="B14">
-        <v>3.24573050439357</v>
+        <v>3.2180449254810801</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -28790,7 +29778,7 @@
         <v>70000</v>
       </c>
       <c r="B15">
-        <v>3.5009155534207799</v>
+        <v>3.4659693166613499</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -28798,7 +29786,7 @@
         <v>75000</v>
       </c>
       <c r="B16">
-        <v>3.74848449230194</v>
+        <v>3.73576307296752</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -28806,7 +29794,7 @@
         <v>80000</v>
       </c>
       <c r="B17">
-        <v>4.0660851895809103</v>
+        <v>4.04451049119234</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -28814,7 +29802,7 @@
         <v>85000</v>
       </c>
       <c r="B18">
-        <v>4.3421271219849498</v>
+        <v>4.2967164963483802</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -28822,7 +29810,7 @@
         <v>90000</v>
       </c>
       <c r="B19">
-        <v>4.6957743838429398</v>
+        <v>4.6426041908562103</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -28830,7 +29818,7 @@
         <v>95000</v>
       </c>
       <c r="B20">
-        <v>4.92130456492304</v>
+        <v>4.8864714354276604</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -28838,7 +29826,7 @@
         <v>100000</v>
       </c>
       <c r="B21">
-        <v>5.0852276235818801</v>
+        <v>5.1012060046195904</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -28846,7 +29834,7 @@
         <v>105000</v>
       </c>
       <c r="B22">
-        <v>5.4002521187066996</v>
+        <v>5.4195951931178499</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -28854,7 +29842,7 @@
         <v>110000</v>
       </c>
       <c r="B23">
-        <v>5.6862730532884598</v>
+        <v>5.6902301907539297</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -28862,7 +29850,7 @@
         <v>115000</v>
       </c>
       <c r="B24">
-        <v>5.8699241280555698</v>
+        <v>5.8280169405043099</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -28870,7 +29858,7 @@
         <v>120000</v>
       </c>
       <c r="B25">
-        <v>6.2431466840207497</v>
+        <v>6.1095849797129604</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -28878,7 +29866,7 @@
         <v>125000</v>
       </c>
       <c r="B26">
-        <v>6.5644953623414004</v>
+        <v>6.4049805589020199</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -28886,7 +29874,7 @@
         <v>130000</v>
       </c>
       <c r="B27">
-        <v>6.7295807525515503</v>
+        <v>6.5553994998335803</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -28894,7 +29882,7 @@
         <v>135000</v>
       </c>
       <c r="B28">
-        <v>6.9686236269771999</v>
+        <v>6.8206861875951201</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -28902,7 +29890,7 @@
         <v>140000</v>
       </c>
       <c r="B29">
-        <v>7.3471433818340302</v>
+        <v>7.1622718758881003</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -28910,7 +29898,7 @@
         <v>145000</v>
       </c>
       <c r="B30">
-        <v>7.6388465650379596</v>
+        <v>7.4341810569167102</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -28918,7 +29906,7 @@
         <v>150000</v>
       </c>
       <c r="B31">
-        <v>7.82126894220709</v>
+        <v>7.6537613719701696</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -28926,7 +29914,7 @@
         <v>155000</v>
       </c>
       <c r="B32">
-        <v>8.2384492494165897</v>
+        <v>8.1159730702638608</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -28934,7 +29922,7 @@
         <v>160000</v>
       </c>
       <c r="B33">
-        <v>8.4374661296605993</v>
+        <v>8.2242235504090697</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -28942,7 +29930,7 @@
         <v>165000</v>
       </c>
       <c r="B34">
-        <v>8.6387074440717697</v>
+        <v>8.4505550004541803</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -28950,7 +29938,7 @@
         <v>170000</v>
       </c>
       <c r="B35">
-        <v>9.0221693217754293</v>
+        <v>8.88100038096308</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -28958,7 +29946,7 @@
         <v>175000</v>
       </c>
       <c r="B36">
-        <v>9.4006117470562405</v>
+        <v>9.1215629912912792</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -28966,7 +29954,7 @@
         <v>180000</v>
       </c>
       <c r="B37">
-        <v>9.7380985505878908</v>
+        <v>9.5587001852691102</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -28974,7 +29962,7 @@
         <v>185000</v>
       </c>
       <c r="B38">
-        <v>9.7194906361400992</v>
+        <v>9.9733838215470296</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -28982,7 +29970,7 @@
         <v>190000</v>
       </c>
       <c r="B39">
-        <v>10.0323565527796</v>
+        <v>10.198628738522499</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -28990,7 +29978,7 @@
         <v>195000</v>
       </c>
       <c r="B40">
-        <v>10.1223034486174</v>
+        <v>10.228653751313599</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -28998,7 +29986,7 @@
         <v>200000</v>
       </c>
       <c r="B41">
-        <v>10.339805189520099</v>
+        <v>10.415818195789999</v>
       </c>
     </row>
   </sheetData>
@@ -29006,7 +29994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FEB25-A74F-5A45-B563-EED0518B676C}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -29353,7 +30341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C32E7-BB37-4B49-90BE-558A0F4C3E2F}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -29700,7 +30688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EC2C70-D28D-5649-B065-1682BAD693A3}">
   <dimension ref="B2:N22"/>
   <sheetViews>
@@ -30249,204 +31237,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF7D883-2303-AA4F-89A1-5EE1247FC595}">
-  <dimension ref="B3:C23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>50000</v>
-      </c>
-      <c r="C4">
-        <v>9.3356444444444402E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <f>B4+50000</f>
-        <v>100000</v>
-      </c>
-      <c r="C5">
-        <v>1.9268066666666601E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <f t="shared" ref="B6:B23" si="0">B5+50000</f>
-        <v>150000</v>
-      </c>
-      <c r="C6">
-        <v>3.0407311111111099E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>200000</v>
-      </c>
-      <c r="C7">
-        <v>4.1367466666666602E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>250000</v>
-      </c>
-      <c r="C8">
-        <v>5.2428288888888799E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-      <c r="C9">
-        <v>6.4871799999999993E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>350000</v>
-      </c>
-      <c r="C10">
-        <v>8.0576155555555501E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>400000</v>
-      </c>
-      <c r="C11">
-        <v>9.1186400000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>450000</v>
-      </c>
-      <c r="C12">
-        <v>0.111102022222222</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>500000</v>
-      </c>
-      <c r="C13">
-        <v>0.112598044444444</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>550000</v>
-      </c>
-      <c r="C14">
-        <v>0.124821622222222</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>600000</v>
-      </c>
-      <c r="C15">
-        <v>0.13755588888888801</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>650000</v>
-      </c>
-      <c r="C16">
-        <v>0.152608111111111</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>700000</v>
-      </c>
-      <c r="C17">
-        <v>0.15943162222222201</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>750000</v>
-      </c>
-      <c r="C18">
-        <v>0.17657208888888801</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>800000</v>
-      </c>
-      <c r="C19">
-        <v>0.18930424444444399</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>850000</v>
-      </c>
-      <c r="C20">
-        <v>0.19828582222222199</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>900000</v>
-      </c>
-      <c r="C21">
-        <v>0.214428955555555</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>950000</v>
-      </c>
-      <c r="C22">
-        <v>0.22844199999999901</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-      <c r="C23">
-        <v>0.239597088888888</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: compare selection sort
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61BADE0-B75D-1D47-BB17-116D904EAAF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9346E2-7EDD-5A4E-A84F-AEDD830BB72A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="5" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
   <sheets>
     <sheet name="reverse1JS" sheetId="3" r:id="rId1"/>
     <sheet name="reverse2JS" sheetId="6" r:id="rId2"/>
     <sheet name="SortJS" sheetId="7" r:id="rId3"/>
-    <sheet name="jsNativeSort.csv" sheetId="11" r:id="rId4"/>
-    <sheet name="arraySortModule.csv" sheetId="13" r:id="rId5"/>
-    <sheet name="customQuickSort.csv" sheetId="12" r:id="rId6"/>
-    <sheet name="jsNativeReverse.csv" sheetId="9" r:id="rId7"/>
-    <sheet name="customReverse1.csv" sheetId="10" r:id="rId8"/>
-    <sheet name="Shuffle" sheetId="1" r:id="rId9"/>
-    <sheet name="Sort" sheetId="2" r:id="rId10"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId11"/>
+    <sheet name="customSelectionSort.csv" sheetId="14" r:id="rId4"/>
+    <sheet name="jsNativeSort.csv" sheetId="11" r:id="rId5"/>
+    <sheet name="arraySortModule.csv" sheetId="13" r:id="rId6"/>
+    <sheet name="customQuickSort.csv" sheetId="12" r:id="rId7"/>
+    <sheet name="jsNativeReverse.csv" sheetId="9" r:id="rId8"/>
+    <sheet name="customReverse1.csv" sheetId="10" r:id="rId9"/>
+    <sheet name="Shuffle" sheetId="1" r:id="rId10"/>
+    <sheet name="Sort" sheetId="2" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="arraySortModule_1" localSheetId="4">arraySortModule.csv!$A$1:$B$41</definedName>
-    <definedName name="customQuickSort_1" localSheetId="5">'customQuickSort.csv'!$A$1:$B$41</definedName>
-    <definedName name="customReverse1" localSheetId="7">'customReverse1.csv'!$A$1:$B$41</definedName>
-    <definedName name="jsNativeReverse" localSheetId="6">jsNativeReverse.csv!$A$1:$B$41</definedName>
-    <definedName name="jsNativeSort_1" localSheetId="3">jsNativeSort.csv!$A$1:$B$41</definedName>
+    <definedName name="arraySortModule_1" localSheetId="5">arraySortModule.csv!$A$1:$B$41</definedName>
+    <definedName name="customQuickSort_1" localSheetId="6">'customQuickSort.csv'!$A$1:$B$41</definedName>
+    <definedName name="customReverse1" localSheetId="8">'customReverse1.csv'!$A$1:$B$41</definedName>
+    <definedName name="customSelectionSort" localSheetId="3">'customSelectionSort.csv'!$A$1:$B$7</definedName>
+    <definedName name="jsNativeReverse" localSheetId="7">jsNativeReverse.csv!$A$1:$B$41</definedName>
+    <definedName name="jsNativeSort_1" localSheetId="4">jsNativeSort.csv!$A$1:$B$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -75,7 +77,15 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{9C73BBB2-53E6-3E40-9352-6501CDC56324}" name="jsNativeReverse" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="4" xr16:uid="{DA5891EA-0CE4-7D4F-8FB6-44DEEBEBE699}" name="customSelectionSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customSelectionSort.csv" tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" xr16:uid="{9C73BBB2-53E6-3E40-9352-6501CDC56324}" name="jsNativeReverse" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/jsNativeReverse.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -83,7 +93,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{E76F3574-ECC5-1A46-8FC9-3D2B01FA329A}" name="jsNativeSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="6" xr16:uid="{E76F3574-ECC5-1A46-8FC9-3D2B01FA329A}" name="jsNativeSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/jsNativeSort.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -95,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="27">
   <si>
     <t>Ruby_Shuffle</t>
   </si>
@@ -173,6 +183,9 @@
   </si>
   <si>
     <t>npm-array-sort_module_mac</t>
+  </si>
+  <si>
+    <t>selection_sort_mac</t>
   </si>
 </sst>
 </file>
@@ -11560,7 +11573,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB" sz="1800" baseline="0"/>
-              <a:t>JavaScript Array Sort - Own vs Native Methods</a:t>
+              <a:t>JavaScript Array Sort - Custom vs npm vs Native Methods</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -12764,9 +12777,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23043345073257326"/>
-          <c:y val="0.91236797328704222"/>
-          <c:w val="0.24360180382627272"/>
+          <c:x val="0.23884872557337"/>
+          <c:y val="0.89676193043063668"/>
+          <c:w val="0.53392842431132326"/>
           <c:h val="8.7632026712957764E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -12844,6 +12857,1525 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" baseline="0"/>
+              <a:t>JavaScript Array Sort - Custom vs npm vs Native Methods</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10053114590374579"/>
+          <c:y val="0.13510164973528074"/>
+          <c:w val="0.80495959466783595"/>
+          <c:h val="0.64069625462183843"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nodeJS_native_sort_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$C$3:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.102104179561138</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18288007006049101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26449694484472203</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44295200332999202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54009718447923605</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.64845924451947201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74817012250423398</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85550755634903897</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96094468608498496</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.09424675256013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1908555626869199</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3038464970886701</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.41307693347334</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5018486306071199</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6071853749453999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.72906507179141</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8329610005021</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9289744459092599</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.07904719188809</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1664838194847098</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.27309099584817</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.3939069323241702</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4993582032620898</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5731642507016601</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.6972448788583199</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.81661182269454</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.8874612487852498</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.0497043095529</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.1712031289935099</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.3488848209381099</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.3672025650739599</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.4657886773347801</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.6366016864776598</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.7163554951548501</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.8447315655648699</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.9402064457535699</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.0289232470095104</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.1664040572941303</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.33424437791109</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.4016934260725904</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F261-F743-8DBA-B19B281452DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>custom_quicksort_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$D$3:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.224419370293617</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48534169048070902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70382000878453199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.944891057908535</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1797451823949801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.44095319136977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6711024269461601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.94047862663865</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2459357976913399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4170888029038902</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6943588666617799</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0461016856133898</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2180449254810801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.4659693166613499</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.73576307296752</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.04451049119234</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2967164963483802</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.6426041908562103</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.8864714354276604</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.1012060046195904</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.4195951931178499</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.6902301907539297</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.8280169405043099</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.1095849797129604</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.4049805589020199</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.5553994998335803</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.8206861875951201</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.1622718758881003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.4341810569167102</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.6537613719701696</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.1159730702638608</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.2242235504090697</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.4505550004541803</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.88100038096308</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.1215629912912792</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.5587001852691102</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.9733838215470296</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10.198628738522499</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10.228653751313599</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10.415818195789999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F261-F743-8DBA-B19B281452DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>npm-array-sort_module_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$E$3:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.112655509263277</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22397561743855399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33785206452012001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52848924696445398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66075130552053396</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78948049619793803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91676411405205704</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.05848781391978</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1791832409799099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3122853115200901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.45074712857604</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.60746737197041</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7320846840739199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9626933634281101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9835802540183001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.11196393892169</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2421319298446099</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4141624271869602</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5126983150839801</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.6471459977328702</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.7636468708515101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.90731174871325</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.04968574270606</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.1576443202793598</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2568029984831801</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.4399440549314</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.5874574966728598</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.69811506569385</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.8563339971005899</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.9518458060920199</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.0669074393808797</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.2685754373669598</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.3928043693304</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.4732246883213502</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.6336993761360601</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.7830456905066896</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.8871905095875201</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.0735971890389902</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.1893460005521703</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.3516968116164199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-76CC-6E4D-AF97-8C75E6ED8E3C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>selection_sort_mac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$F$3:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>10.3245585672557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.293232690542901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.720794811844797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>164.42270037531799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>257.29061499610498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>370.75442412122999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-46C7-3341-BAC7-F5860DCD5FEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1505303248"/>
+        <c:axId val="1505304928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1505303248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>Array Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1505304928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1505304928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>Run Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1505303248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23884872557337"/>
+          <c:y val="0.89676193043063668"/>
+          <c:w val="0.45338561822674261"/>
+          <c:h val="0.10323806956936334"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -14499,7 +16031,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -15271,6 +16803,46 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -18406,6 +19978,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -18749,16 +20837,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>253705</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>236771</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>35386</xdr:rowOff>
+      <xdr:rowOff>187786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>181612</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>164679</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>41310</xdr:rowOff>
+      <xdr:rowOff>193710</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18780,6 +20868,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219836</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>52319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>778933</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>58243</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2D747A1-9C67-7B46-9690-4DFB105ED586}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -18871,22 +20997,26 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeSort_1" refreshOnLoad="1" connectionId="5" xr16:uid="{BBCF7482-98FD-AD4A-9712-69ACE12AE351}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customSelectionSort" refreshOnLoad="1" connectionId="4" xr16:uid="{D622F393-634F-4D4C-82D5-2836861CD48B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeSort_1" refreshOnLoad="1" connectionId="6" xr16:uid="{BBCF7482-98FD-AD4A-9712-69ACE12AE351}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="arraySortModule_1" refreshOnLoad="1" connectionId="1" xr16:uid="{6229A45F-E8FB-5D4E-887A-3055FCD7FF12}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customQuickSort_1" refreshOnLoad="1" connectionId="2" xr16:uid="{73741D56-D32B-A845-966F-3B86276DBDD5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeReverse" refreshOnLoad="1" connectionId="4" xr16:uid="{56AAB590-BEC7-2A4A-83EF-8F6D8BE5A81F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeReverse" refreshOnLoad="1" connectionId="5" xr16:uid="{56AAB590-BEC7-2A4A-83EF-8F6D8BE5A81F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customReverse1" refreshOnLoad="1" connectionId="3" xr16:uid="{F973722E-3E43-7B4F-B612-A86E25BA9E65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -22893,6 +25023,557 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EC2C70-D28D-5649-B065-1682BAD693A3}">
+  <dimension ref="B2:N22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="83" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>50000</v>
+      </c>
+      <c r="C3">
+        <v>1.15404444444444</v>
+      </c>
+      <c r="D3">
+        <v>1.40228997777777</v>
+      </c>
+      <c r="E3">
+        <v>7.9028888888888895</v>
+      </c>
+      <c r="F3">
+        <v>12.3438432666666</v>
+      </c>
+      <c r="G3">
+        <v>7.8472962962962898</v>
+      </c>
+      <c r="H3">
+        <v>12.094564288888801</v>
+      </c>
+      <c r="I3">
+        <v>3.5976296296296297</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <f>B3+50000</f>
+        <v>100000</v>
+      </c>
+      <c r="C4">
+        <v>2.3280444444444401</v>
+      </c>
+      <c r="D4">
+        <v>2.8260463777777702</v>
+      </c>
+      <c r="E4">
+        <v>16.267111111111099</v>
+      </c>
+      <c r="F4">
+        <v>24.954859555555501</v>
+      </c>
+      <c r="G4">
+        <v>16.073037037037</v>
+      </c>
+      <c r="H4">
+        <v>24.201441644444401</v>
+      </c>
+      <c r="I4">
+        <v>16.4758148148148</v>
+      </c>
+      <c r="N4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <f t="shared" ref="B5:B22" si="0">B4+50000</f>
+        <v>150000</v>
+      </c>
+      <c r="C5">
+        <v>3.6934222222222197</v>
+      </c>
+      <c r="D5">
+        <v>4.3713101111111099</v>
+      </c>
+      <c r="E5">
+        <v>24.1606296296296</v>
+      </c>
+      <c r="F5">
+        <v>38.015178755555496</v>
+      </c>
+      <c r="G5">
+        <v>23.861370370370299</v>
+      </c>
+      <c r="H5">
+        <v>36.627184399999997</v>
+      </c>
+      <c r="I5">
+        <v>40.443629629629505</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>200000</v>
+      </c>
+      <c r="C6">
+        <v>4.8577555555555501</v>
+      </c>
+      <c r="D6">
+        <v>5.8404372888888894</v>
+      </c>
+      <c r="E6">
+        <v>32.296259259259202</v>
+      </c>
+      <c r="F6">
+        <v>51.107483377777697</v>
+      </c>
+      <c r="G6">
+        <v>31.255481481481397</v>
+      </c>
+      <c r="H6">
+        <v>49.392725311111001</v>
+      </c>
+      <c r="I6">
+        <v>73.447925925925901</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>250000</v>
+      </c>
+      <c r="C7">
+        <v>6.0637777777777702</v>
+      </c>
+      <c r="D7">
+        <v>6.9460814444444399</v>
+      </c>
+      <c r="E7">
+        <v>41.085814814814796</v>
+      </c>
+      <c r="F7">
+        <v>64.151942911111107</v>
+      </c>
+      <c r="G7">
+        <v>39.560333333333304</v>
+      </c>
+      <c r="H7">
+        <v>61.969233688888799</v>
+      </c>
+      <c r="I7">
+        <v>112.55859259259201</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="C8">
+        <v>7.5223333333333295</v>
+      </c>
+      <c r="D8">
+        <v>8.33814733333333</v>
+      </c>
+      <c r="E8">
+        <v>49.734740740740698</v>
+      </c>
+      <c r="F8">
+        <v>79.63747375555549</v>
+      </c>
+      <c r="G8">
+        <v>50.029074074073996</v>
+      </c>
+      <c r="H8">
+        <v>75.42964099999989</v>
+      </c>
+      <c r="I8">
+        <v>161.51374074074002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>350000</v>
+      </c>
+      <c r="C9">
+        <v>8.6793777777777699</v>
+      </c>
+      <c r="D9">
+        <v>9.4671512</v>
+      </c>
+      <c r="E9">
+        <v>57.6654814814814</v>
+      </c>
+      <c r="F9">
+        <v>93.039540288888801</v>
+      </c>
+      <c r="G9">
+        <v>55.935407407407396</v>
+      </c>
+      <c r="H9">
+        <v>89.336647666666607</v>
+      </c>
+      <c r="I9">
+        <v>222.85903703703698</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>400000</v>
+      </c>
+      <c r="C10">
+        <v>10.1946444444444</v>
+      </c>
+      <c r="D10">
+        <v>11.4091658666666</v>
+      </c>
+      <c r="E10">
+        <v>65.998148148148104</v>
+      </c>
+      <c r="F10">
+        <v>105.88569448888801</v>
+      </c>
+      <c r="G10">
+        <v>64.216296296296292</v>
+      </c>
+      <c r="H10">
+        <v>102.61594882222199</v>
+      </c>
+      <c r="I10">
+        <v>295.16307407407402</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>450000</v>
+      </c>
+      <c r="C11">
+        <v>11.026199999999999</v>
+      </c>
+      <c r="D11">
+        <v>12.6547619555555</v>
+      </c>
+      <c r="E11">
+        <v>75.2657777777777</v>
+      </c>
+      <c r="F11">
+        <v>118.76606431111101</v>
+      </c>
+      <c r="G11">
+        <v>73.974333333333291</v>
+      </c>
+      <c r="H11">
+        <v>113.187225777777</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>500000</v>
+      </c>
+      <c r="C12">
+        <v>11.747444444444401</v>
+      </c>
+      <c r="D12">
+        <v>13.466912733333299</v>
+      </c>
+      <c r="E12">
+        <v>84.995814814814807</v>
+      </c>
+      <c r="F12">
+        <v>132.441457066666</v>
+      </c>
+      <c r="G12">
+        <v>83.467185185185102</v>
+      </c>
+      <c r="H12">
+        <v>127.56304697777701</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>550000</v>
+      </c>
+      <c r="C13">
+        <v>13.1179111111111</v>
+      </c>
+      <c r="D13">
+        <v>14.8641465111111</v>
+      </c>
+      <c r="E13">
+        <v>93.621333333333311</v>
+      </c>
+      <c r="F13">
+        <v>147.73822633333299</v>
+      </c>
+      <c r="G13">
+        <v>94.506185185185089</v>
+      </c>
+      <c r="H13">
+        <v>141.13324488888802</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+      <c r="C14">
+        <v>14.361511111111099</v>
+      </c>
+      <c r="D14">
+        <v>16.4280569777777</v>
+      </c>
+      <c r="E14">
+        <v>104.44374074074</v>
+      </c>
+      <c r="F14">
+        <v>164.62669966666598</v>
+      </c>
+      <c r="G14">
+        <v>114.500925925925</v>
+      </c>
+      <c r="H14">
+        <v>157.27613215555499</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>650000</v>
+      </c>
+      <c r="C15">
+        <v>16.199911111111099</v>
+      </c>
+      <c r="D15">
+        <v>18.853301177777702</v>
+      </c>
+      <c r="E15">
+        <v>112.842296296296</v>
+      </c>
+      <c r="F15">
+        <v>183.37699462222201</v>
+      </c>
+      <c r="G15">
+        <v>114.25796296296201</v>
+      </c>
+      <c r="H15">
+        <v>168.71667495555502</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>700000</v>
+      </c>
+      <c r="C16">
+        <v>16.842755555555499</v>
+      </c>
+      <c r="D16">
+        <v>20.155542911111098</v>
+      </c>
+      <c r="E16">
+        <v>124.86066666666599</v>
+      </c>
+      <c r="F16">
+        <v>193.701255444444</v>
+      </c>
+      <c r="G16">
+        <v>121.19311111111101</v>
+      </c>
+      <c r="H16">
+        <v>186.12291833333299</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>750000</v>
+      </c>
+      <c r="C17">
+        <v>18.7433555555555</v>
+      </c>
+      <c r="D17">
+        <v>22.123518733333299</v>
+      </c>
+      <c r="E17">
+        <v>135.71414814814801</v>
+      </c>
+      <c r="F17">
+        <v>210.24780822222201</v>
+      </c>
+      <c r="G17">
+        <v>134.029888888888</v>
+      </c>
+      <c r="H17">
+        <v>195.876841933333</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>800000</v>
+      </c>
+      <c r="C18">
+        <v>20.256177777777701</v>
+      </c>
+      <c r="D18">
+        <v>23.842707555555499</v>
+      </c>
+      <c r="E18">
+        <v>144.590259259259</v>
+      </c>
+      <c r="F18">
+        <v>220.70003924444401</v>
+      </c>
+      <c r="G18">
+        <v>142.65662962962898</v>
+      </c>
+      <c r="H18">
+        <v>207.84886879999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>850000</v>
+      </c>
+      <c r="C19">
+        <v>22.236555555555498</v>
+      </c>
+      <c r="D19">
+        <v>26.082670488888798</v>
+      </c>
+      <c r="E19">
+        <v>157.63151851851799</v>
+      </c>
+      <c r="F19">
+        <v>236.581600777777</v>
+      </c>
+      <c r="G19">
+        <v>154.05785185185101</v>
+      </c>
+      <c r="H19">
+        <v>222.963460711111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>900000</v>
+      </c>
+      <c r="C20">
+        <v>23.790155555555501</v>
+      </c>
+      <c r="D20">
+        <v>28.613946333333299</v>
+      </c>
+      <c r="E20">
+        <v>166.21792592592499</v>
+      </c>
+      <c r="F20">
+        <v>250.61169626666603</v>
+      </c>
+      <c r="G20">
+        <v>162.91085185185099</v>
+      </c>
+      <c r="H20">
+        <v>239.50266511111101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>950000</v>
+      </c>
+      <c r="C21">
+        <v>25.8042444444444</v>
+      </c>
+      <c r="D21">
+        <v>27.680000666666601</v>
+      </c>
+      <c r="E21">
+        <v>179.18044444444399</v>
+      </c>
+      <c r="F21">
+        <v>265.14206868888903</v>
+      </c>
+      <c r="G21">
+        <v>174.446925925925</v>
+      </c>
+      <c r="H21">
+        <v>257.74343220000003</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="C22">
+        <v>28.145955555555503</v>
+      </c>
+      <c r="D22">
+        <v>30.772209466666599</v>
+      </c>
+      <c r="E22">
+        <v>189.68396296296299</v>
+      </c>
+      <c r="F22">
+        <v>275.159770777777</v>
+      </c>
+      <c r="G22">
+        <v>184.38303703703701</v>
+      </c>
+      <c r="H22">
+        <v>267.94210208888802</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF7D883-2303-AA4F-89A1-5EE1247FC595}">
   <dimension ref="B3:C23"/>
   <sheetViews>
@@ -23092,7 +25773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873D95BF-D23C-644A-9B7B-A0E7AE44E7F3}">
   <dimension ref="A1:R150"/>
   <sheetViews>
@@ -28091,15 +30772,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEBD08F-A22D-004C-B028-B9A5649A9EF3}">
-  <dimension ref="B2:E82"/>
+  <dimension ref="B2:F82"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>23</v>
       </c>
@@ -28109,8 +30790,11 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>5000</v>
       </c>
@@ -28126,8 +30810,12 @@
         <f>arraySortModule.csv!B2</f>
         <v>0.112655509263277</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <f>'customSelectionSort.csv'!B2</f>
+        <v>10.3245585672557</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3+5000</f>
         <v>10000</v>
@@ -28144,8 +30832,12 @@
         <f>arraySortModule.csv!B3</f>
         <v>0.22397561743855399</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f>'customSelectionSort.csv'!B3</f>
+        <v>41.293232690542901</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" ref="B5:B42" si="0">B4+5000</f>
         <v>15000</v>
@@ -28162,8 +30854,12 @@
         <f>arraySortModule.csv!B4</f>
         <v>0.33785206452012001</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <f>'customSelectionSort.csv'!B4</f>
+        <v>92.720794811844797</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>20000</v>
@@ -28180,8 +30876,12 @@
         <f>arraySortModule.csv!B5</f>
         <v>0.52848924696445398</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f>'customSelectionSort.csv'!B5</f>
+        <v>164.42270037531799</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>25000</v>
@@ -28198,8 +30898,12 @@
         <f>arraySortModule.csv!B6</f>
         <v>0.66075130552053396</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f>'customSelectionSort.csv'!B6</f>
+        <v>257.29061499610498</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>30000</v>
@@ -28216,8 +30920,12 @@
         <f>arraySortModule.csv!B7</f>
         <v>0.78948049619793803</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f>'customSelectionSort.csv'!B7</f>
+        <v>370.75442412122999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>35000</v>
@@ -28235,7 +30943,7 @@
         <v>0.91676411405205704</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>40000</v>
@@ -28253,7 +30961,7 @@
         <v>1.05848781391978</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>45000</v>
@@ -28271,7 +30979,7 @@
         <v>1.1791832409799099</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>50000</v>
@@ -28289,7 +30997,7 @@
         <v>1.3122853115200901</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>55000</v>
@@ -28307,7 +31015,7 @@
         <v>1.45074712857604</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>60000</v>
@@ -28325,7 +31033,7 @@
         <v>1.60746737197041</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>65000</v>
@@ -28343,7 +31051,7 @@
         <v>1.7320846840739199</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>70000</v>
@@ -28956,6 +31664,81 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E0AB70-AE84-8747-8725-DAD84F871574}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5000</v>
+      </c>
+      <c r="B2">
+        <v>10.3245585672557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>41.293232690542901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4">
+        <v>92.720794811844797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20000</v>
+      </c>
+      <c r="B5">
+        <v>164.42270037531799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>25000</v>
+      </c>
+      <c r="B6">
+        <v>257.29061499610498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>30000</v>
+      </c>
+      <c r="B7">
+        <v>370.75442412122999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2766C5-C333-C44C-8EFB-EDC7147C1EB1}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -29302,7 +32085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEBB81E-0061-5F4B-A5E8-AFD40BDCA62B}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -29647,11 +32430,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3A630D-BCBD-EA48-90F0-EE0016EF0A47}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -29994,7 +32777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FEB25-A74F-5A45-B563-EED0518B676C}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -30341,7 +33124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C32E7-BB37-4B49-90BE-558A0F4C3E2F}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -30686,555 +33469,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EC2C70-D28D-5649-B065-1682BAD693A3}">
-  <dimension ref="B2:N22"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="83" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>50000</v>
-      </c>
-      <c r="C3">
-        <v>1.15404444444444</v>
-      </c>
-      <c r="D3">
-        <v>1.40228997777777</v>
-      </c>
-      <c r="E3">
-        <v>7.9028888888888895</v>
-      </c>
-      <c r="F3">
-        <v>12.3438432666666</v>
-      </c>
-      <c r="G3">
-        <v>7.8472962962962898</v>
-      </c>
-      <c r="H3">
-        <v>12.094564288888801</v>
-      </c>
-      <c r="I3">
-        <v>3.5976296296296297</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <f>B3+50000</f>
-        <v>100000</v>
-      </c>
-      <c r="C4">
-        <v>2.3280444444444401</v>
-      </c>
-      <c r="D4">
-        <v>2.8260463777777702</v>
-      </c>
-      <c r="E4">
-        <v>16.267111111111099</v>
-      </c>
-      <c r="F4">
-        <v>24.954859555555501</v>
-      </c>
-      <c r="G4">
-        <v>16.073037037037</v>
-      </c>
-      <c r="H4">
-        <v>24.201441644444401</v>
-      </c>
-      <c r="I4">
-        <v>16.4758148148148</v>
-      </c>
-      <c r="N4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <f t="shared" ref="B5:B22" si="0">B4+50000</f>
-        <v>150000</v>
-      </c>
-      <c r="C5">
-        <v>3.6934222222222197</v>
-      </c>
-      <c r="D5">
-        <v>4.3713101111111099</v>
-      </c>
-      <c r="E5">
-        <v>24.1606296296296</v>
-      </c>
-      <c r="F5">
-        <v>38.015178755555496</v>
-      </c>
-      <c r="G5">
-        <v>23.861370370370299</v>
-      </c>
-      <c r="H5">
-        <v>36.627184399999997</v>
-      </c>
-      <c r="I5">
-        <v>40.443629629629505</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>200000</v>
-      </c>
-      <c r="C6">
-        <v>4.8577555555555501</v>
-      </c>
-      <c r="D6">
-        <v>5.8404372888888894</v>
-      </c>
-      <c r="E6">
-        <v>32.296259259259202</v>
-      </c>
-      <c r="F6">
-        <v>51.107483377777697</v>
-      </c>
-      <c r="G6">
-        <v>31.255481481481397</v>
-      </c>
-      <c r="H6">
-        <v>49.392725311111001</v>
-      </c>
-      <c r="I6">
-        <v>73.447925925925901</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>250000</v>
-      </c>
-      <c r="C7">
-        <v>6.0637777777777702</v>
-      </c>
-      <c r="D7">
-        <v>6.9460814444444399</v>
-      </c>
-      <c r="E7">
-        <v>41.085814814814796</v>
-      </c>
-      <c r="F7">
-        <v>64.151942911111107</v>
-      </c>
-      <c r="G7">
-        <v>39.560333333333304</v>
-      </c>
-      <c r="H7">
-        <v>61.969233688888799</v>
-      </c>
-      <c r="I7">
-        <v>112.55859259259201</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>300000</v>
-      </c>
-      <c r="C8">
-        <v>7.5223333333333295</v>
-      </c>
-      <c r="D8">
-        <v>8.33814733333333</v>
-      </c>
-      <c r="E8">
-        <v>49.734740740740698</v>
-      </c>
-      <c r="F8">
-        <v>79.63747375555549</v>
-      </c>
-      <c r="G8">
-        <v>50.029074074073996</v>
-      </c>
-      <c r="H8">
-        <v>75.42964099999989</v>
-      </c>
-      <c r="I8">
-        <v>161.51374074074002</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>350000</v>
-      </c>
-      <c r="C9">
-        <v>8.6793777777777699</v>
-      </c>
-      <c r="D9">
-        <v>9.4671512</v>
-      </c>
-      <c r="E9">
-        <v>57.6654814814814</v>
-      </c>
-      <c r="F9">
-        <v>93.039540288888801</v>
-      </c>
-      <c r="G9">
-        <v>55.935407407407396</v>
-      </c>
-      <c r="H9">
-        <v>89.336647666666607</v>
-      </c>
-      <c r="I9">
-        <v>222.85903703703698</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>400000</v>
-      </c>
-      <c r="C10">
-        <v>10.1946444444444</v>
-      </c>
-      <c r="D10">
-        <v>11.4091658666666</v>
-      </c>
-      <c r="E10">
-        <v>65.998148148148104</v>
-      </c>
-      <c r="F10">
-        <v>105.88569448888801</v>
-      </c>
-      <c r="G10">
-        <v>64.216296296296292</v>
-      </c>
-      <c r="H10">
-        <v>102.61594882222199</v>
-      </c>
-      <c r="I10">
-        <v>295.16307407407402</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>450000</v>
-      </c>
-      <c r="C11">
-        <v>11.026199999999999</v>
-      </c>
-      <c r="D11">
-        <v>12.6547619555555</v>
-      </c>
-      <c r="E11">
-        <v>75.2657777777777</v>
-      </c>
-      <c r="F11">
-        <v>118.76606431111101</v>
-      </c>
-      <c r="G11">
-        <v>73.974333333333291</v>
-      </c>
-      <c r="H11">
-        <v>113.187225777777</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>500000</v>
-      </c>
-      <c r="C12">
-        <v>11.747444444444401</v>
-      </c>
-      <c r="D12">
-        <v>13.466912733333299</v>
-      </c>
-      <c r="E12">
-        <v>84.995814814814807</v>
-      </c>
-      <c r="F12">
-        <v>132.441457066666</v>
-      </c>
-      <c r="G12">
-        <v>83.467185185185102</v>
-      </c>
-      <c r="H12">
-        <v>127.56304697777701</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>550000</v>
-      </c>
-      <c r="C13">
-        <v>13.1179111111111</v>
-      </c>
-      <c r="D13">
-        <v>14.8641465111111</v>
-      </c>
-      <c r="E13">
-        <v>93.621333333333311</v>
-      </c>
-      <c r="F13">
-        <v>147.73822633333299</v>
-      </c>
-      <c r="G13">
-        <v>94.506185185185089</v>
-      </c>
-      <c r="H13">
-        <v>141.13324488888802</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>600000</v>
-      </c>
-      <c r="C14">
-        <v>14.361511111111099</v>
-      </c>
-      <c r="D14">
-        <v>16.4280569777777</v>
-      </c>
-      <c r="E14">
-        <v>104.44374074074</v>
-      </c>
-      <c r="F14">
-        <v>164.62669966666598</v>
-      </c>
-      <c r="G14">
-        <v>114.500925925925</v>
-      </c>
-      <c r="H14">
-        <v>157.27613215555499</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>650000</v>
-      </c>
-      <c r="C15">
-        <v>16.199911111111099</v>
-      </c>
-      <c r="D15">
-        <v>18.853301177777702</v>
-      </c>
-      <c r="E15">
-        <v>112.842296296296</v>
-      </c>
-      <c r="F15">
-        <v>183.37699462222201</v>
-      </c>
-      <c r="G15">
-        <v>114.25796296296201</v>
-      </c>
-      <c r="H15">
-        <v>168.71667495555502</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>700000</v>
-      </c>
-      <c r="C16">
-        <v>16.842755555555499</v>
-      </c>
-      <c r="D16">
-        <v>20.155542911111098</v>
-      </c>
-      <c r="E16">
-        <v>124.86066666666599</v>
-      </c>
-      <c r="F16">
-        <v>193.701255444444</v>
-      </c>
-      <c r="G16">
-        <v>121.19311111111101</v>
-      </c>
-      <c r="H16">
-        <v>186.12291833333299</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>750000</v>
-      </c>
-      <c r="C17">
-        <v>18.7433555555555</v>
-      </c>
-      <c r="D17">
-        <v>22.123518733333299</v>
-      </c>
-      <c r="E17">
-        <v>135.71414814814801</v>
-      </c>
-      <c r="F17">
-        <v>210.24780822222201</v>
-      </c>
-      <c r="G17">
-        <v>134.029888888888</v>
-      </c>
-      <c r="H17">
-        <v>195.876841933333</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>800000</v>
-      </c>
-      <c r="C18">
-        <v>20.256177777777701</v>
-      </c>
-      <c r="D18">
-        <v>23.842707555555499</v>
-      </c>
-      <c r="E18">
-        <v>144.590259259259</v>
-      </c>
-      <c r="F18">
-        <v>220.70003924444401</v>
-      </c>
-      <c r="G18">
-        <v>142.65662962962898</v>
-      </c>
-      <c r="H18">
-        <v>207.84886879999999</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>850000</v>
-      </c>
-      <c r="C19">
-        <v>22.236555555555498</v>
-      </c>
-      <c r="D19">
-        <v>26.082670488888798</v>
-      </c>
-      <c r="E19">
-        <v>157.63151851851799</v>
-      </c>
-      <c r="F19">
-        <v>236.581600777777</v>
-      </c>
-      <c r="G19">
-        <v>154.05785185185101</v>
-      </c>
-      <c r="H19">
-        <v>222.963460711111</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>900000</v>
-      </c>
-      <c r="C20">
-        <v>23.790155555555501</v>
-      </c>
-      <c r="D20">
-        <v>28.613946333333299</v>
-      </c>
-      <c r="E20">
-        <v>166.21792592592499</v>
-      </c>
-      <c r="F20">
-        <v>250.61169626666603</v>
-      </c>
-      <c r="G20">
-        <v>162.91085185185099</v>
-      </c>
-      <c r="H20">
-        <v>239.50266511111101</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>950000</v>
-      </c>
-      <c r="C21">
-        <v>25.8042444444444</v>
-      </c>
-      <c r="D21">
-        <v>27.680000666666601</v>
-      </c>
-      <c r="E21">
-        <v>179.18044444444399</v>
-      </c>
-      <c r="F21">
-        <v>265.14206868888903</v>
-      </c>
-      <c r="G21">
-        <v>174.446925925925</v>
-      </c>
-      <c r="H21">
-        <v>257.74343220000003</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-      <c r="C22">
-        <v>28.145955555555503</v>
-      </c>
-      <c r="D22">
-        <v>30.772209466666599</v>
-      </c>
-      <c r="E22">
-        <v>189.68396296296299</v>
-      </c>
-      <c r="F22">
-        <v>275.159770777777</v>
-      </c>
-      <c r="G22">
-        <v>184.38303703703701</v>
-      </c>
-      <c r="H22">
-        <v>267.94210208888802</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: save excel file
</commit_message>
<xml_diff>
--- a/Time_Plots.xlsx
+++ b/Time_Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abacon/Projects/algorithm_complexity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9346E2-7EDD-5A4E-A84F-AEDD830BB72A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979D9990-D3AC-E44E-B8B5-66776D916B2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{71EB3432-FC80-0741-9FEA-3F0E2C059469}"/>
   </bookViews>
@@ -17,22 +17,24 @@
     <sheet name="reverse2JS" sheetId="6" r:id="rId2"/>
     <sheet name="SortJS" sheetId="7" r:id="rId3"/>
     <sheet name="customSelectionSort.csv" sheetId="14" r:id="rId4"/>
-    <sheet name="jsNativeSort.csv" sheetId="11" r:id="rId5"/>
-    <sheet name="arraySortModule.csv" sheetId="13" r:id="rId6"/>
-    <sheet name="customQuickSort.csv" sheetId="12" r:id="rId7"/>
-    <sheet name="jsNativeReverse.csv" sheetId="9" r:id="rId8"/>
-    <sheet name="customReverse1.csv" sheetId="10" r:id="rId9"/>
-    <sheet name="Shuffle" sheetId="1" r:id="rId10"/>
-    <sheet name="Sort" sheetId="2" r:id="rId11"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId12"/>
+    <sheet name="customMergeSort.js" sheetId="15" r:id="rId5"/>
+    <sheet name="jsNativeSort.csv" sheetId="11" r:id="rId6"/>
+    <sheet name="arraySortModule.csv" sheetId="13" r:id="rId7"/>
+    <sheet name="customQuickSort.csv" sheetId="12" r:id="rId8"/>
+    <sheet name="jsNativeReverse.csv" sheetId="9" r:id="rId9"/>
+    <sheet name="customReverse1.csv" sheetId="10" r:id="rId10"/>
+    <sheet name="Shuffle" sheetId="1" r:id="rId11"/>
+    <sheet name="Sort" sheetId="2" r:id="rId12"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="arraySortModule_1" localSheetId="5">arraySortModule.csv!$A$1:$B$41</definedName>
-    <definedName name="customQuickSort_1" localSheetId="6">'customQuickSort.csv'!$A$1:$B$41</definedName>
-    <definedName name="customReverse1" localSheetId="8">'customReverse1.csv'!$A$1:$B$41</definedName>
+    <definedName name="arraySortModule_1" localSheetId="6">arraySortModule.csv!$A$1:$B$41</definedName>
+    <definedName name="customMergeSort" localSheetId="4">'customMergeSort.js'!$A$1:$B$41</definedName>
+    <definedName name="customQuickSort_1" localSheetId="7">'customQuickSort.csv'!$A$1:$B$41</definedName>
+    <definedName name="customReverse1" localSheetId="9">'customReverse1.csv'!$A$1:$B$41</definedName>
     <definedName name="customSelectionSort" localSheetId="3">'customSelectionSort.csv'!$A$1:$B$7</definedName>
-    <definedName name="jsNativeReverse" localSheetId="7">jsNativeReverse.csv!$A$1:$B$41</definedName>
-    <definedName name="jsNativeSort_1" localSheetId="4">jsNativeSort.csv!$A$1:$B$41</definedName>
+    <definedName name="jsNativeReverse" localSheetId="8">jsNativeReverse.csv!$A$1:$B$41</definedName>
+    <definedName name="jsNativeSort_1" localSheetId="5">jsNativeSort.csv!$A$1:$B$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +63,15 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{AEEB8A18-EF97-2842-9A1D-B553F804E5ED}" name="customQuickSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="2" xr16:uid="{99996971-92DB-1A4D-B7B2-BD043CF226AC}" name="customMergeSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customMergeSort.csv" tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" xr16:uid="{AEEB8A18-EF97-2842-9A1D-B553F804E5ED}" name="customQuickSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customQuickSort.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -69,7 +79,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{213ABC1B-D4DE-5947-BFE0-24F20803A464}" name="customReverse1" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="4" xr16:uid="{213ABC1B-D4DE-5947-BFE0-24F20803A464}" name="customReverse1" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customReverse1.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -77,7 +87,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{DA5891EA-0CE4-7D4F-8FB6-44DEEBEBE699}" name="customSelectionSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="5" xr16:uid="{DA5891EA-0CE4-7D4F-8FB6-44DEEBEBE699}" name="customSelectionSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/customSelectionSort.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -85,7 +95,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{9C73BBB2-53E6-3E40-9352-6501CDC56324}" name="jsNativeReverse" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="6" xr16:uid="{9C73BBB2-53E6-3E40-9352-6501CDC56324}" name="jsNativeReverse" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/jsNativeReverse.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -93,7 +103,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{E76F3574-ECC5-1A46-8FC9-3D2B01FA329A}" name="jsNativeSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="7" xr16:uid="{E76F3574-ECC5-1A46-8FC9-3D2B01FA329A}" name="jsNativeSort" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="10000" sourceFile="/Users/abacon/Projects/algorithm_complexity/javascript/csv_files/jsNativeSort.csv" tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -105,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="28">
   <si>
     <t>Ruby_Shuffle</t>
   </si>
@@ -186,6 +196,9 @@
   </si>
   <si>
     <t>selection_sort_mac</t>
+  </si>
+  <si>
+    <t>custom_merge_sort</t>
   </si>
 </sst>
 </file>
@@ -12532,6 +12545,309 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SortJS!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>custom_merge_sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SortJS!$B$3:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SortJS!$F$3:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.69490344077348698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4361888170242301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.27043944597244</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8635772578418202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7252026796340898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5803109444677803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4385872408747602</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0181418098509303</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.9068851172923997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.8328684903681198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.6506594419479299</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.5122598819434607</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.337758317589699</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.241470687091301</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.8513147532939</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.575908616185099</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.7388828098773</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.3126616254448</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.294380869716401</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.096475634723902</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17.044781435280999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>18.160772245377299</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19.089035626500799</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20.1981613785028</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21.152310568839301</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>21.9093673117458</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>23.2180359959602</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23.879339989274701</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24.893236063420701</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25.243973806500399</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26.144210502505299</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.626715440302998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>27.333615753799599</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28.376636248081901</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>29.192978996783399</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>29.856619935482701</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>31.233818110078499</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>32.279850810766199</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33.3288043737411</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>34.000848684459903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-76CC-6E4D-AF97-8C75E6ED8E3C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -13855,7 +14171,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>SortJS!$F$2</c:f>
+              <c:f>SortJS!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -14019,7 +14335,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>SortJS!$F$3:$F$42</c:f>
+              <c:f>SortJS!$G$3:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -20837,13 +21153,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>236771</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>187786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>164679</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>193710</xdr:rowOff>
@@ -20875,13 +21191,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>219836</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>52319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>778933</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>58243</xdr:rowOff>
@@ -20997,27 +21313,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customSelectionSort" refreshOnLoad="1" connectionId="4" xr16:uid="{D622F393-634F-4D4C-82D5-2836861CD48B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customSelectionSort" refreshOnLoad="1" connectionId="5" xr16:uid="{D622F393-634F-4D4C-82D5-2836861CD48B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeSort_1" refreshOnLoad="1" connectionId="6" xr16:uid="{BBCF7482-98FD-AD4A-9712-69ACE12AE351}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customMergeSort" refreshOnLoad="1" connectionId="2" xr16:uid="{C17CC625-D39A-0841-A055-F9E81CC119CA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeSort_1" refreshOnLoad="1" connectionId="7" xr16:uid="{BBCF7482-98FD-AD4A-9712-69ACE12AE351}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="arraySortModule_1" refreshOnLoad="1" connectionId="1" xr16:uid="{6229A45F-E8FB-5D4E-887A-3055FCD7FF12}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customQuickSort_1" refreshOnLoad="1" connectionId="2" xr16:uid="{73741D56-D32B-A845-966F-3B86276DBDD5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeReverse" refreshOnLoad="1" connectionId="5" xr16:uid="{56AAB590-BEC7-2A4A-83EF-8F6D8BE5A81F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customQuickSort_1" refreshOnLoad="1" connectionId="3" xr16:uid="{73741D56-D32B-A845-966F-3B86276DBDD5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customReverse1" refreshOnLoad="1" connectionId="3" xr16:uid="{F973722E-3E43-7B4F-B612-A86E25BA9E65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="jsNativeReverse" refreshOnLoad="1" connectionId="6" xr16:uid="{56AAB590-BEC7-2A4A-83EF-8F6D8BE5A81F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="customReverse1" refreshOnLoad="1" connectionId="4" xr16:uid="{F973722E-3E43-7B4F-B612-A86E25BA9E65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25023,6 +25343,353 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C32E7-BB37-4B49-90BE-558A0F4C3E2F}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5000</v>
+      </c>
+      <c r="B2">
+        <v>5.1777474582195204E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>9.9681802093982697E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4">
+        <v>1.4743987470865199E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20000</v>
+      </c>
+      <c r="B5">
+        <v>1.95064954459667E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>25000</v>
+      </c>
+      <c r="B6">
+        <v>2.4367738515138598E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>30000</v>
+      </c>
+      <c r="B7">
+        <v>2.91337557137012E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>35000</v>
+      </c>
+      <c r="B8">
+        <v>3.3923618495464297E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>40000</v>
+      </c>
+      <c r="B9">
+        <v>3.8609936833381597E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>45000</v>
+      </c>
+      <c r="B10">
+        <v>4.3939996510743998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>50000</v>
+      </c>
+      <c r="B11">
+        <v>4.8216823488473802E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>55000</v>
+      </c>
+      <c r="B12">
+        <v>5.3119439631700502E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>60000</v>
+      </c>
+      <c r="B13">
+        <v>5.7685434818267801E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>65000</v>
+      </c>
+      <c r="B14">
+        <v>6.24238140881061E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>70000</v>
+      </c>
+      <c r="B15">
+        <v>6.8036064505577004E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>75000</v>
+      </c>
+      <c r="B16">
+        <v>7.1969565004110295E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80000</v>
+      </c>
+      <c r="B17">
+        <v>7.6947562396526295E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>85000</v>
+      </c>
+      <c r="B18">
+        <v>8.1471879035234396E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>90000</v>
+      </c>
+      <c r="B19">
+        <v>8.6254868656396796E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>95000</v>
+      </c>
+      <c r="B20">
+        <v>9.1352686285972595E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>100000</v>
+      </c>
+      <c r="B21">
+        <v>9.6435941755771595E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>105000</v>
+      </c>
+      <c r="B22">
+        <v>0.100425634533166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>110000</v>
+      </c>
+      <c r="B23">
+        <v>0.10606912150979</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>115000</v>
+      </c>
+      <c r="B24">
+        <v>0.111143123358488</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>120000</v>
+      </c>
+      <c r="B25">
+        <v>0.11494356393813999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>125000</v>
+      </c>
+      <c r="B26">
+        <v>0.119756389409303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>130000</v>
+      </c>
+      <c r="B27">
+        <v>0.12411617860198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>135000</v>
+      </c>
+      <c r="B28">
+        <v>0.12881200388073899</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>140000</v>
+      </c>
+      <c r="B29">
+        <v>0.13357987627387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>145000</v>
+      </c>
+      <c r="B30">
+        <v>0.14248574897646901</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>150000</v>
+      </c>
+      <c r="B31">
+        <v>0.14327919110655701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>155000</v>
+      </c>
+      <c r="B32">
+        <v>0.147832252085208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>160000</v>
+      </c>
+      <c r="B33">
+        <v>0.15256081521511</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>165000</v>
+      </c>
+      <c r="B34">
+        <v>0.157056614756584</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>170000</v>
+      </c>
+      <c r="B35">
+        <v>0.163948308676481</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>175000</v>
+      </c>
+      <c r="B36">
+        <v>0.16656081005930901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>180000</v>
+      </c>
+      <c r="B37">
+        <v>0.17375981807708701</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>185000</v>
+      </c>
+      <c r="B38">
+        <v>0.17616043984889901</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>190000</v>
+      </c>
+      <c r="B39">
+        <v>0.183250121772289</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>195000</v>
+      </c>
+      <c r="B40">
+        <v>0.18713506311178199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>200000</v>
+      </c>
+      <c r="B41">
+        <v>0.19145537540316501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EC2C70-D28D-5649-B065-1682BAD693A3}">
   <dimension ref="B2:N22"/>
   <sheetViews>
@@ -25573,7 +26240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF7D883-2303-AA4F-89A1-5EE1247FC595}">
   <dimension ref="B3:C23"/>
   <sheetViews>
@@ -25773,7 +26440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873D95BF-D23C-644A-9B7B-A0E7AE44E7F3}">
   <dimension ref="A1:R150"/>
   <sheetViews>
@@ -30032,7 +30699,7 @@
   <dimension ref="B2:E82"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30772,15 +31439,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEBD08F-A22D-004C-B028-B9A5649A9EF3}">
-  <dimension ref="B2:F82"/>
+  <dimension ref="B2:G82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>23</v>
       </c>
@@ -30791,10 +31458,13 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>5000</v>
       </c>
@@ -30810,12 +31480,16 @@
         <f>arraySortModule.csv!B2</f>
         <v>0.112655509263277</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
+        <f>'customMergeSort.js'!B2</f>
+        <v>0.69490344077348698</v>
+      </c>
+      <c r="G3">
         <f>'customSelectionSort.csv'!B2</f>
         <v>10.3245585672557</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>B3+5000</f>
         <v>10000</v>
@@ -30832,12 +31506,16 @@
         <f>arraySortModule.csv!B3</f>
         <v>0.22397561743855399</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
+        <f>'customMergeSort.js'!B3</f>
+        <v>1.4361888170242301</v>
+      </c>
+      <c r="G4">
         <f>'customSelectionSort.csv'!B3</f>
         <v>41.293232690542901</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5">
         <f t="shared" ref="B5:B42" si="0">B4+5000</f>
         <v>15000</v>
@@ -30854,12 +31532,16 @@
         <f>arraySortModule.csv!B4</f>
         <v>0.33785206452012001</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
+        <f>'customMergeSort.js'!B4</f>
+        <v>2.27043944597244</v>
+      </c>
+      <c r="G5">
         <f>'customSelectionSort.csv'!B4</f>
         <v>92.720794811844797</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>20000</v>
@@ -30876,12 +31558,16 @@
         <f>arraySortModule.csv!B5</f>
         <v>0.52848924696445398</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
+        <f>'customMergeSort.js'!B5</f>
+        <v>2.8635772578418202</v>
+      </c>
+      <c r="G6">
         <f>'customSelectionSort.csv'!B5</f>
         <v>164.42270037531799</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>25000</v>
@@ -30898,12 +31584,16 @@
         <f>arraySortModule.csv!B6</f>
         <v>0.66075130552053396</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
+        <f>'customMergeSort.js'!B6</f>
+        <v>3.7252026796340898</v>
+      </c>
+      <c r="G7">
         <f>'customSelectionSort.csv'!B6</f>
         <v>257.29061499610498</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>30000</v>
@@ -30920,12 +31610,16 @@
         <f>arraySortModule.csv!B7</f>
         <v>0.78948049619793803</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
+        <f>'customMergeSort.js'!B7</f>
+        <v>4.5803109444677803</v>
+      </c>
+      <c r="G8">
         <f>'customSelectionSort.csv'!B7</f>
         <v>370.75442412122999</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>35000</v>
@@ -30942,8 +31636,12 @@
         <f>arraySortModule.csv!B8</f>
         <v>0.91676411405205704</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="2">
+        <f>'customMergeSort.js'!B8</f>
+        <v>5.4385872408747602</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>40000</v>
@@ -30960,8 +31658,12 @@
         <f>arraySortModule.csv!B9</f>
         <v>1.05848781391978</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="2">
+        <f>'customMergeSort.js'!B9</f>
+        <v>6.0181418098509303</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>45000</v>
@@ -30978,8 +31680,12 @@
         <f>arraySortModule.csv!B10</f>
         <v>1.1791832409799099</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="2">
+        <f>'customMergeSort.js'!B10</f>
+        <v>6.9068851172923997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>50000</v>
@@ -30996,8 +31702,12 @@
         <f>arraySortModule.csv!B11</f>
         <v>1.3122853115200901</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="2">
+        <f>'customMergeSort.js'!B11</f>
+        <v>7.8328684903681198</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>55000</v>
@@ -31014,8 +31724,12 @@
         <f>arraySortModule.csv!B12</f>
         <v>1.45074712857604</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="2">
+        <f>'customMergeSort.js'!B12</f>
+        <v>8.6506594419479299</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>60000</v>
@@ -31032,8 +31746,12 @@
         <f>arraySortModule.csv!B13</f>
         <v>1.60746737197041</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="2">
+        <f>'customMergeSort.js'!B13</f>
+        <v>9.5122598819434607</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>65000</v>
@@ -31050,8 +31768,12 @@
         <f>arraySortModule.csv!B14</f>
         <v>1.7320846840739199</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="2">
+        <f>'customMergeSort.js'!B14</f>
+        <v>10.337758317589699</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>70000</v>
@@ -31068,8 +31790,12 @@
         <f>arraySortModule.csv!B15</f>
         <v>1.9626933634281101</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="2">
+        <f>'customMergeSort.js'!B15</f>
+        <v>11.241470687091301</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>75000</v>
@@ -31086,8 +31812,12 @@
         <f>arraySortModule.csv!B16</f>
         <v>1.9835802540183001</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="2">
+        <f>'customMergeSort.js'!B16</f>
+        <v>11.8513147532939</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>80000</v>
@@ -31104,8 +31834,12 @@
         <f>arraySortModule.csv!B17</f>
         <v>2.11196393892169</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="2">
+        <f>'customMergeSort.js'!B17</f>
+        <v>12.575908616185099</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>85000</v>
@@ -31122,8 +31856,12 @@
         <f>arraySortModule.csv!B18</f>
         <v>2.2421319298446099</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="2">
+        <f>'customMergeSort.js'!B18</f>
+        <v>13.7388828098773</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>90000</v>
@@ -31140,8 +31878,12 @@
         <f>arraySortModule.csv!B19</f>
         <v>2.4141624271869602</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="2">
+        <f>'customMergeSort.js'!B19</f>
+        <v>14.3126616254448</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>95000</v>
@@ -31158,8 +31900,12 @@
         <f>arraySortModule.csv!B20</f>
         <v>2.5126983150839801</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="2">
+        <f>'customMergeSort.js'!B20</f>
+        <v>15.294380869716401</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22">
         <f t="shared" si="0"/>
         <v>100000</v>
@@ -31176,8 +31922,12 @@
         <f>arraySortModule.csv!B21</f>
         <v>2.6471459977328702</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="2">
+        <f>'customMergeSort.js'!B21</f>
+        <v>16.096475634723902</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23">
         <f t="shared" si="0"/>
         <v>105000</v>
@@ -31194,8 +31944,12 @@
         <f>arraySortModule.csv!B22</f>
         <v>2.7636468708515101</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="2">
+        <f>'customMergeSort.js'!B22</f>
+        <v>17.044781435280999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24">
         <f t="shared" si="0"/>
         <v>110000</v>
@@ -31212,8 +31966,12 @@
         <f>arraySortModule.csv!B23</f>
         <v>2.90731174871325</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="2">
+        <f>'customMergeSort.js'!B23</f>
+        <v>18.160772245377299</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25">
         <f t="shared" si="0"/>
         <v>115000</v>
@@ -31230,8 +31988,12 @@
         <f>arraySortModule.csv!B24</f>
         <v>3.04968574270606</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="2">
+        <f>'customMergeSort.js'!B24</f>
+        <v>19.089035626500799</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26">
         <f t="shared" si="0"/>
         <v>120000</v>
@@ -31248,8 +32010,12 @@
         <f>arraySortModule.csv!B25</f>
         <v>3.1576443202793598</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="2">
+        <f>'customMergeSort.js'!B25</f>
+        <v>20.1981613785028</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27">
         <f t="shared" si="0"/>
         <v>125000</v>
@@ -31266,8 +32032,12 @@
         <f>arraySortModule.csv!B26</f>
         <v>3.2568029984831801</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="2">
+        <f>'customMergeSort.js'!B26</f>
+        <v>21.152310568839301</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28">
         <f t="shared" si="0"/>
         <v>130000</v>
@@ -31284,8 +32054,12 @@
         <f>arraySortModule.csv!B27</f>
         <v>3.4399440549314</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="2">
+        <f>'customMergeSort.js'!B27</f>
+        <v>21.9093673117458</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29">
         <f t="shared" si="0"/>
         <v>135000</v>
@@ -31302,8 +32076,12 @@
         <f>arraySortModule.csv!B28</f>
         <v>3.5874574966728598</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="2">
+        <f>'customMergeSort.js'!B28</f>
+        <v>23.2180359959602</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30">
         <f t="shared" si="0"/>
         <v>140000</v>
@@ -31320,8 +32098,12 @@
         <f>arraySortModule.csv!B29</f>
         <v>3.69811506569385</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="2">
+        <f>'customMergeSort.js'!B29</f>
+        <v>23.879339989274701</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31">
         <f t="shared" si="0"/>
         <v>145000</v>
@@ -31338,8 +32120,12 @@
         <f>arraySortModule.csv!B30</f>
         <v>3.8563339971005899</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="2">
+        <f>'customMergeSort.js'!B30</f>
+        <v>24.893236063420701</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32">
         <f t="shared" si="0"/>
         <v>150000</v>
@@ -31356,8 +32142,12 @@
         <f>arraySortModule.csv!B31</f>
         <v>3.9518458060920199</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="2">
+        <f>'customMergeSort.js'!B31</f>
+        <v>25.243973806500399</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33">
         <f t="shared" si="0"/>
         <v>155000</v>
@@ -31374,8 +32164,12 @@
         <f>arraySortModule.csv!B32</f>
         <v>4.0669074393808797</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="2">
+        <f>'customMergeSort.js'!B32</f>
+        <v>26.144210502505299</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34">
         <f t="shared" si="0"/>
         <v>160000</v>
@@ -31392,8 +32186,12 @@
         <f>arraySortModule.csv!B33</f>
         <v>4.2685754373669598</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="2">
+        <f>'customMergeSort.js'!B33</f>
+        <v>26.626715440302998</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35">
         <f t="shared" si="0"/>
         <v>165000</v>
@@ -31410,8 +32208,12 @@
         <f>arraySortModule.csv!B34</f>
         <v>4.3928043693304</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="2">
+        <f>'customMergeSort.js'!B34</f>
+        <v>27.333615753799599</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36">
         <f t="shared" si="0"/>
         <v>170000</v>
@@ -31428,8 +32230,12 @@
         <f>arraySortModule.csv!B35</f>
         <v>4.4732246883213502</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="2">
+        <f>'customMergeSort.js'!B35</f>
+        <v>28.376636248081901</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37">
         <f t="shared" si="0"/>
         <v>175000</v>
@@ -31446,8 +32252,12 @@
         <f>arraySortModule.csv!B36</f>
         <v>4.6336993761360601</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="2">
+        <f>'customMergeSort.js'!B36</f>
+        <v>29.192978996783399</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38">
         <f t="shared" si="0"/>
         <v>180000</v>
@@ -31464,8 +32274,12 @@
         <f>arraySortModule.csv!B37</f>
         <v>4.7830456905066896</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="2">
+        <f>'customMergeSort.js'!B37</f>
+        <v>29.856619935482701</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39">
         <f t="shared" si="0"/>
         <v>185000</v>
@@ -31482,8 +32296,12 @@
         <f>arraySortModule.csv!B38</f>
         <v>4.8871905095875201</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="2">
+        <f>'customMergeSort.js'!B38</f>
+        <v>31.233818110078499</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40">
         <f t="shared" si="0"/>
         <v>190000</v>
@@ -31500,8 +32318,12 @@
         <f>arraySortModule.csv!B39</f>
         <v>5.0735971890389902</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="2">
+        <f>'customMergeSort.js'!B39</f>
+        <v>32.279850810766199</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41">
         <f t="shared" si="0"/>
         <v>195000</v>
@@ -31518,8 +32340,12 @@
         <f>arraySortModule.csv!B40</f>
         <v>5.1893460005521703</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="2">
+        <f>'customMergeSort.js'!B40</f>
+        <v>33.3288043737411</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42">
         <f t="shared" si="0"/>
         <v>200000</v>
@@ -31536,23 +32362,27 @@
         <f>arraySortModule.csv!B41</f>
         <v>5.3516968116164199</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="2">
+        <f>'customMergeSort.js'!B41</f>
+        <v>34.000848684459903</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C48" s="2"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.2">
@@ -31739,6 +32569,351 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5607A52B-6A33-2C4D-9438-99C2BEC42A35}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5000</v>
+      </c>
+      <c r="B2">
+        <v>0.69490344077348698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>1.4361888170242301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>15000</v>
+      </c>
+      <c r="B4">
+        <v>2.27043944597244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20000</v>
+      </c>
+      <c r="B5">
+        <v>2.8635772578418202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>25000</v>
+      </c>
+      <c r="B6">
+        <v>3.7252026796340898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>30000</v>
+      </c>
+      <c r="B7">
+        <v>4.5803109444677803</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>35000</v>
+      </c>
+      <c r="B8">
+        <v>5.4385872408747602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>40000</v>
+      </c>
+      <c r="B9">
+        <v>6.0181418098509303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>45000</v>
+      </c>
+      <c r="B10">
+        <v>6.9068851172923997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>50000</v>
+      </c>
+      <c r="B11">
+        <v>7.8328684903681198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>55000</v>
+      </c>
+      <c r="B12">
+        <v>8.6506594419479299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>60000</v>
+      </c>
+      <c r="B13">
+        <v>9.5122598819434607</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>65000</v>
+      </c>
+      <c r="B14">
+        <v>10.337758317589699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>70000</v>
+      </c>
+      <c r="B15">
+        <v>11.241470687091301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>75000</v>
+      </c>
+      <c r="B16">
+        <v>11.8513147532939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>80000</v>
+      </c>
+      <c r="B17">
+        <v>12.575908616185099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>85000</v>
+      </c>
+      <c r="B18">
+        <v>13.7388828098773</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>90000</v>
+      </c>
+      <c r="B19">
+        <v>14.3126616254448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>95000</v>
+      </c>
+      <c r="B20">
+        <v>15.294380869716401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>100000</v>
+      </c>
+      <c r="B21">
+        <v>16.096475634723902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>105000</v>
+      </c>
+      <c r="B22">
+        <v>17.044781435280999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>110000</v>
+      </c>
+      <c r="B23">
+        <v>18.160772245377299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>115000</v>
+      </c>
+      <c r="B24">
+        <v>19.089035626500799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>120000</v>
+      </c>
+      <c r="B25">
+        <v>20.1981613785028</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>125000</v>
+      </c>
+      <c r="B26">
+        <v>21.152310568839301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>130000</v>
+      </c>
+      <c r="B27">
+        <v>21.9093673117458</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>135000</v>
+      </c>
+      <c r="B28">
+        <v>23.2180359959602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>140000</v>
+      </c>
+      <c r="B29">
+        <v>23.879339989274701</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>145000</v>
+      </c>
+      <c r="B30">
+        <v>24.893236063420701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>150000</v>
+      </c>
+      <c r="B31">
+        <v>25.243973806500399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>155000</v>
+      </c>
+      <c r="B32">
+        <v>26.144210502505299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>160000</v>
+      </c>
+      <c r="B33">
+        <v>26.626715440302998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>165000</v>
+      </c>
+      <c r="B34">
+        <v>27.333615753799599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>170000</v>
+      </c>
+      <c r="B35">
+        <v>28.376636248081901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>175000</v>
+      </c>
+      <c r="B36">
+        <v>29.192978996783399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>180000</v>
+      </c>
+      <c r="B37">
+        <v>29.856619935482701</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>185000</v>
+      </c>
+      <c r="B38">
+        <v>31.233818110078499</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>190000</v>
+      </c>
+      <c r="B39">
+        <v>32.279850810766199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>195000</v>
+      </c>
+      <c r="B40">
+        <v>33.3288043737411</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>200000</v>
+      </c>
+      <c r="B41">
+        <v>34.000848684459903</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2766C5-C333-C44C-8EFB-EDC7147C1EB1}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -32085,7 +33260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEBB81E-0061-5F4B-A5E8-AFD40BDCA62B}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -32430,7 +33605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3A630D-BCBD-EA48-90F0-EE0016EF0A47}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -32777,7 +33952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FEB25-A74F-5A45-B563-EED0518B676C}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -33122,351 +34297,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C32E7-BB37-4B49-90BE-558A0F4C3E2F}">
-  <dimension ref="A1:B41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>5000</v>
-      </c>
-      <c r="B2">
-        <v>5.1777474582195204E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10000</v>
-      </c>
-      <c r="B3">
-        <v>9.9681802093982697E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>15000</v>
-      </c>
-      <c r="B4">
-        <v>1.4743987470865199E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>20000</v>
-      </c>
-      <c r="B5">
-        <v>1.95064954459667E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>25000</v>
-      </c>
-      <c r="B6">
-        <v>2.4367738515138598E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>30000</v>
-      </c>
-      <c r="B7">
-        <v>2.91337557137012E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>35000</v>
-      </c>
-      <c r="B8">
-        <v>3.3923618495464297E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>40000</v>
-      </c>
-      <c r="B9">
-        <v>3.8609936833381597E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>45000</v>
-      </c>
-      <c r="B10">
-        <v>4.3939996510743998E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>50000</v>
-      </c>
-      <c r="B11">
-        <v>4.8216823488473802E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>55000</v>
-      </c>
-      <c r="B12">
-        <v>5.3119439631700502E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>60000</v>
-      </c>
-      <c r="B13">
-        <v>5.7685434818267801E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>65000</v>
-      </c>
-      <c r="B14">
-        <v>6.24238140881061E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>70000</v>
-      </c>
-      <c r="B15">
-        <v>6.8036064505577004E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>75000</v>
-      </c>
-      <c r="B16">
-        <v>7.1969565004110295E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>80000</v>
-      </c>
-      <c r="B17">
-        <v>7.6947562396526295E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>85000</v>
-      </c>
-      <c r="B18">
-        <v>8.1471879035234396E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>90000</v>
-      </c>
-      <c r="B19">
-        <v>8.6254868656396796E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>95000</v>
-      </c>
-      <c r="B20">
-        <v>9.1352686285972595E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>100000</v>
-      </c>
-      <c r="B21">
-        <v>9.6435941755771595E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>105000</v>
-      </c>
-      <c r="B22">
-        <v>0.100425634533166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>110000</v>
-      </c>
-      <c r="B23">
-        <v>0.10606912150979</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>115000</v>
-      </c>
-      <c r="B24">
-        <v>0.111143123358488</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>120000</v>
-      </c>
-      <c r="B25">
-        <v>0.11494356393813999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>125000</v>
-      </c>
-      <c r="B26">
-        <v>0.119756389409303</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>130000</v>
-      </c>
-      <c r="B27">
-        <v>0.12411617860198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>135000</v>
-      </c>
-      <c r="B28">
-        <v>0.12881200388073899</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>140000</v>
-      </c>
-      <c r="B29">
-        <v>0.13357987627387</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>145000</v>
-      </c>
-      <c r="B30">
-        <v>0.14248574897646901</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>150000</v>
-      </c>
-      <c r="B31">
-        <v>0.14327919110655701</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>155000</v>
-      </c>
-      <c r="B32">
-        <v>0.147832252085208</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>160000</v>
-      </c>
-      <c r="B33">
-        <v>0.15256081521511</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>165000</v>
-      </c>
-      <c r="B34">
-        <v>0.157056614756584</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>170000</v>
-      </c>
-      <c r="B35">
-        <v>0.163948308676481</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>175000</v>
-      </c>
-      <c r="B36">
-        <v>0.16656081005930901</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>180000</v>
-      </c>
-      <c r="B37">
-        <v>0.17375981807708701</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>185000</v>
-      </c>
-      <c r="B38">
-        <v>0.17616043984889901</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>190000</v>
-      </c>
-      <c r="B39">
-        <v>0.183250121772289</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>195000</v>
-      </c>
-      <c r="B40">
-        <v>0.18713506311178199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>200000</v>
-      </c>
-      <c r="B41">
-        <v>0.19145537540316501</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>